<commit_message>
Fixed records for 1805, 1897, and 1898 containing problematical quote characters.
</commit_message>
<xml_diff>
--- a/xlsx/timeline_links.xlsx
+++ b/xlsx/timeline_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Desktop\ken_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B3B88E-1868-42DE-B8F5-6B6F4749877C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3150CB-69F9-4CB4-9E16-8A9F534D1CD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -246,9 +246,6 @@
     <t>https://historicipswich.org/2019/02/11/over-every-hill-and-missing-every-town/</t>
   </si>
   <si>
-    <t>Newburyport Turnpike opens, February 11, 1805: “Over every hill and missing every town”</t>
-  </si>
-  <si>
     <t>Middlesex Turnpike Reconstruction Project (Phase 3) - MassDOT TIP Project</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
     <t>https://www.boston.gov/news/notes-archives-tremont-street-subway</t>
   </si>
   <si>
-    <t>History of MBTA’s Green Line</t>
-  </si>
-  <si>
     <t>https://www.boston.com/uncategorized/noprimarytagmatch/2012/08/31/recent-changes-history-of-mbtas-green-line</t>
   </si>
   <si>
@@ -538,6 +532,12 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>Newburyport Turnpike opens, February 11, 1805: 'Over every hill and missing every town'</t>
+  </si>
+  <si>
+    <t>History of MBTA's Green Line</t>
   </si>
 </sst>
 </file>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -941,19 +941,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>72</v>
@@ -1134,10 +1134,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E12" t="s">
         <v>71</v>
@@ -1151,10 +1151,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
         <v>71</v>
@@ -1457,10 +1457,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E31" t="s">
         <v>71</v>
@@ -1508,10 +1508,10 @@
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
         <v>71</v>
@@ -1525,10 +1525,10 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
         <v>71</v>
@@ -1576,10 +1576,10 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" t="s">
         <v>71</v>
@@ -1607,13 +1607,13 @@
         <v>1848</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E40" t="s">
         <v>71</v>
@@ -1644,10 +1644,10 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
         <v>71</v>
@@ -1678,10 +1678,10 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="E44" t="s">
         <v>71</v>
@@ -1695,10 +1695,10 @@
         <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E45" t="s">
         <v>71</v>
@@ -1746,10 +1746,10 @@
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E48" t="s">
         <v>71</v>
@@ -1794,13 +1794,13 @@
         <v>1867</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C51" t="s">
-        <v>97</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E51" t="s">
         <v>71</v>
@@ -1814,10 +1814,10 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52" t="s">
         <v>71</v>
@@ -1831,10 +1831,10 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E53" t="s">
         <v>71</v>
@@ -1848,10 +1848,10 @@
         <v>22</v>
       </c>
       <c r="C54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E54" t="s">
         <v>71</v>
@@ -1899,10 +1899,10 @@
         <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E57" t="s">
         <v>71</v>
@@ -1916,10 +1916,10 @@
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E58" t="s">
         <v>71</v>
@@ -1984,10 +1984,10 @@
         <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E62" t="s">
         <v>71</v>
@@ -2001,10 +2001,10 @@
         <v>22</v>
       </c>
       <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E63" t="s">
         <v>71</v>
@@ -2018,10 +2018,10 @@
         <v>22</v>
       </c>
       <c r="C64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E64" t="s">
         <v>71</v>
@@ -2035,10 +2035,10 @@
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E65" t="s">
         <v>71</v>
@@ -2052,10 +2052,10 @@
         <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E66" t="s">
         <v>71</v>
@@ -2069,10 +2069,10 @@
         <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E67" t="s">
         <v>71</v>
@@ -2086,7 +2086,7 @@
         <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>63</v>
@@ -2103,10 +2103,10 @@
         <v>22</v>
       </c>
       <c r="C69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E69" t="s">
         <v>71</v>
@@ -2120,10 +2120,10 @@
         <v>22</v>
       </c>
       <c r="C70" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E70" t="s">
         <v>71</v>
@@ -2137,10 +2137,10 @@
         <v>22</v>
       </c>
       <c r="C71" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E71" t="s">
         <v>71</v>
@@ -2154,10 +2154,10 @@
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E72" t="s">
         <v>71</v>
@@ -2171,7 +2171,7 @@
         <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>63</v>
@@ -2188,10 +2188,10 @@
         <v>22</v>
       </c>
       <c r="C74" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E74" t="s">
         <v>71</v>
@@ -2205,10 +2205,10 @@
         <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E75" t="s">
         <v>71</v>
@@ -2222,10 +2222,10 @@
         <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E76" t="s">
         <v>71</v>
@@ -2236,13 +2236,13 @@
         <v>1901</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E77" t="s">
         <v>71</v>
@@ -2256,10 +2256,10 @@
         <v>22</v>
       </c>
       <c r="C78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E78" t="s">
         <v>71</v>
@@ -2273,10 +2273,10 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E79" t="s">
         <v>71</v>
@@ -2290,10 +2290,10 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E80" t="s">
         <v>71</v>
@@ -2341,10 +2341,10 @@
         <v>22</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E83" t="s">
         <v>71</v>
@@ -2358,10 +2358,10 @@
         <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D84" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E84" t="s">
         <v>71</v>
@@ -2375,10 +2375,10 @@
         <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E85" t="s">
         <v>71</v>
@@ -2392,10 +2392,10 @@
         <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E86" t="s">
         <v>71</v>
@@ -2409,10 +2409,10 @@
         <v>22</v>
       </c>
       <c r="C87" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E87" t="s">
         <v>71</v>
@@ -2426,10 +2426,10 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D88" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E88" t="s">
         <v>71</v>
@@ -2443,10 +2443,10 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E89" t="s">
         <v>71</v>
@@ -2460,10 +2460,10 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E90" t="s">
         <v>71</v>
@@ -2477,10 +2477,10 @@
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E91" t="s">
         <v>71</v>
@@ -2494,10 +2494,10 @@
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E92" t="s">
         <v>71</v>
@@ -2511,10 +2511,10 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E93" t="s">
         <v>71</v>
@@ -2528,10 +2528,10 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E94" t="s">
         <v>71</v>
@@ -2545,10 +2545,10 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E95" t="s">
         <v>71</v>
@@ -2562,10 +2562,10 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E96" t="s">
         <v>71</v>
@@ -2579,10 +2579,10 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D97" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E97" t="s">
         <v>71</v>
@@ -2596,10 +2596,10 @@
         <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E98" t="s">
         <v>71</v>
@@ -2613,10 +2613,10 @@
         <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E99" t="s">
         <v>71</v>
@@ -2630,10 +2630,10 @@
         <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E100" t="s">
         <v>71</v>
@@ -2647,10 +2647,10 @@
         <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E101" t="s">
         <v>71</v>
@@ -2664,10 +2664,10 @@
         <v>22</v>
       </c>
       <c r="C102" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D102" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E102" t="s">
         <v>71</v>
@@ -2681,10 +2681,10 @@
         <v>22</v>
       </c>
       <c r="C103" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D103" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E103" t="s">
         <v>71</v>
@@ -2698,10 +2698,10 @@
         <v>22</v>
       </c>
       <c r="C104" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D104" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E104" t="s">
         <v>71</v>
@@ -2715,10 +2715,10 @@
         <v>22</v>
       </c>
       <c r="C105" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E105" t="s">
         <v>71</v>
@@ -2732,10 +2732,10 @@
         <v>22</v>
       </c>
       <c r="C106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E106" t="s">
         <v>71</v>
@@ -2749,10 +2749,10 @@
         <v>22</v>
       </c>
       <c r="C107" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E107" t="s">
         <v>71</v>
@@ -2766,10 +2766,10 @@
         <v>22</v>
       </c>
       <c r="C108" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E108" t="s">
         <v>71</v>
@@ -2783,10 +2783,10 @@
         <v>22</v>
       </c>
       <c r="C109" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E109" t="s">
         <v>71</v>
@@ -2800,10 +2800,10 @@
         <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D110" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E110" t="s">
         <v>71</v>
@@ -2817,10 +2817,10 @@
         <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E111" t="s">
         <v>71</v>
@@ -2834,10 +2834,10 @@
         <v>22</v>
       </c>
       <c r="C112" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E112" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Latest version from Ken, dated 3/12/2021.
</commit_message>
<xml_diff>
--- a/xlsx/timeline_links.xlsx
+++ b/xlsx/timeline_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF824F98-C9A0-4748-9BB7-78F2C06D9443}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC36433F-7F40-43B4-BD32-2D06E78CA42D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -246,6 +246,9 @@
     <t>https://historicipswich.org/2019/02/11/over-every-hill-and-missing-every-town/</t>
   </si>
   <si>
+    <t>Newburyport Turnpike opens, February 11, 1805: “Over every hill and missing every town”</t>
+  </si>
+  <si>
     <t>Middlesex Turnpike Reconstruction Project (Phase 3) - MassDOT TIP Project</t>
   </si>
   <si>
@@ -693,39 +696,21 @@
     <t>https://www.bostonmpo.org/se_expr_concept</t>
   </si>
   <si>
-    <t>Southeast Expressway Travel Times: Southbound General-Purpose Lanes, PM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3286</t>
   </si>
   <si>
-    <t>Southeast Expressway Travel Times: Northbound Travel Lanes, AM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3285</t>
   </si>
   <si>
-    <t>Southeast Expressway Travel Times: Northbound HOV Lane, AM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3313</t>
   </si>
   <si>
-    <t>Southeast Expressway Travel Times: Northbound General-Purpose Lanes, AM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3312</t>
   </si>
   <si>
-    <t>Southeast Expressway Travel Times: Southbound Travel Lanes, PM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3288</t>
   </si>
   <si>
-    <t>Southeast Expressway Travel Times: Southbound HOV Lane, PM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3287</t>
   </si>
   <si>
@@ -735,21 +720,12 @@
     <t>https://www.bostonmpo.org/node/3267</t>
   </si>
   <si>
-    <t>I-93 North Travel Times: Southbound HOV Lane, AM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3256</t>
   </si>
   <si>
-    <t>I-93 North Travel Times: Southbound Travel Lanes, AM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3232</t>
   </si>
   <si>
-    <t>I-93 North Travel Times: Southbound General-Purpose Lanes, AM Peak Period, 2002–11</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/node/3211</t>
   </si>
   <si>
@@ -1209,7 +1185,31 @@
     <t>The Stony Brook Railroad History</t>
   </si>
   <si>
-    <t>Newburyport Turnpike opens, February 11, 1805: "Over every hill and missing every town"</t>
+    <t>Southeast Expressway Travel Times: Southbound General-Purpose Lanes, PM Peak Period, 2002+C15211</t>
+  </si>
+  <si>
+    <t>Southeast Expressway Travel Times: Northbound Travel Lanes, AM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>Southeast Expressway Travel Times: Northbound HOV Lane, AM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>Southeast Expressway Travel Times: Northbound General-Purpose Lanes, AM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>Southeast Expressway Travel Times: Southbound Travel Lanes, PM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>Southeast Expressway Travel Times: Southbound HOV Lane, PM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>I-93 North Travel Times: Southbound HOV Lane, AM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>I-93 North Travel Times: Southbound Travel Lanes, AM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>I-93 North Travel Times: Southbound General-Purpose Lanes, AM Peak Period, 2002-11</t>
   </si>
 </sst>
 </file>
@@ -1627,33 +1627,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
   <dimension ref="A1:E288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C291" sqref="C291"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="10.875" style="1"/>
-    <col min="3" max="3" width="76.375" customWidth="1"/>
+    <col min="3" max="3" width="89.875" customWidth="1"/>
     <col min="4" max="4" width="74.875" customWidth="1"/>
     <col min="5" max="5" width="14.875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1715,7 +1715,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>394</v>
+        <v>73</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>72</v>
@@ -1834,10 +1834,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>71</v>
@@ -1851,10 +1851,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>71</v>
@@ -1885,7 +1885,7 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>63</v>
@@ -2157,10 +2157,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>71</v>
@@ -2208,10 +2208,10 @@
         <v>22</v>
       </c>
       <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>71</v>
@@ -2225,10 +2225,10 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>71</v>
@@ -2276,10 +2276,10 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>71</v>
@@ -2307,13 +2307,13 @@
         <v>1848</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>71</v>
@@ -2344,10 +2344,10 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>71</v>
@@ -2378,10 +2378,10 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>71</v>
@@ -2395,10 +2395,10 @@
         <v>22</v>
       </c>
       <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>71</v>
@@ -2446,10 +2446,10 @@
         <v>22</v>
       </c>
       <c r="C48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>71</v>
@@ -2494,13 +2494,13 @@
         <v>1867</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>71</v>
@@ -2514,10 +2514,10 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>71</v>
@@ -2531,10 +2531,10 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>71</v>
@@ -2548,10 +2548,10 @@
         <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>71</v>
@@ -2599,10 +2599,10 @@
         <v>22</v>
       </c>
       <c r="C57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="E57" s="11" t="s">
         <v>71</v>
@@ -2616,10 +2616,10 @@
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>71</v>
@@ -2650,7 +2650,7 @@
         <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D60" t="s">
         <v>67</v>
@@ -2684,10 +2684,10 @@
         <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>71</v>
@@ -2701,10 +2701,10 @@
         <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>71</v>
@@ -2718,10 +2718,10 @@
         <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>71</v>
@@ -2735,10 +2735,10 @@
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>71</v>
@@ -2752,10 +2752,10 @@
         <v>22</v>
       </c>
       <c r="C66" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>71</v>
@@ -2769,10 +2769,10 @@
         <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>71</v>
@@ -2786,7 +2786,7 @@
         <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>63</v>
@@ -2803,10 +2803,10 @@
         <v>22</v>
       </c>
       <c r="C69" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>71</v>
@@ -2820,10 +2820,10 @@
         <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>71</v>
@@ -2837,10 +2837,10 @@
         <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>71</v>
@@ -2854,10 +2854,10 @@
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>71</v>
@@ -2871,7 +2871,7 @@
         <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>63</v>
@@ -2888,10 +2888,10 @@
         <v>22</v>
       </c>
       <c r="C74" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>71</v>
@@ -2905,10 +2905,10 @@
         <v>22</v>
       </c>
       <c r="C75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>71</v>
@@ -2922,10 +2922,10 @@
         <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>71</v>
@@ -2939,10 +2939,10 @@
         <v>22</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>71</v>
@@ -2953,13 +2953,13 @@
         <v>1901</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>71</v>
@@ -2973,10 +2973,10 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>71</v>
@@ -2990,10 +2990,10 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>71</v>
@@ -3007,10 +3007,10 @@
         <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>71</v>
@@ -3058,10 +3058,10 @@
         <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>71</v>
@@ -3075,10 +3075,10 @@
         <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D85" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>71</v>
@@ -3092,10 +3092,10 @@
         <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>71</v>
@@ -3109,10 +3109,10 @@
         <v>22</v>
       </c>
       <c r="C87" t="s">
+        <v>122</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>71</v>
@@ -3126,10 +3126,10 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>71</v>
@@ -3143,10 +3143,10 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
+        <v>126</v>
+      </c>
+      <c r="D89" t="s">
         <v>125</v>
-      </c>
-      <c r="D89" t="s">
-        <v>124</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>71</v>
@@ -3160,10 +3160,10 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>71</v>
@@ -3177,10 +3177,10 @@
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>71</v>
@@ -3194,10 +3194,10 @@
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>71</v>
@@ -3211,10 +3211,10 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>71</v>
@@ -3228,10 +3228,10 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E94" s="11" t="s">
         <v>71</v>
@@ -3245,10 +3245,10 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>71</v>
@@ -3262,10 +3262,10 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>71</v>
@@ -3279,10 +3279,10 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>71</v>
@@ -3296,10 +3296,10 @@
         <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D98" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>71</v>
@@ -3313,10 +3313,10 @@
         <v>22</v>
       </c>
       <c r="C99" t="s">
+        <v>139</v>
+      </c>
+      <c r="D99" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>71</v>
@@ -3330,10 +3330,10 @@
         <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>71</v>
@@ -3347,10 +3347,10 @@
         <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>71</v>
@@ -3364,10 +3364,10 @@
         <v>22</v>
       </c>
       <c r="C102" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>71</v>
@@ -3381,10 +3381,10 @@
         <v>22</v>
       </c>
       <c r="C103" t="s">
+        <v>141</v>
+      </c>
+      <c r="D103" t="s">
         <v>140</v>
-      </c>
-      <c r="D103" t="s">
-        <v>139</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>71</v>
@@ -3398,10 +3398,10 @@
         <v>22</v>
       </c>
       <c r="C104" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D104" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>71</v>
@@ -3415,10 +3415,10 @@
         <v>22</v>
       </c>
       <c r="C105" t="s">
+        <v>143</v>
+      </c>
+      <c r="D105" t="s">
         <v>142</v>
-      </c>
-      <c r="D105" t="s">
-        <v>141</v>
       </c>
       <c r="E105" s="11" t="s">
         <v>71</v>
@@ -3432,10 +3432,10 @@
         <v>22</v>
       </c>
       <c r="C106" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E106" s="11" t="s">
         <v>71</v>
@@ -3449,10 +3449,10 @@
         <v>22</v>
       </c>
       <c r="C107" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>71</v>
@@ -3466,10 +3466,10 @@
         <v>22</v>
       </c>
       <c r="C108" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>71</v>
@@ -3483,10 +3483,10 @@
         <v>22</v>
       </c>
       <c r="C109" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E109" s="11" t="s">
         <v>71</v>
@@ -3500,10 +3500,10 @@
         <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>71</v>
@@ -3517,10 +3517,10 @@
         <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D111" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E111" s="11" t="s">
         <v>71</v>
@@ -3534,10 +3534,10 @@
         <v>22</v>
       </c>
       <c r="C112" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E112" s="11" t="s">
         <v>71</v>
@@ -3551,10 +3551,10 @@
         <v>22</v>
       </c>
       <c r="C113" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E113" s="11" t="s">
         <v>71</v>
@@ -3568,10 +3568,10 @@
         <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E114" s="11" t="s">
         <v>70</v>
@@ -3585,10 +3585,10 @@
         <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E115" s="11" t="s">
         <v>70</v>
@@ -3602,10 +3602,10 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E116" s="11" t="s">
         <v>70</v>
@@ -3619,10 +3619,10 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>70</v>
@@ -3636,10 +3636,10 @@
         <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>70</v>
@@ -3653,10 +3653,10 @@
         <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E119" s="11" t="s">
         <v>70</v>
@@ -3670,10 +3670,10 @@
         <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>70</v>
@@ -3687,10 +3687,10 @@
         <v>6</v>
       </c>
       <c r="C121" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>70</v>
@@ -3704,10 +3704,10 @@
         <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E122" s="11" t="s">
         <v>70</v>
@@ -3721,10 +3721,10 @@
         <v>22</v>
       </c>
       <c r="C123" t="s">
+        <v>184</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="E123" s="11" t="s">
         <v>71</v>
@@ -3738,10 +3738,10 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E124" s="11" t="s">
         <v>70</v>
@@ -3755,10 +3755,10 @@
         <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>70</v>
@@ -3772,10 +3772,10 @@
         <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E126" s="11" t="s">
         <v>70</v>
@@ -3789,10 +3789,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E127" s="11" t="s">
         <v>70</v>
@@ -3806,10 +3806,10 @@
         <v>22</v>
       </c>
       <c r="C128" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E128" s="11" t="s">
         <v>71</v>
@@ -3823,10 +3823,10 @@
         <v>22</v>
       </c>
       <c r="C129" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E129" s="11" t="s">
         <v>71</v>
@@ -3840,10 +3840,10 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>70</v>
@@ -3857,10 +3857,10 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E131" s="11" t="s">
         <v>70</v>
@@ -3874,10 +3874,10 @@
         <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E132" s="11" t="s">
         <v>70</v>
@@ -3891,10 +3891,10 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E133" s="11" t="s">
         <v>70</v>
@@ -3908,10 +3908,10 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E134" s="11" t="s">
         <v>70</v>
@@ -3925,10 +3925,10 @@
         <v>22</v>
       </c>
       <c r="C135" t="s">
+        <v>204</v>
+      </c>
+      <c r="D135" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="E135" s="11" t="s">
         <v>71</v>
@@ -3942,10 +3942,10 @@
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>70</v>
@@ -3959,10 +3959,10 @@
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>70</v>
@@ -3976,10 +3976,10 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E138" s="11" t="s">
         <v>70</v>
@@ -3993,10 +3993,10 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E139" s="11" t="s">
         <v>70</v>
@@ -4010,10 +4010,10 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E140" s="11" t="s">
         <v>70</v>
@@ -4027,10 +4027,10 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E141" s="11" t="s">
         <v>70</v>
@@ -4044,10 +4044,10 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E142" s="11" t="s">
         <v>70</v>
@@ -4061,10 +4061,10 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E143" s="11" t="s">
         <v>70</v>
@@ -4078,10 +4078,10 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E144" s="11" t="s">
         <v>70</v>
@@ -4095,10 +4095,10 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E145" s="11" t="s">
         <v>70</v>
@@ -4112,10 +4112,10 @@
         <v>22</v>
       </c>
       <c r="C146" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D146" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="D146" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="E146" s="12" t="s">
         <v>71</v>
@@ -4129,10 +4129,10 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E147" s="11" t="s">
         <v>70</v>
@@ -4146,10 +4146,10 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E148" s="11" t="s">
         <v>70</v>
@@ -4163,10 +4163,10 @@
         <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E149" s="11" t="s">
         <v>70</v>
@@ -4180,10 +4180,10 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E150" s="11" t="s">
         <v>70</v>
@@ -4197,7 +4197,7 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>222</v>
+        <v>386</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>223</v>
@@ -4214,10 +4214,10 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
+        <v>387</v>
+      </c>
+      <c r="D152" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="D152" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="E152" s="11" t="s">
         <v>70</v>
@@ -4231,10 +4231,10 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>226</v>
+        <v>388</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E153" s="11" t="s">
         <v>70</v>
@@ -4248,10 +4248,10 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>228</v>
+        <v>389</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E154" s="11" t="s">
         <v>70</v>
@@ -4265,10 +4265,10 @@
         <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>230</v>
+        <v>390</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E155" s="11" t="s">
         <v>70</v>
@@ -4282,10 +4282,10 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>232</v>
+        <v>391</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E156" s="11" t="s">
         <v>70</v>
@@ -4299,10 +4299,10 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E157" s="11" t="s">
         <v>70</v>
@@ -4316,10 +4316,10 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>236</v>
+        <v>392</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E158" s="11" t="s">
         <v>70</v>
@@ -4333,10 +4333,10 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>238</v>
+        <v>393</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>70</v>
@@ -4350,10 +4350,10 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>240</v>
+        <v>394</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E160" s="11" t="s">
         <v>70</v>
@@ -4367,10 +4367,10 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>70</v>
@@ -4384,10 +4384,10 @@
         <v>22</v>
       </c>
       <c r="C162" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E162" s="11" t="s">
         <v>71</v>
@@ -4435,10 +4435,10 @@
         <v>22</v>
       </c>
       <c r="C165" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E165" s="11" t="s">
         <v>71</v>
@@ -4469,10 +4469,10 @@
         <v>6</v>
       </c>
       <c r="C167" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E167" s="11" t="s">
         <v>70</v>
@@ -4486,10 +4486,10 @@
         <v>6</v>
       </c>
       <c r="C168" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>70</v>
@@ -4503,10 +4503,10 @@
         <v>6</v>
       </c>
       <c r="C169" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E169" s="11" t="s">
         <v>70</v>
@@ -4520,10 +4520,10 @@
         <v>22</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E170" s="11" t="s">
         <v>71</v>
@@ -4537,10 +4537,10 @@
         <v>6</v>
       </c>
       <c r="C171" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E171" s="11" t="s">
         <v>70</v>
@@ -4554,7 +4554,7 @@
         <v>22</v>
       </c>
       <c r="C172" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>63</v>
@@ -4571,10 +4571,10 @@
         <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E173" s="11" t="s">
         <v>70</v>
@@ -4588,10 +4588,10 @@
         <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E174" s="11" t="s">
         <v>70</v>
@@ -4605,10 +4605,10 @@
         <v>6</v>
       </c>
       <c r="C175" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E175" s="11" t="s">
         <v>70</v>
@@ -4622,10 +4622,10 @@
         <v>6</v>
       </c>
       <c r="C176" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E176" s="11" t="s">
         <v>70</v>
@@ -4639,10 +4639,10 @@
         <v>6</v>
       </c>
       <c r="C177" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="E177" s="11" t="s">
         <v>70</v>
@@ -4656,10 +4656,10 @@
         <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E178" s="11" t="s">
         <v>70</v>
@@ -4673,10 +4673,10 @@
         <v>6</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>70</v>
@@ -4690,10 +4690,10 @@
         <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E180" s="11" t="s">
         <v>70</v>
@@ -4707,10 +4707,10 @@
         <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E181" s="11" t="s">
         <v>70</v>
@@ -4724,10 +4724,10 @@
         <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E182" s="11" t="s">
         <v>70</v>
@@ -4741,10 +4741,10 @@
         <v>6</v>
       </c>
       <c r="C183" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E183" s="11" t="s">
         <v>70</v>
@@ -4758,10 +4758,10 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E184" s="11" t="s">
         <v>70</v>
@@ -4775,10 +4775,10 @@
         <v>6</v>
       </c>
       <c r="C185" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E185" s="11" t="s">
         <v>70</v>
@@ -4792,7 +4792,7 @@
         <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>13</v>
@@ -4809,10 +4809,10 @@
         <v>6</v>
       </c>
       <c r="C187" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E187" s="11" t="s">
         <v>70</v>
@@ -4843,10 +4843,10 @@
         <v>22</v>
       </c>
       <c r="C189" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E189" s="11" t="s">
         <v>71</v>
@@ -4860,10 +4860,10 @@
         <v>22</v>
       </c>
       <c r="C190" t="s">
+        <v>85</v>
+      </c>
+      <c r="D190" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D190" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E190" s="11" t="s">
         <v>71</v>
@@ -4877,10 +4877,10 @@
         <v>6</v>
       </c>
       <c r="C191" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>70</v>
@@ -4894,10 +4894,10 @@
         <v>6</v>
       </c>
       <c r="C192" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E192" s="11" t="s">
         <v>70</v>
@@ -4911,10 +4911,10 @@
         <v>6</v>
       </c>
       <c r="C193" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>71</v>
@@ -4928,10 +4928,10 @@
         <v>22</v>
       </c>
       <c r="C194" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D194" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E194" s="11" t="s">
         <v>71</v>
@@ -4945,10 +4945,10 @@
         <v>22</v>
       </c>
       <c r="C195" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="E195" s="11" t="s">
         <v>71</v>
@@ -4962,10 +4962,10 @@
         <v>22</v>
       </c>
       <c r="C196" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E196" s="11" t="s">
         <v>71</v>
@@ -5013,10 +5013,10 @@
         <v>22</v>
       </c>
       <c r="C199" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D199" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E199" s="11" t="s">
         <v>71</v>
@@ -5030,10 +5030,10 @@
         <v>15</v>
       </c>
       <c r="C200" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5044,10 +5044,10 @@
         <v>22</v>
       </c>
       <c r="C201" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E201" s="11" t="s">
         <v>71</v>
@@ -5061,10 +5061,10 @@
         <v>22</v>
       </c>
       <c r="C202" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E202" s="11" t="s">
         <v>71</v>
@@ -5078,10 +5078,10 @@
         <v>22</v>
       </c>
       <c r="C203" t="s">
+        <v>85</v>
+      </c>
+      <c r="D203" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D203" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E203" s="11" t="s">
         <v>71</v>
@@ -5112,10 +5112,10 @@
         <v>22</v>
       </c>
       <c r="C205" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E205" s="11" t="s">
         <v>71</v>
@@ -5129,10 +5129,10 @@
         <v>22</v>
       </c>
       <c r="C206" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E206" s="11" t="s">
         <v>71</v>
@@ -5146,10 +5146,10 @@
         <v>22</v>
       </c>
       <c r="C207" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E207" s="11" t="s">
         <v>71</v>
@@ -5163,10 +5163,10 @@
         <v>22</v>
       </c>
       <c r="C208" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E208" s="11" t="s">
         <v>70</v>
@@ -5180,10 +5180,10 @@
         <v>22</v>
       </c>
       <c r="C209" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D209" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E209" s="11" t="s">
         <v>71</v>
@@ -5197,10 +5197,10 @@
         <v>22</v>
       </c>
       <c r="C210" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E210" s="11" t="s">
         <v>71</v>
@@ -5214,10 +5214,10 @@
         <v>22</v>
       </c>
       <c r="C211" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E211" s="11" t="s">
         <v>71</v>
@@ -5231,10 +5231,10 @@
         <v>22</v>
       </c>
       <c r="C212" t="s">
+        <v>91</v>
+      </c>
+      <c r="D212" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D212" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E212" s="11" t="s">
         <v>71</v>
@@ -5248,10 +5248,10 @@
         <v>22</v>
       </c>
       <c r="C213" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E213" s="11" t="s">
         <v>71</v>
@@ -5265,10 +5265,10 @@
         <v>22</v>
       </c>
       <c r="C214" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E214" s="11" t="s">
         <v>71</v>
@@ -5282,10 +5282,10 @@
         <v>15</v>
       </c>
       <c r="C215" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E215" s="11" t="s">
         <v>70</v>
@@ -5299,10 +5299,10 @@
         <v>22</v>
       </c>
       <c r="C216" t="s">
+        <v>91</v>
+      </c>
+      <c r="D216" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E216" s="11" t="s">
         <v>71</v>
@@ -5316,10 +5316,10 @@
         <v>22</v>
       </c>
       <c r="C217" t="s">
+        <v>89</v>
+      </c>
+      <c r="D217" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D217" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E217" s="11" t="s">
         <v>71</v>
@@ -5333,10 +5333,10 @@
         <v>22</v>
       </c>
       <c r="C218" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E218" s="11" t="s">
         <v>71</v>
@@ -5350,10 +5350,10 @@
         <v>22</v>
       </c>
       <c r="C219" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E219" s="11" t="s">
         <v>71</v>
@@ -5367,10 +5367,10 @@
         <v>15</v>
       </c>
       <c r="C220" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="E220" s="11" t="s">
         <v>71</v>
@@ -5381,13 +5381,13 @@
         <v>1993</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C221" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E221" s="11" t="s">
         <v>71</v>
@@ -5401,10 +5401,10 @@
         <v>22</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E222" s="12" t="s">
         <v>71</v>
@@ -5418,10 +5418,10 @@
         <v>15</v>
       </c>
       <c r="C223" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E223" s="11" t="s">
         <v>70</v>
@@ -5435,10 +5435,10 @@
         <v>5</v>
       </c>
       <c r="C224" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E224" s="11" t="s">
         <v>70</v>
@@ -5449,13 +5449,13 @@
         <v>1993</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C225" t="s">
+        <v>96</v>
+      </c>
+      <c r="D225" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E225" s="11" t="s">
         <v>71</v>
@@ -5469,10 +5469,10 @@
         <v>22</v>
       </c>
       <c r="C226" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="E226" s="11" t="s">
         <v>71</v>
@@ -5486,10 +5486,10 @@
         <v>6</v>
       </c>
       <c r="C227" t="s">
-        <v>236</v>
+        <v>392</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E227" s="11" t="s">
         <v>70</v>
@@ -5503,10 +5503,10 @@
         <v>6</v>
       </c>
       <c r="C228" t="s">
-        <v>238</v>
+        <v>393</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E228" s="11" t="s">
         <v>70</v>
@@ -5520,10 +5520,10 @@
         <v>6</v>
       </c>
       <c r="C229" t="s">
-        <v>240</v>
+        <v>394</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E229" s="11" t="s">
         <v>70</v>
@@ -5537,7 +5537,7 @@
         <v>22</v>
       </c>
       <c r="C230" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>21</v>
@@ -5554,10 +5554,10 @@
         <v>22</v>
       </c>
       <c r="C231" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E231" s="11" t="s">
         <v>71</v>
@@ -5571,10 +5571,10 @@
         <v>22</v>
       </c>
       <c r="C232" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="E232" s="11" t="s">
         <v>71</v>
@@ -5588,10 +5588,10 @@
         <v>22</v>
       </c>
       <c r="C233" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="E233" s="11" t="s">
         <v>71</v>
@@ -5605,10 +5605,10 @@
         <v>6</v>
       </c>
       <c r="C234" t="s">
-        <v>226</v>
+        <v>388</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E234" s="11" t="s">
         <v>70</v>
@@ -5622,10 +5622,10 @@
         <v>6</v>
       </c>
       <c r="C235" t="s">
-        <v>232</v>
+        <v>391</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E235" s="11" t="s">
         <v>70</v>
@@ -5639,10 +5639,10 @@
         <v>6</v>
       </c>
       <c r="C236" t="s">
-        <v>236</v>
+        <v>392</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E236" s="11" t="s">
         <v>70</v>
@@ -5656,10 +5656,10 @@
         <v>22</v>
       </c>
       <c r="C237" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="E237" s="11" t="s">
         <v>71</v>
@@ -5673,10 +5673,10 @@
         <v>22</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E238" s="12" t="s">
         <v>71</v>
@@ -5724,10 +5724,10 @@
         <v>22</v>
       </c>
       <c r="C241" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E241" s="11" t="s">
         <v>71</v>
@@ -5738,13 +5738,13 @@
         <v>1998</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C242" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D242" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E242" s="11" t="s">
         <v>71</v>
@@ -5775,10 +5775,10 @@
         <v>22</v>
       </c>
       <c r="C244" t="s">
+        <v>98</v>
+      </c>
+      <c r="D244" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D244" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E244" s="11" t="s">
         <v>71</v>
@@ -5789,13 +5789,13 @@
         <v>2002</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C245" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E245" s="11" t="s">
         <v>71</v>
@@ -5809,10 +5809,10 @@
         <v>22</v>
       </c>
       <c r="C246" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E246" s="11" t="s">
         <v>71</v>
@@ -5826,10 +5826,10 @@
         <v>22</v>
       </c>
       <c r="C247" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E247" s="11" t="s">
         <v>71</v>
@@ -5843,10 +5843,10 @@
         <v>22</v>
       </c>
       <c r="C248" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E248" s="11" t="s">
         <v>71</v>
@@ -5860,10 +5860,10 @@
         <v>22</v>
       </c>
       <c r="C249" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E249" s="11" t="s">
         <v>71</v>
@@ -5877,10 +5877,10 @@
         <v>22</v>
       </c>
       <c r="C250" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E250" s="11" t="s">
         <v>71</v>
@@ -5894,10 +5894,10 @@
         <v>22</v>
       </c>
       <c r="C251" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E251" s="11" t="s">
         <v>71</v>
@@ -5911,10 +5911,10 @@
         <v>22</v>
       </c>
       <c r="C252" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E252" s="11" t="s">
         <v>71</v>
@@ -5928,10 +5928,10 @@
         <v>6</v>
       </c>
       <c r="C253" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E253" s="11" t="s">
         <v>70</v>
@@ -5945,10 +5945,10 @@
         <v>6</v>
       </c>
       <c r="C254" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E254" s="11" t="s">
         <v>70</v>
@@ -5962,10 +5962,10 @@
         <v>6</v>
       </c>
       <c r="C255" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E255" s="11" t="s">
         <v>70</v>
@@ -5979,10 +5979,10 @@
         <v>22</v>
       </c>
       <c r="C256" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E256" s="11" t="s">
         <v>71</v>
@@ -5996,10 +5996,10 @@
         <v>22</v>
       </c>
       <c r="C257" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E257" s="11" t="s">
         <v>71</v>
@@ -6013,10 +6013,10 @@
         <v>22</v>
       </c>
       <c r="C258" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E258" s="11" t="s">
         <v>71</v>
@@ -6047,7 +6047,7 @@
         <v>22</v>
       </c>
       <c r="C260" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D260" s="3" t="s">
         <v>67</v>
@@ -6064,10 +6064,10 @@
         <v>22</v>
       </c>
       <c r="C261" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E261" s="11" t="s">
         <v>71</v>
@@ -6081,10 +6081,10 @@
         <v>22</v>
       </c>
       <c r="C262" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="E262" s="11" t="s">
         <v>71</v>
@@ -6098,10 +6098,10 @@
         <v>22</v>
       </c>
       <c r="C263" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E263" s="11" t="s">
         <v>71</v>
@@ -6115,10 +6115,10 @@
         <v>15</v>
       </c>
       <c r="C264" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E264" s="11" t="s">
         <v>70</v>
@@ -6132,10 +6132,10 @@
         <v>22</v>
       </c>
       <c r="C265" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E265" s="11" t="s">
         <v>71</v>
@@ -6146,13 +6146,13 @@
         <v>2008</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C266" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E266" s="11" t="s">
         <v>71</v>
@@ -6166,10 +6166,10 @@
         <v>22</v>
       </c>
       <c r="C267" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E267" s="11" t="s">
         <v>71</v>
@@ -6183,10 +6183,10 @@
         <v>22</v>
       </c>
       <c r="C268" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E268" s="11" t="s">
         <v>71</v>
@@ -6200,10 +6200,10 @@
         <v>15</v>
       </c>
       <c r="C269" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E269" s="11" t="s">
         <v>70</v>
@@ -6217,10 +6217,10 @@
         <v>22</v>
       </c>
       <c r="C270" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E270" s="11" t="s">
         <v>71</v>
@@ -6234,10 +6234,10 @@
         <v>15</v>
       </c>
       <c r="C271" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E271" s="11" t="s">
         <v>71</v>
@@ -6265,13 +6265,13 @@
         <v>2011</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C273" t="s">
+        <v>96</v>
+      </c>
+      <c r="D273" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D273" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E273" s="11" t="s">
         <v>71</v>
@@ -6285,10 +6285,10 @@
         <v>22</v>
       </c>
       <c r="C274" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E274" s="11" t="s">
         <v>71</v>
@@ -6302,10 +6302,10 @@
         <v>22</v>
       </c>
       <c r="C275" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="E275" s="11" t="s">
         <v>71</v>
@@ -6319,10 +6319,10 @@
         <v>22</v>
       </c>
       <c r="C276" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E276" s="11" t="s">
         <v>71</v>
@@ -6336,10 +6336,10 @@
         <v>22</v>
       </c>
       <c r="C277" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E277" s="11" t="s">
         <v>71</v>
@@ -6353,10 +6353,10 @@
         <v>22</v>
       </c>
       <c r="C278" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="E278" s="11" t="s">
         <v>71</v>
@@ -6370,10 +6370,10 @@
         <v>22</v>
       </c>
       <c r="C279" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E279" s="11" t="s">
         <v>71</v>
@@ -6387,10 +6387,10 @@
         <v>22</v>
       </c>
       <c r="C280" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="E280" s="11" t="s">
         <v>71</v>
@@ -6404,10 +6404,10 @@
         <v>22</v>
       </c>
       <c r="C281" t="s">
+        <v>184</v>
+      </c>
+      <c r="D281" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="D281" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="E281" s="11" t="s">
         <v>71</v>
@@ -6421,10 +6421,10 @@
         <v>22</v>
       </c>
       <c r="C282" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D282" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="E282" s="11" t="s">
         <v>71</v>
@@ -6438,10 +6438,10 @@
         <v>22</v>
       </c>
       <c r="C283" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="E283" s="11" t="s">
         <v>71</v>
@@ -6455,10 +6455,10 @@
         <v>15</v>
       </c>
       <c r="C284" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E284" s="11" t="s">
         <v>70</v>
@@ -6472,10 +6472,10 @@
         <v>22</v>
       </c>
       <c r="C285" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="E285" s="11" t="s">
         <v>71</v>
@@ -6489,10 +6489,10 @@
         <v>22</v>
       </c>
       <c r="C286" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E286" s="11" t="s">
         <v>71</v>
@@ -6506,10 +6506,10 @@
         <v>22</v>
       </c>
       <c r="C287" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="E287" s="11" t="s">
         <v>71</v>
@@ -6523,10 +6523,10 @@
         <v>22</v>
       </c>
       <c r="C288" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E288" s="11" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Replaced a few non-ASCII characters with HTML entities.
</commit_message>
<xml_diff>
--- a/xlsx/timeline_links.xlsx
+++ b/xlsx/timeline_links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC36433F-7F40-43B4-BD32-2D06E78CA42D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D752FA53-3BA9-406B-B276-376283D01449}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -246,9 +246,6 @@
     <t>https://historicipswich.org/2019/02/11/over-every-hill-and-missing-every-town/</t>
   </si>
   <si>
-    <t>Newburyport Turnpike opens, February 11, 1805: “Over every hill and missing every town”</t>
-  </si>
-  <si>
     <t>Middlesex Turnpike Reconstruction Project (Phase 3) - MassDOT TIP Project</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>https://www.boston.gov/news/notes-archives-tremont-street-subway</t>
   </si>
   <si>
-    <t>History of MBTA’s Green Line</t>
-  </si>
-  <si>
     <t>https://www.boston.com/uncategorized/noprimarytagmatch/2012/08/31/recent-changes-history-of-mbtas-green-line</t>
   </si>
   <si>
@@ -1210,6 +1204,12 @@
   </si>
   <si>
     <t>I-93 North Travel Times: Southbound General-Purpose Lanes, AM Peak Period, 2002-11</t>
+  </si>
+  <si>
+    <t>Newburyport Turnpike opens, February 11, 1805: &amp;ldquo;Over every hill and missing every town&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>History of MBTA&amp;rsquo;s Green Line</t>
   </si>
 </sst>
 </file>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
   <dimension ref="A1:E288"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1641,19 +1641,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1715,7 +1715,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>393</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>72</v>
@@ -1834,10 +1834,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>71</v>
@@ -1851,10 +1851,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>71</v>
@@ -1885,7 +1885,7 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>63</v>
@@ -2157,10 +2157,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>71</v>
@@ -2208,10 +2208,10 @@
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>71</v>
@@ -2225,10 +2225,10 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>71</v>
@@ -2276,10 +2276,10 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>71</v>
@@ -2307,13 +2307,13 @@
         <v>1848</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>383</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C40" t="s">
-        <v>385</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>71</v>
@@ -2344,10 +2344,10 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>71</v>
@@ -2378,10 +2378,10 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>71</v>
@@ -2395,10 +2395,10 @@
         <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>71</v>
@@ -2446,10 +2446,10 @@
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>71</v>
@@ -2494,13 +2494,13 @@
         <v>1867</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>71</v>
@@ -2514,10 +2514,10 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>71</v>
@@ -2531,10 +2531,10 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>71</v>
@@ -2548,10 +2548,10 @@
         <v>22</v>
       </c>
       <c r="C54" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>71</v>
@@ -2599,10 +2599,10 @@
         <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E57" s="11" t="s">
         <v>71</v>
@@ -2616,10 +2616,10 @@
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>71</v>
@@ -2650,7 +2650,7 @@
         <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
         <v>67</v>
@@ -2684,10 +2684,10 @@
         <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>71</v>
@@ -2701,10 +2701,10 @@
         <v>22</v>
       </c>
       <c r="C63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>71</v>
@@ -2718,10 +2718,10 @@
         <v>22</v>
       </c>
       <c r="C64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>71</v>
@@ -2735,10 +2735,10 @@
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>71</v>
@@ -2752,10 +2752,10 @@
         <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>71</v>
@@ -2769,10 +2769,10 @@
         <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>394</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>71</v>
@@ -2786,7 +2786,7 @@
         <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>63</v>
@@ -2803,10 +2803,10 @@
         <v>22</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>71</v>
@@ -2820,10 +2820,10 @@
         <v>22</v>
       </c>
       <c r="C70" t="s">
+        <v>102</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>71</v>
@@ -2837,10 +2837,10 @@
         <v>22</v>
       </c>
       <c r="C71" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>71</v>
@@ -2854,10 +2854,10 @@
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>107</v>
+        <v>394</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>71</v>
@@ -2871,7 +2871,7 @@
         <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>63</v>
@@ -2888,10 +2888,10 @@
         <v>22</v>
       </c>
       <c r="C74" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>71</v>
@@ -2905,10 +2905,10 @@
         <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>71</v>
@@ -2922,10 +2922,10 @@
         <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>71</v>
@@ -2939,10 +2939,10 @@
         <v>22</v>
       </c>
       <c r="C77" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>71</v>
@@ -2953,13 +2953,13 @@
         <v>1901</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C78" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>71</v>
@@ -2973,10 +2973,10 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>71</v>
@@ -2990,10 +2990,10 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>71</v>
@@ -3007,10 +3007,10 @@
         <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>71</v>
@@ -3058,10 +3058,10 @@
         <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>71</v>
@@ -3075,10 +3075,10 @@
         <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D85" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>71</v>
@@ -3092,10 +3092,10 @@
         <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>71</v>
@@ -3109,10 +3109,10 @@
         <v>22</v>
       </c>
       <c r="C87" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>71</v>
@@ -3126,10 +3126,10 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>71</v>
@@ -3143,10 +3143,10 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D89" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>71</v>
@@ -3160,10 +3160,10 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>71</v>
@@ -3177,10 +3177,10 @@
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>71</v>
@@ -3194,10 +3194,10 @@
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>71</v>
@@ -3211,10 +3211,10 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>71</v>
@@ -3228,10 +3228,10 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E94" s="11" t="s">
         <v>71</v>
@@ -3245,10 +3245,10 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>71</v>
@@ -3262,10 +3262,10 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>71</v>
@@ -3279,10 +3279,10 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>71</v>
@@ -3296,10 +3296,10 @@
         <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D98" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>71</v>
@@ -3313,10 +3313,10 @@
         <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>71</v>
@@ -3330,10 +3330,10 @@
         <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>71</v>
@@ -3347,10 +3347,10 @@
         <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>71</v>
@@ -3364,10 +3364,10 @@
         <v>22</v>
       </c>
       <c r="C102" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>71</v>
@@ -3381,10 +3381,10 @@
         <v>22</v>
       </c>
       <c r="C103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D103" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>71</v>
@@ -3398,10 +3398,10 @@
         <v>22</v>
       </c>
       <c r="C104" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D104" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>71</v>
@@ -3415,10 +3415,10 @@
         <v>22</v>
       </c>
       <c r="C105" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D105" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E105" s="11" t="s">
         <v>71</v>
@@ -3432,10 +3432,10 @@
         <v>22</v>
       </c>
       <c r="C106" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E106" s="11" t="s">
         <v>71</v>
@@ -3449,10 +3449,10 @@
         <v>22</v>
       </c>
       <c r="C107" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>71</v>
@@ -3466,10 +3466,10 @@
         <v>22</v>
       </c>
       <c r="C108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>71</v>
@@ -3483,10 +3483,10 @@
         <v>22</v>
       </c>
       <c r="C109" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E109" s="11" t="s">
         <v>71</v>
@@ -3500,10 +3500,10 @@
         <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>71</v>
@@ -3517,10 +3517,10 @@
         <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D111" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E111" s="11" t="s">
         <v>71</v>
@@ -3534,10 +3534,10 @@
         <v>22</v>
       </c>
       <c r="C112" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E112" s="11" t="s">
         <v>71</v>
@@ -3551,10 +3551,10 @@
         <v>22</v>
       </c>
       <c r="C113" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E113" s="11" t="s">
         <v>71</v>
@@ -3568,10 +3568,10 @@
         <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E114" s="11" t="s">
         <v>70</v>
@@ -3585,10 +3585,10 @@
         <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E115" s="11" t="s">
         <v>70</v>
@@ -3602,10 +3602,10 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E116" s="11" t="s">
         <v>70</v>
@@ -3619,10 +3619,10 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>70</v>
@@ -3636,10 +3636,10 @@
         <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>70</v>
@@ -3653,10 +3653,10 @@
         <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E119" s="11" t="s">
         <v>70</v>
@@ -3670,10 +3670,10 @@
         <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>70</v>
@@ -3687,10 +3687,10 @@
         <v>6</v>
       </c>
       <c r="C121" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>70</v>
@@ -3704,10 +3704,10 @@
         <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E122" s="11" t="s">
         <v>70</v>
@@ -3721,10 +3721,10 @@
         <v>22</v>
       </c>
       <c r="C123" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E123" s="11" t="s">
         <v>71</v>
@@ -3738,10 +3738,10 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E124" s="11" t="s">
         <v>70</v>
@@ -3755,10 +3755,10 @@
         <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>70</v>
@@ -3772,10 +3772,10 @@
         <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E126" s="11" t="s">
         <v>70</v>
@@ -3789,10 +3789,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E127" s="11" t="s">
         <v>70</v>
@@ -3806,10 +3806,10 @@
         <v>22</v>
       </c>
       <c r="C128" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E128" s="11" t="s">
         <v>71</v>
@@ -3823,10 +3823,10 @@
         <v>22</v>
       </c>
       <c r="C129" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E129" s="11" t="s">
         <v>71</v>
@@ -3840,10 +3840,10 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>70</v>
@@ -3857,10 +3857,10 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E131" s="11" t="s">
         <v>70</v>
@@ -3874,10 +3874,10 @@
         <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E132" s="11" t="s">
         <v>70</v>
@@ -3891,10 +3891,10 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E133" s="11" t="s">
         <v>70</v>
@@ -3908,10 +3908,10 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E134" s="11" t="s">
         <v>70</v>
@@ -3925,10 +3925,10 @@
         <v>22</v>
       </c>
       <c r="C135" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E135" s="11" t="s">
         <v>71</v>
@@ -3942,10 +3942,10 @@
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>70</v>
@@ -3959,10 +3959,10 @@
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>70</v>
@@ -3976,10 +3976,10 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E138" s="11" t="s">
         <v>70</v>
@@ -3993,10 +3993,10 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E139" s="11" t="s">
         <v>70</v>
@@ -4010,10 +4010,10 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E140" s="11" t="s">
         <v>70</v>
@@ -4027,10 +4027,10 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E141" s="11" t="s">
         <v>70</v>
@@ -4044,10 +4044,10 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E142" s="11" t="s">
         <v>70</v>
@@ -4061,10 +4061,10 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E143" s="11" t="s">
         <v>70</v>
@@ -4078,10 +4078,10 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E144" s="11" t="s">
         <v>70</v>
@@ -4095,10 +4095,10 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E145" s="11" t="s">
         <v>70</v>
@@ -4112,10 +4112,10 @@
         <v>22</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E146" s="12" t="s">
         <v>71</v>
@@ -4129,10 +4129,10 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E147" s="11" t="s">
         <v>70</v>
@@ -4146,10 +4146,10 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E148" s="11" t="s">
         <v>70</v>
@@ -4163,10 +4163,10 @@
         <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E149" s="11" t="s">
         <v>70</v>
@@ -4180,10 +4180,10 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E150" s="11" t="s">
         <v>70</v>
@@ -4197,10 +4197,10 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E151" s="11" t="s">
         <v>70</v>
@@ -4214,10 +4214,10 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E152" s="11" t="s">
         <v>70</v>
@@ -4231,10 +4231,10 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E153" s="11" t="s">
         <v>70</v>
@@ -4248,10 +4248,10 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E154" s="11" t="s">
         <v>70</v>
@@ -4265,10 +4265,10 @@
         <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E155" s="11" t="s">
         <v>70</v>
@@ -4282,10 +4282,10 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E156" s="11" t="s">
         <v>70</v>
@@ -4299,10 +4299,10 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E157" s="11" t="s">
         <v>70</v>
@@ -4316,10 +4316,10 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E158" s="11" t="s">
         <v>70</v>
@@ -4333,10 +4333,10 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>70</v>
@@ -4350,10 +4350,10 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E160" s="11" t="s">
         <v>70</v>
@@ -4367,10 +4367,10 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>70</v>
@@ -4384,10 +4384,10 @@
         <v>22</v>
       </c>
       <c r="C162" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E162" s="11" t="s">
         <v>71</v>
@@ -4435,10 +4435,10 @@
         <v>22</v>
       </c>
       <c r="C165" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E165" s="11" t="s">
         <v>71</v>
@@ -4469,10 +4469,10 @@
         <v>6</v>
       </c>
       <c r="C167" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E167" s="11" t="s">
         <v>70</v>
@@ -4486,10 +4486,10 @@
         <v>6</v>
       </c>
       <c r="C168" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>70</v>
@@ -4503,10 +4503,10 @@
         <v>6</v>
       </c>
       <c r="C169" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E169" s="11" t="s">
         <v>70</v>
@@ -4520,10 +4520,10 @@
         <v>22</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E170" s="11" t="s">
         <v>71</v>
@@ -4537,10 +4537,10 @@
         <v>6</v>
       </c>
       <c r="C171" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E171" s="11" t="s">
         <v>70</v>
@@ -4554,7 +4554,7 @@
         <v>22</v>
       </c>
       <c r="C172" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>63</v>
@@ -4571,10 +4571,10 @@
         <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E173" s="11" t="s">
         <v>70</v>
@@ -4588,10 +4588,10 @@
         <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E174" s="11" t="s">
         <v>70</v>
@@ -4605,10 +4605,10 @@
         <v>6</v>
       </c>
       <c r="C175" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E175" s="11" t="s">
         <v>70</v>
@@ -4622,10 +4622,10 @@
         <v>6</v>
       </c>
       <c r="C176" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E176" s="11" t="s">
         <v>70</v>
@@ -4639,10 +4639,10 @@
         <v>6</v>
       </c>
       <c r="C177" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E177" s="11" t="s">
         <v>70</v>
@@ -4656,10 +4656,10 @@
         <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E178" s="11" t="s">
         <v>70</v>
@@ -4673,10 +4673,10 @@
         <v>6</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>70</v>
@@ -4690,10 +4690,10 @@
         <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E180" s="11" t="s">
         <v>70</v>
@@ -4707,10 +4707,10 @@
         <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E181" s="11" t="s">
         <v>70</v>
@@ -4724,10 +4724,10 @@
         <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E182" s="11" t="s">
         <v>70</v>
@@ -4741,10 +4741,10 @@
         <v>6</v>
       </c>
       <c r="C183" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E183" s="11" t="s">
         <v>70</v>
@@ -4758,10 +4758,10 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E184" s="11" t="s">
         <v>70</v>
@@ -4775,10 +4775,10 @@
         <v>6</v>
       </c>
       <c r="C185" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E185" s="11" t="s">
         <v>70</v>
@@ -4792,7 +4792,7 @@
         <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>13</v>
@@ -4809,10 +4809,10 @@
         <v>6</v>
       </c>
       <c r="C187" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E187" s="11" t="s">
         <v>70</v>
@@ -4843,10 +4843,10 @@
         <v>22</v>
       </c>
       <c r="C189" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E189" s="11" t="s">
         <v>71</v>
@@ -4860,10 +4860,10 @@
         <v>22</v>
       </c>
       <c r="C190" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E190" s="11" t="s">
         <v>71</v>
@@ -4877,10 +4877,10 @@
         <v>6</v>
       </c>
       <c r="C191" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>70</v>
@@ -4894,10 +4894,10 @@
         <v>6</v>
       </c>
       <c r="C192" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E192" s="11" t="s">
         <v>70</v>
@@ -4911,10 +4911,10 @@
         <v>6</v>
       </c>
       <c r="C193" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>71</v>
@@ -4928,10 +4928,10 @@
         <v>22</v>
       </c>
       <c r="C194" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D194" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E194" s="11" t="s">
         <v>71</v>
@@ -4945,10 +4945,10 @@
         <v>22</v>
       </c>
       <c r="C195" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E195" s="11" t="s">
         <v>71</v>
@@ -4962,10 +4962,10 @@
         <v>22</v>
       </c>
       <c r="C196" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E196" s="11" t="s">
         <v>71</v>
@@ -5013,10 +5013,10 @@
         <v>22</v>
       </c>
       <c r="C199" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D199" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E199" s="11" t="s">
         <v>71</v>
@@ -5030,10 +5030,10 @@
         <v>15</v>
       </c>
       <c r="C200" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5044,10 +5044,10 @@
         <v>22</v>
       </c>
       <c r="C201" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E201" s="11" t="s">
         <v>71</v>
@@ -5061,10 +5061,10 @@
         <v>22</v>
       </c>
       <c r="C202" t="s">
+        <v>100</v>
+      </c>
+      <c r="D202" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E202" s="11" t="s">
         <v>71</v>
@@ -5078,10 +5078,10 @@
         <v>22</v>
       </c>
       <c r="C203" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E203" s="11" t="s">
         <v>71</v>
@@ -5112,10 +5112,10 @@
         <v>22</v>
       </c>
       <c r="C205" t="s">
+        <v>79</v>
+      </c>
+      <c r="D205" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D205" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E205" s="11" t="s">
         <v>71</v>
@@ -5129,10 +5129,10 @@
         <v>22</v>
       </c>
       <c r="C206" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E206" s="11" t="s">
         <v>71</v>
@@ -5146,10 +5146,10 @@
         <v>22</v>
       </c>
       <c r="C207" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E207" s="11" t="s">
         <v>71</v>
@@ -5163,10 +5163,10 @@
         <v>22</v>
       </c>
       <c r="C208" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E208" s="11" t="s">
         <v>70</v>
@@ -5180,10 +5180,10 @@
         <v>22</v>
       </c>
       <c r="C209" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D209" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E209" s="11" t="s">
         <v>71</v>
@@ -5197,10 +5197,10 @@
         <v>22</v>
       </c>
       <c r="C210" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E210" s="11" t="s">
         <v>71</v>
@@ -5214,10 +5214,10 @@
         <v>22</v>
       </c>
       <c r="C211" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E211" s="11" t="s">
         <v>71</v>
@@ -5231,10 +5231,10 @@
         <v>22</v>
       </c>
       <c r="C212" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E212" s="11" t="s">
         <v>71</v>
@@ -5248,10 +5248,10 @@
         <v>22</v>
       </c>
       <c r="C213" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E213" s="11" t="s">
         <v>71</v>
@@ -5265,10 +5265,10 @@
         <v>22</v>
       </c>
       <c r="C214" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E214" s="11" t="s">
         <v>71</v>
@@ -5282,10 +5282,10 @@
         <v>15</v>
       </c>
       <c r="C215" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E215" s="11" t="s">
         <v>70</v>
@@ -5299,10 +5299,10 @@
         <v>22</v>
       </c>
       <c r="C216" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E216" s="11" t="s">
         <v>71</v>
@@ -5316,10 +5316,10 @@
         <v>22</v>
       </c>
       <c r="C217" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E217" s="11" t="s">
         <v>71</v>
@@ -5333,10 +5333,10 @@
         <v>22</v>
       </c>
       <c r="C218" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E218" s="11" t="s">
         <v>71</v>
@@ -5350,10 +5350,10 @@
         <v>22</v>
       </c>
       <c r="C219" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E219" s="11" t="s">
         <v>71</v>
@@ -5367,10 +5367,10 @@
         <v>15</v>
       </c>
       <c r="C220" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E220" s="11" t="s">
         <v>71</v>
@@ -5381,13 +5381,13 @@
         <v>1993</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C221" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E221" s="11" t="s">
         <v>71</v>
@@ -5401,10 +5401,10 @@
         <v>22</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E222" s="12" t="s">
         <v>71</v>
@@ -5418,10 +5418,10 @@
         <v>15</v>
       </c>
       <c r="C223" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E223" s="11" t="s">
         <v>70</v>
@@ -5435,10 +5435,10 @@
         <v>5</v>
       </c>
       <c r="C224" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E224" s="11" t="s">
         <v>70</v>
@@ -5449,13 +5449,13 @@
         <v>1993</v>
       </c>
       <c r="B225" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C225" t="s">
+        <v>95</v>
+      </c>
+      <c r="D225" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C225" t="s">
-        <v>96</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="E225" s="11" t="s">
         <v>71</v>
@@ -5469,10 +5469,10 @@
         <v>22</v>
       </c>
       <c r="C226" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E226" s="11" t="s">
         <v>71</v>
@@ -5486,10 +5486,10 @@
         <v>6</v>
       </c>
       <c r="C227" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E227" s="11" t="s">
         <v>70</v>
@@ -5503,10 +5503,10 @@
         <v>6</v>
       </c>
       <c r="C228" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E228" s="11" t="s">
         <v>70</v>
@@ -5520,10 +5520,10 @@
         <v>6</v>
       </c>
       <c r="C229" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E229" s="11" t="s">
         <v>70</v>
@@ -5537,7 +5537,7 @@
         <v>22</v>
       </c>
       <c r="C230" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>21</v>
@@ -5554,10 +5554,10 @@
         <v>22</v>
       </c>
       <c r="C231" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E231" s="11" t="s">
         <v>71</v>
@@ -5571,10 +5571,10 @@
         <v>22</v>
       </c>
       <c r="C232" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E232" s="11" t="s">
         <v>71</v>
@@ -5588,10 +5588,10 @@
         <v>22</v>
       </c>
       <c r="C233" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E233" s="11" t="s">
         <v>71</v>
@@ -5605,10 +5605,10 @@
         <v>6</v>
       </c>
       <c r="C234" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E234" s="11" t="s">
         <v>70</v>
@@ -5622,10 +5622,10 @@
         <v>6</v>
       </c>
       <c r="C235" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E235" s="11" t="s">
         <v>70</v>
@@ -5639,10 +5639,10 @@
         <v>6</v>
       </c>
       <c r="C236" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E236" s="11" t="s">
         <v>70</v>
@@ -5656,10 +5656,10 @@
         <v>22</v>
       </c>
       <c r="C237" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E237" s="11" t="s">
         <v>71</v>
@@ -5673,10 +5673,10 @@
         <v>22</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E238" s="12" t="s">
         <v>71</v>
@@ -5724,10 +5724,10 @@
         <v>22</v>
       </c>
       <c r="C241" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E241" s="11" t="s">
         <v>71</v>
@@ -5738,13 +5738,13 @@
         <v>1998</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C242" t="s">
         <v>315</v>
       </c>
-      <c r="C242" t="s">
-        <v>317</v>
-      </c>
       <c r="D242" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E242" s="11" t="s">
         <v>71</v>
@@ -5775,10 +5775,10 @@
         <v>22</v>
       </c>
       <c r="C244" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E244" s="11" t="s">
         <v>71</v>
@@ -5789,13 +5789,13 @@
         <v>2002</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C245" t="s">
         <v>322</v>
       </c>
-      <c r="C245" t="s">
-        <v>324</v>
-      </c>
       <c r="D245" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E245" s="11" t="s">
         <v>71</v>
@@ -5809,10 +5809,10 @@
         <v>22</v>
       </c>
       <c r="C246" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E246" s="11" t="s">
         <v>71</v>
@@ -5826,10 +5826,10 @@
         <v>22</v>
       </c>
       <c r="C247" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E247" s="11" t="s">
         <v>71</v>
@@ -5843,10 +5843,10 @@
         <v>22</v>
       </c>
       <c r="C248" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E248" s="11" t="s">
         <v>71</v>
@@ -5860,10 +5860,10 @@
         <v>22</v>
       </c>
       <c r="C249" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E249" s="11" t="s">
         <v>71</v>
@@ -5877,10 +5877,10 @@
         <v>22</v>
       </c>
       <c r="C250" t="s">
+        <v>323</v>
+      </c>
+      <c r="D250" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="D250" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="E250" s="11" t="s">
         <v>71</v>
@@ -5894,10 +5894,10 @@
         <v>22</v>
       </c>
       <c r="C251" t="s">
+        <v>324</v>
+      </c>
+      <c r="D251" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="D251" s="3" t="s">
-        <v>328</v>
       </c>
       <c r="E251" s="11" t="s">
         <v>71</v>
@@ -5911,10 +5911,10 @@
         <v>22</v>
       </c>
       <c r="C252" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E252" s="11" t="s">
         <v>71</v>
@@ -5928,10 +5928,10 @@
         <v>6</v>
       </c>
       <c r="C253" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E253" s="11" t="s">
         <v>70</v>
@@ -5945,10 +5945,10 @@
         <v>6</v>
       </c>
       <c r="C254" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E254" s="11" t="s">
         <v>70</v>
@@ -5962,10 +5962,10 @@
         <v>6</v>
       </c>
       <c r="C255" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E255" s="11" t="s">
         <v>70</v>
@@ -5979,10 +5979,10 @@
         <v>22</v>
       </c>
       <c r="C256" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E256" s="11" t="s">
         <v>71</v>
@@ -5996,10 +5996,10 @@
         <v>22</v>
       </c>
       <c r="C257" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E257" s="11" t="s">
         <v>71</v>
@@ -6013,10 +6013,10 @@
         <v>22</v>
       </c>
       <c r="C258" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E258" s="11" t="s">
         <v>71</v>
@@ -6047,7 +6047,7 @@
         <v>22</v>
       </c>
       <c r="C260" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D260" s="3" t="s">
         <v>67</v>
@@ -6064,10 +6064,10 @@
         <v>22</v>
       </c>
       <c r="C261" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E261" s="11" t="s">
         <v>71</v>
@@ -6081,10 +6081,10 @@
         <v>22</v>
       </c>
       <c r="C262" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E262" s="11" t="s">
         <v>71</v>
@@ -6098,10 +6098,10 @@
         <v>22</v>
       </c>
       <c r="C263" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E263" s="11" t="s">
         <v>71</v>
@@ -6115,10 +6115,10 @@
         <v>15</v>
       </c>
       <c r="C264" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E264" s="11" t="s">
         <v>70</v>
@@ -6132,10 +6132,10 @@
         <v>22</v>
       </c>
       <c r="C265" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E265" s="11" t="s">
         <v>71</v>
@@ -6146,13 +6146,13 @@
         <v>2008</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C266" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E266" s="11" t="s">
         <v>71</v>
@@ -6166,10 +6166,10 @@
         <v>22</v>
       </c>
       <c r="C267" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E267" s="11" t="s">
         <v>71</v>
@@ -6183,10 +6183,10 @@
         <v>22</v>
       </c>
       <c r="C268" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E268" s="11" t="s">
         <v>71</v>
@@ -6200,10 +6200,10 @@
         <v>15</v>
       </c>
       <c r="C269" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E269" s="11" t="s">
         <v>70</v>
@@ -6217,10 +6217,10 @@
         <v>22</v>
       </c>
       <c r="C270" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E270" s="11" t="s">
         <v>71</v>
@@ -6234,10 +6234,10 @@
         <v>15</v>
       </c>
       <c r="C271" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E271" s="11" t="s">
         <v>71</v>
@@ -6265,13 +6265,13 @@
         <v>2011</v>
       </c>
       <c r="B273" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C273" t="s">
+        <v>95</v>
+      </c>
+      <c r="D273" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C273" t="s">
-        <v>96</v>
-      </c>
-      <c r="D273" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="E273" s="11" t="s">
         <v>71</v>
@@ -6285,10 +6285,10 @@
         <v>22</v>
       </c>
       <c r="C274" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E274" s="11" t="s">
         <v>71</v>
@@ -6302,10 +6302,10 @@
         <v>22</v>
       </c>
       <c r="C275" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E275" s="11" t="s">
         <v>71</v>
@@ -6319,10 +6319,10 @@
         <v>22</v>
       </c>
       <c r="C276" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E276" s="11" t="s">
         <v>71</v>
@@ -6336,10 +6336,10 @@
         <v>22</v>
       </c>
       <c r="C277" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E277" s="11" t="s">
         <v>71</v>
@@ -6353,10 +6353,10 @@
         <v>22</v>
       </c>
       <c r="C278" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E278" s="11" t="s">
         <v>71</v>
@@ -6370,10 +6370,10 @@
         <v>22</v>
       </c>
       <c r="C279" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E279" s="11" t="s">
         <v>71</v>
@@ -6387,10 +6387,10 @@
         <v>22</v>
       </c>
       <c r="C280" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E280" s="11" t="s">
         <v>71</v>
@@ -6404,10 +6404,10 @@
         <v>22</v>
       </c>
       <c r="C281" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E281" s="11" t="s">
         <v>71</v>
@@ -6421,10 +6421,10 @@
         <v>22</v>
       </c>
       <c r="C282" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D282" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E282" s="11" t="s">
         <v>71</v>
@@ -6438,10 +6438,10 @@
         <v>22</v>
       </c>
       <c r="C283" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E283" s="11" t="s">
         <v>71</v>
@@ -6455,10 +6455,10 @@
         <v>15</v>
       </c>
       <c r="C284" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E284" s="11" t="s">
         <v>70</v>
@@ -6472,10 +6472,10 @@
         <v>22</v>
       </c>
       <c r="C285" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E285" s="11" t="s">
         <v>71</v>
@@ -6489,10 +6489,10 @@
         <v>22</v>
       </c>
       <c r="C286" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E286" s="11" t="s">
         <v>71</v>
@@ -6506,10 +6506,10 @@
         <v>22</v>
       </c>
       <c r="C287" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E287" s="11" t="s">
         <v>71</v>
@@ -6523,10 +6523,10 @@
         <v>22</v>
       </c>
       <c r="C288" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E288" s="11" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Ken's 3/26/2021 version - includes Molasses Flood.
</commit_message>
<xml_diff>
--- a/xlsx/timeline_links.xlsx
+++ b/xlsx/timeline_links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D752FA53-3BA9-406B-B276-376283D01449}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF6423F-C484-4266-B824-C74E67456C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="401">
   <si>
     <t>https://www.bostonmpo.org/data/html/studies/highway/2014_safety_operations/Weymouth_Safety_Operations_2014.html</t>
   </si>
@@ -1210,6 +1210,24 @@
   </si>
   <si>
     <t>History of MBTA&amp;rsquo;s Green Line</t>
+  </si>
+  <si>
+    <t>https://www.theatlantic.com/photo/2015/01/on-this-day-the-boston-molasses-disaster-in-1919/384573/</t>
+  </si>
+  <si>
+    <t>The Boston Molasses Disaster</t>
+  </si>
+  <si>
+    <t>The Great Boston Molasses Flood</t>
+  </si>
+  <si>
+    <t>http://www.billdamon.com/the-great-boston-molasses-flood-of-1919/#sthash.CLyG4oHQ.dpbs</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/cityofbostonarchives/albums/72157647488510784/</t>
+  </si>
+  <si>
+    <t>Atlantic Avenue Elevated Photo Album</t>
   </si>
 </sst>
 </file>
@@ -1625,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
-  <dimension ref="A1:E288"/>
+  <dimension ref="A1:E291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2973,10 +2991,10 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>133</v>
+        <v>400</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>134</v>
+        <v>399</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>71</v>
@@ -2990,10 +3008,10 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>71</v>
@@ -3001,16 +3019,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>71</v>
@@ -3018,16 +3036,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C82" t="s">
-        <v>53</v>
-      </c>
-      <c r="D82" t="s">
-        <v>54</v>
+        <v>117</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>71</v>
@@ -3035,7 +3053,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>22</v>
@@ -3052,16 +3070,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>115</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>116</v>
+        <v>53</v>
+      </c>
+      <c r="D84" t="s">
+        <v>54</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>71</v>
@@ -3075,10 +3093,10 @@
         <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>127</v>
-      </c>
-      <c r="D85" t="s">
-        <v>110</v>
+        <v>115</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>71</v>
@@ -3086,16 +3104,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1">
-        <v>1912</v>
+        <v>1908</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>113</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>114</v>
+        <v>127</v>
+      </c>
+      <c r="D86" t="s">
+        <v>110</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>71</v>
@@ -3109,10 +3127,10 @@
         <v>22</v>
       </c>
       <c r="C87" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>71</v>
@@ -3126,10 +3144,10 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>71</v>
@@ -3143,10 +3161,10 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>124</v>
-      </c>
-      <c r="D89" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>71</v>
@@ -3154,16 +3172,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>113</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>114</v>
+        <v>124</v>
+      </c>
+      <c r="D90" t="s">
+        <v>123</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>71</v>
@@ -3171,16 +3189,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>71</v>
@@ -3188,16 +3206,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>71</v>
@@ -3205,16 +3223,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>71</v>
@@ -3222,7 +3240,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>22</v>
@@ -3239,16 +3257,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="1">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>71</v>
@@ -3262,10 +3280,10 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>71</v>
@@ -3279,10 +3297,10 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>71</v>
@@ -3296,10 +3314,10 @@
         <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>127</v>
-      </c>
-      <c r="D98" t="s">
-        <v>110</v>
+        <v>135</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>71</v>
@@ -3307,16 +3325,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1">
-        <v>1923</v>
+        <v>1919</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>137</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
+      </c>
+      <c r="D99" t="s">
+        <v>110</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>71</v>
@@ -3324,16 +3342,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1">
-        <v>1927</v>
+        <v>1919</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>121</v>
+        <v>396</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>122</v>
+        <v>395</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>71</v>
@@ -3341,16 +3359,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1">
-        <v>1928</v>
+        <v>1919</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>121</v>
+        <v>397</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>122</v>
+        <v>398</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>71</v>
@@ -3358,16 +3376,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="1">
-        <v>1929</v>
+        <v>1923</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C102" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>71</v>
@@ -3375,16 +3393,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C103" t="s">
-        <v>139</v>
-      </c>
-      <c r="D103" t="s">
-        <v>138</v>
+        <v>121</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>71</v>
@@ -3392,16 +3410,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="1">
-        <v>1934</v>
+        <v>1928</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
-      </c>
-      <c r="D104" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>71</v>
@@ -3409,16 +3427,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="1">
-        <v>1936</v>
+        <v>1929</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C105" t="s">
-        <v>141</v>
-      </c>
-      <c r="D105" t="s">
-        <v>140</v>
+        <v>121</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="E105" s="11" t="s">
         <v>71</v>
@@ -3426,16 +3444,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="1">
-        <v>1936</v>
+        <v>1929</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C106" t="s">
-        <v>142</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="D106" t="s">
+        <v>138</v>
       </c>
       <c r="E106" s="11" t="s">
         <v>71</v>
@@ -3443,16 +3461,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="1">
-        <v>1941</v>
+        <v>1934</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C107" t="s">
-        <v>148</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="D107" t="s">
+        <v>145</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>71</v>
@@ -3460,16 +3478,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C108" t="s">
-        <v>150</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
+      </c>
+      <c r="D108" t="s">
+        <v>140</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>71</v>
@@ -3477,16 +3495,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="1">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="E109" s="11" t="s">
         <v>71</v>
@@ -3500,10 +3518,10 @@
         <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>71</v>
@@ -3511,16 +3529,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>146</v>
-      </c>
-      <c r="D111" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="E111" s="11" t="s">
         <v>71</v>
@@ -3528,16 +3546,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1">
-        <v>1950</v>
+        <v>1941</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C112" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="E112" s="11" t="s">
         <v>71</v>
@@ -3545,16 +3563,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="1">
-        <v>1950</v>
+        <v>1941</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C113" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E113" s="11" t="s">
         <v>71</v>
@@ -3562,53 +3580,53 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="1">
-        <v>1951</v>
+        <v>1943</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C114" t="s">
-        <v>163</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>164</v>
+        <v>146</v>
+      </c>
+      <c r="D114" t="s">
+        <v>147</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="1">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C115" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="1">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C116" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3619,10 +3637,10 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>70</v>
@@ -3636,10 +3654,10 @@
         <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>70</v>
@@ -3653,10 +3671,10 @@
         <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E119" s="11" t="s">
         <v>70</v>
@@ -3670,10 +3688,10 @@
         <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>70</v>
@@ -3687,10 +3705,10 @@
         <v>6</v>
       </c>
       <c r="C121" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>70</v>
@@ -3704,10 +3722,10 @@
         <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E122" s="11" t="s">
         <v>70</v>
@@ -3715,33 +3733,33 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="1">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="1">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E124" s="11" t="s">
         <v>70</v>
@@ -3749,16 +3767,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="1">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>70</v>
@@ -3769,16 +3787,16 @@
         <v>1952</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C126" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3789,10 +3807,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E127" s="11" t="s">
         <v>70</v>
@@ -3803,47 +3821,47 @@
         <v>1952</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="1">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C129" t="s">
-        <v>117</v>
+        <v>187</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>118</v>
+        <v>188</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="1">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>70</v>
@@ -3851,50 +3869,50 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="1">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C131" t="s">
-        <v>193</v>
+        <v>117</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="1">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C132" t="s">
-        <v>195</v>
+        <v>117</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="1">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E133" s="11" t="s">
         <v>70</v>
@@ -3902,16 +3920,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="1">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E134" s="11" t="s">
         <v>70</v>
@@ -3919,33 +3937,33 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="1">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="1">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>70</v>
@@ -3953,16 +3971,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="1">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>70</v>
@@ -3970,19 +3988,19 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="1">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C138" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3993,10 +4011,10 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="E139" s="11" t="s">
         <v>70</v>
@@ -4010,10 +4028,10 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="E140" s="11" t="s">
         <v>70</v>
@@ -4021,16 +4039,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="1">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="E141" s="11" t="s">
         <v>70</v>
@@ -4038,16 +4056,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="1">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E142" s="11" t="s">
         <v>70</v>
@@ -4055,16 +4073,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="1">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E143" s="11" t="s">
         <v>70</v>
@@ -4078,10 +4096,10 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E144" s="11" t="s">
         <v>70</v>
@@ -4095,44 +4113,44 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E145" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="7">
+      <c r="A146" s="1">
         <v>1958</v>
       </c>
-      <c r="B146" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D146" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E146" s="12" t="s">
-        <v>71</v>
+      <c r="B146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146" t="s">
+        <v>211</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E146" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="1">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E147" s="11" t="s">
         <v>70</v>
@@ -4140,36 +4158,36 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="1">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="E148" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="1">
-        <v>1959</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C149" t="s">
-        <v>193</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E149" s="11" t="s">
-        <v>70</v>
+      <c r="A149" s="7">
+        <v>1958</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E149" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -4180,10 +4198,10 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E150" s="11" t="s">
         <v>70</v>
@@ -4197,10 +4215,10 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>384</v>
+        <v>191</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="E151" s="11" t="s">
         <v>70</v>
@@ -4214,10 +4232,10 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>385</v>
+        <v>193</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="E152" s="11" t="s">
         <v>70</v>
@@ -4231,10 +4249,10 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>386</v>
+        <v>219</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E153" s="11" t="s">
         <v>70</v>
@@ -4248,10 +4266,10 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E154" s="11" t="s">
         <v>70</v>
@@ -4265,10 +4283,10 @@
         <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E155" s="11" t="s">
         <v>70</v>
@@ -4282,10 +4300,10 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E156" s="11" t="s">
         <v>70</v>
@@ -4299,10 +4317,10 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>227</v>
+        <v>387</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E157" s="11" t="s">
         <v>70</v>
@@ -4316,10 +4334,10 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E158" s="11" t="s">
         <v>70</v>
@@ -4333,10 +4351,10 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>70</v>
@@ -4350,10 +4368,10 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>392</v>
+        <v>227</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E160" s="11" t="s">
         <v>70</v>
@@ -4367,10 +4385,10 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>232</v>
+        <v>390</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>70</v>
@@ -4381,16 +4399,16 @@
         <v>1959</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C162" t="s">
-        <v>113</v>
+        <v>391</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E162" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -4398,16 +4416,16 @@
         <v>1959</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C163" t="s">
-        <v>41</v>
+        <v>392</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
       <c r="E163" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -4415,16 +4433,16 @@
         <v>1959</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C164" t="s">
-        <v>40</v>
+        <v>232</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>42</v>
+        <v>233</v>
       </c>
       <c r="E164" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -4435,10 +4453,10 @@
         <v>22</v>
       </c>
       <c r="C165" t="s">
-        <v>241</v>
+        <v>113</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E165" s="11" t="s">
         <v>71</v>
@@ -4446,16 +4464,16 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="1">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C166" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E166" s="11" t="s">
         <v>71</v>
@@ -4463,53 +4481,53 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="1">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C167" t="s">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>243</v>
+        <v>42</v>
       </c>
       <c r="E167" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="1">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C168" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E168" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="1">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C169" t="s">
-        <v>246</v>
+        <v>48</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>247</v>
+        <v>47</v>
       </c>
       <c r="E169" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -4517,30 +4535,30 @@
         <v>1961</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C170" s="9" t="s">
-        <v>249</v>
+        <v>6</v>
+      </c>
+      <c r="C170" t="s">
+        <v>242</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E170" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="1">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C171" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E171" s="11" t="s">
         <v>70</v>
@@ -4548,50 +4566,50 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="1">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C172" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>63</v>
+        <v>247</v>
       </c>
       <c r="E172" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="1">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" t="s">
-        <v>183</v>
+        <v>22</v>
+      </c>
+      <c r="C173" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
       <c r="E173" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="1">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="E174" s="11" t="s">
         <v>70</v>
@@ -4602,16 +4620,16 @@
         <v>1964</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C175" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>254</v>
+        <v>63</v>
       </c>
       <c r="E175" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4622,10 +4640,10 @@
         <v>6</v>
       </c>
       <c r="C176" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E176" s="11" t="s">
         <v>70</v>
@@ -4639,10 +4657,10 @@
         <v>6</v>
       </c>
       <c r="C177" t="s">
-        <v>255</v>
+        <v>185</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>256</v>
+        <v>186</v>
       </c>
       <c r="E177" s="11" t="s">
         <v>70</v>
@@ -4656,10 +4674,10 @@
         <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E178" s="11" t="s">
         <v>70</v>
@@ -4672,11 +4690,11 @@
       <c r="B179" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C179" s="10" t="s">
-        <v>262</v>
+      <c r="C179" t="s">
+        <v>189</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>259</v>
+        <v>190</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>70</v>
@@ -4684,16 +4702,16 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="1">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E180" s="11" t="s">
         <v>70</v>
@@ -4701,16 +4719,16 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="1">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>183</v>
+        <v>257</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>184</v>
+        <v>258</v>
       </c>
       <c r="E181" s="11" t="s">
         <v>70</v>
@@ -4718,16 +4736,16 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="1">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C182" t="s">
-        <v>185</v>
+      <c r="C182" s="10" t="s">
+        <v>262</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>186</v>
+        <v>259</v>
       </c>
       <c r="E182" s="11" t="s">
         <v>70</v>
@@ -4741,10 +4759,10 @@
         <v>6</v>
       </c>
       <c r="C183" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>196</v>
+        <v>261</v>
       </c>
       <c r="E183" s="11" t="s">
         <v>70</v>
@@ -4758,10 +4776,10 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="E184" s="11" t="s">
         <v>70</v>
@@ -4775,10 +4793,10 @@
         <v>6</v>
       </c>
       <c r="C185" t="s">
-        <v>263</v>
+        <v>185</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>264</v>
+        <v>186</v>
       </c>
       <c r="E185" s="11" t="s">
         <v>70</v>
@@ -4792,10 +4810,10 @@
         <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>265</v>
+        <v>195</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="E186" s="11" t="s">
         <v>70</v>
@@ -4809,112 +4827,112 @@
         <v>6</v>
       </c>
       <c r="C187" t="s">
-        <v>266</v>
+        <v>197</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>267</v>
+        <v>198</v>
       </c>
       <c r="E187" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="188" spans="1:5">
-      <c r="A188" s="7">
-        <v>1966</v>
-      </c>
-      <c r="B188" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>45</v>
+      <c r="A188" s="1">
+        <v>1965</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188" t="s">
+        <v>263</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E188" s="12" t="s">
-        <v>71</v>
+        <v>264</v>
+      </c>
+      <c r="E188" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="1">
-        <v>1971</v>
+        <v>1965</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C189" t="s">
-        <v>121</v>
+        <v>265</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="E189" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="1">
-        <v>1972</v>
+        <v>1965</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C190" t="s">
-        <v>84</v>
+        <v>266</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>83</v>
+        <v>267</v>
       </c>
       <c r="E190" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="1">
-        <v>1973</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C191" t="s">
-        <v>268</v>
+      <c r="A191" s="7">
+        <v>1966</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E191" s="11" t="s">
-        <v>70</v>
+        <v>46</v>
+      </c>
+      <c r="E191" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="1">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C192" t="s">
-        <v>270</v>
+        <v>121</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>271</v>
+        <v>122</v>
       </c>
       <c r="E192" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="1">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C193" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>71</v>
@@ -4922,50 +4940,50 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="1">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C194" t="s">
-        <v>127</v>
-      </c>
-      <c r="D194" t="s">
-        <v>110</v>
+        <v>268</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="E194" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C195" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E195" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="1">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C196" t="s">
-        <v>274</v>
+        <v>148</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>275</v>
+        <v>149</v>
       </c>
       <c r="E196" s="11" t="s">
         <v>71</v>
@@ -4973,16 +4991,16 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="1">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C197" t="s">
-        <v>36</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>37</v>
+        <v>127</v>
+      </c>
+      <c r="D197" t="s">
+        <v>110</v>
       </c>
       <c r="E197" s="11" t="s">
         <v>71</v>
@@ -4990,33 +5008,33 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="1">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C198" t="s">
-        <v>58</v>
+        <v>272</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>57</v>
+        <v>273</v>
       </c>
       <c r="E198" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C199" t="s">
-        <v>127</v>
-      </c>
-      <c r="D199" t="s">
-        <v>110</v>
+        <v>274</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="E199" s="11" t="s">
         <v>71</v>
@@ -5024,47 +5042,50 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C200" t="s">
-        <v>305</v>
+        <v>36</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>306</v>
+        <v>37</v>
+      </c>
+      <c r="E200" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C201" t="s">
-        <v>277</v>
+        <v>58</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>276</v>
+        <v>57</v>
       </c>
       <c r="E201" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="1">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C202" t="s">
-        <v>100</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>101</v>
+        <v>127</v>
+      </c>
+      <c r="D202" t="s">
+        <v>110</v>
       </c>
       <c r="E202" s="11" t="s">
         <v>71</v>
@@ -5072,33 +5093,30 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="1">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C203" t="s">
-        <v>84</v>
+        <v>305</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E203" s="11" t="s">
-        <v>71</v>
+        <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C204" t="s">
-        <v>50</v>
+        <v>277</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>49</v>
+        <v>276</v>
       </c>
       <c r="E204" s="11" t="s">
         <v>71</v>
@@ -5106,16 +5124,16 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="1">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C205" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="E205" s="11" t="s">
         <v>71</v>
@@ -5123,16 +5141,16 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="1">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C206" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="E206" s="11" t="s">
         <v>71</v>
@@ -5140,16 +5158,16 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="1">
-        <v>1985</v>
+        <v>1980</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C207" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="E207" s="11" t="s">
         <v>71</v>
@@ -5157,33 +5175,33 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="1">
-        <v>1985</v>
+        <v>1980</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C208" t="s">
-        <v>266</v>
+        <v>79</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>267</v>
+        <v>80</v>
       </c>
       <c r="E208" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="1">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C209" t="s">
-        <v>127</v>
-      </c>
-      <c r="D209" t="s">
-        <v>110</v>
+        <v>121</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="E209" s="11" t="s">
         <v>71</v>
@@ -5191,16 +5209,16 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="1">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C210" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E210" s="11" t="s">
         <v>71</v>
@@ -5208,19 +5226,19 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="1">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C211" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="E211" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -5231,10 +5249,10 @@
         <v>22</v>
       </c>
       <c r="C212" t="s">
-        <v>90</v>
-      </c>
-      <c r="D212" s="3" t="s">
-        <v>89</v>
+        <v>127</v>
+      </c>
+      <c r="D212" t="s">
+        <v>110</v>
       </c>
       <c r="E212" s="11" t="s">
         <v>71</v>
@@ -5248,10 +5266,10 @@
         <v>22</v>
       </c>
       <c r="C213" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>281</v>
+        <v>116</v>
       </c>
       <c r="E213" s="11" t="s">
         <v>71</v>
@@ -5265,10 +5283,10 @@
         <v>22</v>
       </c>
       <c r="C214" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E214" s="11" t="s">
         <v>71</v>
@@ -5279,16 +5297,16 @@
         <v>1987</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C215" t="s">
-        <v>291</v>
+        <v>90</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>290</v>
+        <v>89</v>
       </c>
       <c r="E215" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -5299,10 +5317,10 @@
         <v>22</v>
       </c>
       <c r="C216" t="s">
-        <v>90</v>
+        <v>280</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>89</v>
+        <v>281</v>
       </c>
       <c r="E216" s="11" t="s">
         <v>71</v>
@@ -5310,16 +5328,16 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C217" t="s">
-        <v>88</v>
+        <v>283</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>87</v>
+        <v>282</v>
       </c>
       <c r="E217" s="11" t="s">
         <v>71</v>
@@ -5327,33 +5345,33 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C218" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E218" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="1">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C219" t="s">
-        <v>286</v>
+        <v>90</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>287</v>
+        <v>89</v>
       </c>
       <c r="E219" s="11" t="s">
         <v>71</v>
@@ -5364,13 +5382,13 @@
         <v>1992</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C220" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>288</v>
+        <v>87</v>
       </c>
       <c r="E220" s="11" t="s">
         <v>71</v>
@@ -5378,53 +5396,53 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="1">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="C221" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E221" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="222" spans="1:5">
-      <c r="A222" s="7">
-        <v>1993</v>
-      </c>
-      <c r="B222" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>334</v>
+      <c r="A222" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C222" t="s">
+        <v>286</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E222" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E222" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="1">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C223" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E223" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -5432,64 +5450,64 @@
         <v>1993</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C224" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E224" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="225" spans="1:5">
-      <c r="A225" s="1">
+      <c r="A225" s="7">
         <v>1993</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C225" t="s">
-        <v>95</v>
+      <c r="B225" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E225" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E225" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C226" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E226" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C227" t="s">
-        <v>390</v>
+        <v>296</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>229</v>
+        <v>297</v>
       </c>
       <c r="E227" s="11" t="s">
         <v>70</v>
@@ -5497,19 +5515,19 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C228" t="s">
-        <v>391</v>
+        <v>95</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>230</v>
+        <v>94</v>
       </c>
       <c r="E228" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -5517,16 +5535,16 @@
         <v>1994</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C229" t="s">
-        <v>392</v>
+        <v>298</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>231</v>
+        <v>299</v>
       </c>
       <c r="E229" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -5534,64 +5552,64 @@
         <v>1994</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C230" t="s">
-        <v>300</v>
+        <v>390</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>21</v>
+        <v>229</v>
       </c>
       <c r="E230" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C231" t="s">
-        <v>302</v>
+        <v>391</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>301</v>
+        <v>230</v>
       </c>
       <c r="E231" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C232" t="s">
-        <v>303</v>
+        <v>392</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>304</v>
+        <v>231</v>
       </c>
       <c r="E232" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C233" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>307</v>
+        <v>21</v>
       </c>
       <c r="E233" s="11" t="s">
         <v>71</v>
@@ -5602,16 +5620,16 @@
         <v>1995</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C234" t="s">
-        <v>386</v>
+        <v>302</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>223</v>
+        <v>301</v>
       </c>
       <c r="E234" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -5619,16 +5637,16 @@
         <v>1995</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C235" t="s">
-        <v>389</v>
+        <v>303</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>226</v>
+        <v>304</v>
       </c>
       <c r="E235" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -5636,16 +5654,16 @@
         <v>1995</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C236" t="s">
-        <v>390</v>
+        <v>308</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>229</v>
+        <v>307</v>
       </c>
       <c r="E236" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -5653,98 +5671,98 @@
         <v>1995</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C237" t="s">
-        <v>310</v>
+        <v>386</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>309</v>
+        <v>223</v>
       </c>
       <c r="E237" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="238" spans="1:5">
-      <c r="A238" s="7">
+      <c r="A238" s="1">
         <v>1995</v>
       </c>
-      <c r="B238" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>334</v>
+      <c r="B238" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C238" t="s">
+        <v>389</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E238" s="12" t="s">
-        <v>71</v>
+        <v>226</v>
+      </c>
+      <c r="E238" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C239" t="s">
-        <v>40</v>
+        <v>390</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="E239" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C240" t="s">
-        <v>41</v>
+        <v>310</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>43</v>
+        <v>309</v>
       </c>
       <c r="E240" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="241" spans="1:5">
-      <c r="A241" s="1">
-        <v>1998</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C241" t="s">
-        <v>311</v>
+      <c r="A241" s="7">
+        <v>1995</v>
+      </c>
+      <c r="B241" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="E241" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E241" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>313</v>
+        <v>22</v>
       </c>
       <c r="C242" t="s">
-        <v>315</v>
-      </c>
-      <c r="D242" t="s">
-        <v>314</v>
+        <v>40</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E242" s="11" t="s">
         <v>71</v>
@@ -5752,16 +5770,16 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C243" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E243" s="11" t="s">
         <v>71</v>
@@ -5769,16 +5787,16 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C244" t="s">
-        <v>97</v>
+        <v>311</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>96</v>
+        <v>312</v>
       </c>
       <c r="E244" s="11" t="s">
         <v>71</v>
@@ -5786,16 +5804,16 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1">
-        <v>2002</v>
+        <v>1998</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C245" t="s">
-        <v>322</v>
-      </c>
-      <c r="D245" s="3" t="s">
-        <v>321</v>
+        <v>315</v>
+      </c>
+      <c r="D245" t="s">
+        <v>314</v>
       </c>
       <c r="E245" s="11" t="s">
         <v>71</v>
@@ -5803,16 +5821,16 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C246" t="s">
-        <v>316</v>
+        <v>36</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>317</v>
+        <v>37</v>
       </c>
       <c r="E246" s="11" t="s">
         <v>71</v>
@@ -5820,16 +5838,16 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C247" t="s">
-        <v>318</v>
+        <v>97</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>319</v>
+        <v>96</v>
       </c>
       <c r="E247" s="11" t="s">
         <v>71</v>
@@ -5840,13 +5858,13 @@
         <v>2002</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>22</v>
+        <v>320</v>
       </c>
       <c r="C248" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E248" s="11" t="s">
         <v>71</v>
@@ -5860,10 +5878,10 @@
         <v>22</v>
       </c>
       <c r="C249" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="E249" s="11" t="s">
         <v>71</v>
@@ -5871,16 +5889,16 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C250" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E250" s="11" t="s">
         <v>71</v>
@@ -5888,16 +5906,16 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C251" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E251" s="11" t="s">
         <v>71</v>
@@ -5905,16 +5923,16 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C252" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E252" s="11" t="s">
         <v>71</v>
@@ -5922,70 +5940,70 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C253" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>218</v>
+        <v>325</v>
       </c>
       <c r="E253" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C254" t="s">
-        <v>191</v>
+        <v>324</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>192</v>
+        <v>326</v>
       </c>
       <c r="E254" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C255" t="s">
-        <v>193</v>
+        <v>332</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>194</v>
+        <v>331</v>
       </c>
       <c r="E255" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C256" t="s">
-        <v>334</v>
+        <v>217</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>333</v>
+        <v>218</v>
       </c>
       <c r="E256" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -5993,47 +6011,47 @@
         <v>2004</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C257" t="s">
-        <v>334</v>
+        <v>191</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>333</v>
+        <v>192</v>
       </c>
       <c r="E257" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C258" t="s">
-        <v>334</v>
+        <v>193</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>333</v>
+        <v>194</v>
       </c>
       <c r="E258" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="1">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C259" t="s">
-        <v>68</v>
+        <v>334</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>69</v>
+        <v>333</v>
       </c>
       <c r="E259" s="11" t="s">
         <v>71</v>
@@ -6041,16 +6059,16 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C260" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>67</v>
+        <v>333</v>
       </c>
       <c r="E260" s="11" t="s">
         <v>71</v>
@@ -6064,10 +6082,10 @@
         <v>22</v>
       </c>
       <c r="C261" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="E261" s="11" t="s">
         <v>71</v>
@@ -6075,16 +6093,16 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C262" t="s">
-        <v>340</v>
+        <v>68</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>341</v>
+        <v>69</v>
       </c>
       <c r="E262" s="11" t="s">
         <v>71</v>
@@ -6092,16 +6110,16 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="1">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C263" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>343</v>
+        <v>67</v>
       </c>
       <c r="E263" s="11" t="s">
         <v>71</v>
@@ -6109,33 +6127,33 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="1">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C264" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="E264" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="265" spans="1:5">
       <c r="A265" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C265" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E265" s="11" t="s">
         <v>71</v>
@@ -6143,16 +6161,16 @@
     </row>
     <row r="266" spans="1:5">
       <c r="A266" s="1">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>313</v>
+        <v>22</v>
       </c>
       <c r="C266" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E266" s="11" t="s">
         <v>71</v>
@@ -6160,33 +6178,33 @@
     </row>
     <row r="267" spans="1:5">
       <c r="A267" s="1">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C267" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E267" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="268" spans="1:5">
       <c r="A268" s="1">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C268" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>126</v>
+        <v>347</v>
       </c>
       <c r="E268" s="11" t="s">
         <v>71</v>
@@ -6194,33 +6212,33 @@
     </row>
     <row r="269" spans="1:5">
       <c r="A269" s="1">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="C269" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E269" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="270" spans="1:5">
       <c r="A270" s="1">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C270" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="E270" s="11" t="s">
         <v>71</v>
@@ -6228,16 +6246,16 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" s="1">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C271" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>357</v>
+        <v>126</v>
       </c>
       <c r="E271" s="11" t="s">
         <v>71</v>
@@ -6245,33 +6263,33 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" s="1">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C272" t="s">
-        <v>45</v>
+        <v>353</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>46</v>
+        <v>354</v>
       </c>
       <c r="E272" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="273" spans="1:5">
       <c r="A273" s="1">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="C273" t="s">
-        <v>95</v>
+        <v>356</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>94</v>
+        <v>355</v>
       </c>
       <c r="E273" s="11" t="s">
         <v>71</v>
@@ -6279,16 +6297,16 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" s="1">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C274" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E274" s="11" t="s">
         <v>71</v>
@@ -6296,16 +6314,16 @@
     </row>
     <row r="275" spans="1:5">
       <c r="A275" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C275" t="s">
-        <v>360</v>
+        <v>45</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>359</v>
+        <v>46</v>
       </c>
       <c r="E275" s="11" t="s">
         <v>71</v>
@@ -6313,16 +6331,16 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="C276" t="s">
-        <v>362</v>
+        <v>95</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>361</v>
+        <v>94</v>
       </c>
       <c r="E276" s="11" t="s">
         <v>71</v>
@@ -6330,16 +6348,16 @@
     </row>
     <row r="277" spans="1:5">
       <c r="A277" s="1">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C277" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E277" s="11" t="s">
         <v>71</v>
@@ -6347,16 +6365,16 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" s="1">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C278" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E278" s="11" t="s">
         <v>71</v>
@@ -6364,16 +6382,16 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" s="1">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C279" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="E279" s="11" t="s">
         <v>71</v>
@@ -6381,16 +6399,16 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C280" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E280" s="11" t="s">
         <v>71</v>
@@ -6398,16 +6416,16 @@
     </row>
     <row r="281" spans="1:5">
       <c r="A281" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C281" t="s">
-        <v>182</v>
+        <v>365</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>181</v>
+        <v>366</v>
       </c>
       <c r="E281" s="11" t="s">
         <v>71</v>
@@ -6415,16 +6433,16 @@
     </row>
     <row r="282" spans="1:5">
       <c r="A282" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C282" t="s">
-        <v>370</v>
-      </c>
-      <c r="D282" t="s">
-        <v>369</v>
+        <v>378</v>
+      </c>
+      <c r="D282" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="E282" s="11" t="s">
         <v>71</v>
@@ -6432,16 +6450,16 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C283" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E283" s="11" t="s">
         <v>71</v>
@@ -6449,33 +6467,33 @@
     </row>
     <row r="284" spans="1:5">
       <c r="A284" s="1">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C284" t="s">
-        <v>353</v>
+        <v>182</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>354</v>
+        <v>181</v>
       </c>
       <c r="E284" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="285" spans="1:5">
       <c r="A285" s="1">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C285" t="s">
-        <v>374</v>
-      </c>
-      <c r="D285" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
+      </c>
+      <c r="D285" t="s">
+        <v>369</v>
       </c>
       <c r="E285" s="11" t="s">
         <v>71</v>
@@ -6483,16 +6501,16 @@
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C286" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E286" s="11" t="s">
         <v>71</v>
@@ -6500,35 +6518,86 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C287" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
       <c r="E287" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="288" spans="1:5">
       <c r="A288" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C288" t="s">
+        <v>374</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E288" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C289" t="s">
+        <v>375</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E289" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C290" t="s">
+        <v>379</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E290" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" s="1">
         <v>2021</v>
       </c>
-      <c r="B288" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C288" t="s">
+      <c r="B291" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C291" t="s">
         <v>382</v>
       </c>
-      <c r="D288" s="3" t="s">
+      <c r="D291" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E288" s="11" t="s">
+      <c r="E291" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6587,204 +6656,207 @@
     <hyperlink ref="D75" r:id="rId51" xr:uid="{7F1EFF99-583A-6B4D-A3EB-824895A98C6F}"/>
     <hyperlink ref="D78" r:id="rId52" xr:uid="{F3A77ECC-804C-1E44-94A7-51411C449BA3}"/>
     <hyperlink ref="D76" r:id="rId53" xr:uid="{A3CF8173-1ABB-874D-AFE8-C0816C3C4A29}"/>
-    <hyperlink ref="D81" r:id="rId54" xr:uid="{42481CE0-DCAC-7347-A21F-7C04B44C6492}"/>
-    <hyperlink ref="D84" r:id="rId55" xr:uid="{8B79ADB7-F134-A54C-8A6F-8029C920BB98}"/>
-    <hyperlink ref="D87" r:id="rId56" xr:uid="{0F29D32C-0E67-F248-8C35-9710D68A7F85}"/>
-    <hyperlink ref="D88" r:id="rId57" xr:uid="{BA71FBDC-01A3-4A48-BCA0-1C6E4893F910}"/>
+    <hyperlink ref="D82" r:id="rId54" xr:uid="{42481CE0-DCAC-7347-A21F-7C04B44C6492}"/>
+    <hyperlink ref="D85" r:id="rId55" xr:uid="{8B79ADB7-F134-A54C-8A6F-8029C920BB98}"/>
+    <hyperlink ref="D88" r:id="rId56" xr:uid="{0F29D32C-0E67-F248-8C35-9710D68A7F85}"/>
+    <hyperlink ref="D89" r:id="rId57" xr:uid="{BA71FBDC-01A3-4A48-BCA0-1C6E4893F910}"/>
     <hyperlink ref="D69" r:id="rId58" xr:uid="{9995D19A-7C18-FD4A-B802-9520BA771167}"/>
-    <hyperlink ref="D90" r:id="rId59" xr:uid="{304009F6-D9B7-CA4A-8889-BE080E8A7654}"/>
-    <hyperlink ref="D91" r:id="rId60" xr:uid="{4795B6FC-18EE-9043-8CE7-AF2924E6749D}"/>
-    <hyperlink ref="D93" r:id="rId61" xr:uid="{D578DF58-1254-4444-A5AA-946137A0D551}"/>
-    <hyperlink ref="D94" r:id="rId62" xr:uid="{18921900-3790-4748-9B02-AE7CF2E83568}"/>
-    <hyperlink ref="D92" r:id="rId63" xr:uid="{86F5F152-3AE3-C84D-9FFC-1DEDBE048190}"/>
-    <hyperlink ref="D95" r:id="rId64" xr:uid="{AD61CAC4-24BC-954B-A0DF-1642FA6C333B}"/>
-    <hyperlink ref="D96" r:id="rId65" xr:uid="{D07E7B17-1A5D-4544-BA76-5313EC783C1A}"/>
+    <hyperlink ref="D91" r:id="rId59" xr:uid="{304009F6-D9B7-CA4A-8889-BE080E8A7654}"/>
+    <hyperlink ref="D92" r:id="rId60" xr:uid="{4795B6FC-18EE-9043-8CE7-AF2924E6749D}"/>
+    <hyperlink ref="D94" r:id="rId61" xr:uid="{D578DF58-1254-4444-A5AA-946137A0D551}"/>
+    <hyperlink ref="D95" r:id="rId62" xr:uid="{18921900-3790-4748-9B02-AE7CF2E83568}"/>
+    <hyperlink ref="D93" r:id="rId63" xr:uid="{86F5F152-3AE3-C84D-9FFC-1DEDBE048190}"/>
+    <hyperlink ref="D96" r:id="rId64" xr:uid="{AD61CAC4-24BC-954B-A0DF-1642FA6C333B}"/>
+    <hyperlink ref="D97" r:id="rId65" xr:uid="{D07E7B17-1A5D-4544-BA76-5313EC783C1A}"/>
     <hyperlink ref="D77" r:id="rId66" xr:uid="{A15B0F1F-A780-1F46-B188-D9ABDB5704B5}"/>
-    <hyperlink ref="D97" r:id="rId67" xr:uid="{979D158A-596F-9A47-AB5E-A72097511FA1}"/>
+    <hyperlink ref="D98" r:id="rId67" xr:uid="{979D158A-596F-9A47-AB5E-A72097511FA1}"/>
     <hyperlink ref="D65" r:id="rId68" xr:uid="{A15BE685-A40C-734C-AD72-47F9BF601FDA}"/>
-    <hyperlink ref="D80" r:id="rId69" xr:uid="{FB025A70-6F06-4E4E-8984-BA9B9A2AF297}"/>
-    <hyperlink ref="D79" r:id="rId70" xr:uid="{1E58D491-53C2-2A42-A667-CC2FC0000945}"/>
-    <hyperlink ref="D99" r:id="rId71" xr:uid="{3ACCDC43-EF65-2A4A-A85E-EAF5CBC58797}"/>
-    <hyperlink ref="D100" r:id="rId72" xr:uid="{25D4D054-F5CD-6342-9DEC-8930BA66BE1A}"/>
-    <hyperlink ref="D101" r:id="rId73" xr:uid="{8CCF119F-F952-D34D-AF8C-DFB4362DB485}"/>
-    <hyperlink ref="D102" r:id="rId74" xr:uid="{54F9A12F-EE15-FF41-AC0A-F0A2DEAF65D5}"/>
-    <hyperlink ref="D106" r:id="rId75" xr:uid="{A324DF56-4206-4746-9CDE-46BC8817E2EB}"/>
-    <hyperlink ref="D107" r:id="rId76" xr:uid="{F809319C-4A84-3B46-A615-A43A53515FA1}"/>
-    <hyperlink ref="D108" r:id="rId77" xr:uid="{331E1E74-43DD-8B44-BF01-87A292B96D3E}"/>
-    <hyperlink ref="D110" r:id="rId78" xr:uid="{0450769E-D191-D142-8255-A056AD20F92E}"/>
+    <hyperlink ref="D81" r:id="rId69" xr:uid="{FB025A70-6F06-4E4E-8984-BA9B9A2AF297}"/>
+    <hyperlink ref="D80" r:id="rId70" xr:uid="{1E58D491-53C2-2A42-A667-CC2FC0000945}"/>
+    <hyperlink ref="D102" r:id="rId71" xr:uid="{3ACCDC43-EF65-2A4A-A85E-EAF5CBC58797}"/>
+    <hyperlink ref="D103" r:id="rId72" xr:uid="{25D4D054-F5CD-6342-9DEC-8930BA66BE1A}"/>
+    <hyperlink ref="D104" r:id="rId73" xr:uid="{8CCF119F-F952-D34D-AF8C-DFB4362DB485}"/>
+    <hyperlink ref="D105" r:id="rId74" xr:uid="{54F9A12F-EE15-FF41-AC0A-F0A2DEAF65D5}"/>
+    <hyperlink ref="D109" r:id="rId75" xr:uid="{A324DF56-4206-4746-9CDE-46BC8817E2EB}"/>
+    <hyperlink ref="D110" r:id="rId76" xr:uid="{F809319C-4A84-3B46-A615-A43A53515FA1}"/>
+    <hyperlink ref="D111" r:id="rId77" xr:uid="{331E1E74-43DD-8B44-BF01-87A292B96D3E}"/>
+    <hyperlink ref="D113" r:id="rId78" xr:uid="{0450769E-D191-D142-8255-A056AD20F92E}"/>
     <hyperlink ref="D57" r:id="rId79" xr:uid="{877003D4-412B-1C4A-B9C5-07DF56DA7218}"/>
     <hyperlink ref="D58" r:id="rId80" xr:uid="{BF399E5E-1ECA-414D-A2D4-57E85D27B367}"/>
-    <hyperlink ref="D112" r:id="rId81" xr:uid="{BB764D03-6EBC-9C46-ACF7-5FD301EB57E9}"/>
-    <hyperlink ref="D113" r:id="rId82" xr:uid="{E0E6E7A9-4B34-9D48-B226-2529539960C3}"/>
-    <hyperlink ref="D114" r:id="rId83" xr:uid="{EE01CD31-A0CC-FB4E-9234-D39DC44BBEF2}"/>
-    <hyperlink ref="D115" r:id="rId84" xr:uid="{3C47FF5A-BE3C-7C4E-829E-4945618A9C1F}"/>
-    <hyperlink ref="D116" r:id="rId85" xr:uid="{F5493FE6-0313-1940-AEFF-050A934E8083}"/>
-    <hyperlink ref="D117" r:id="rId86" xr:uid="{F415321A-3F49-EB4E-B6A9-EFE163590B41}"/>
-    <hyperlink ref="D118" r:id="rId87" xr:uid="{C84C6E00-5661-0D49-A0D1-CFD70865A82D}"/>
-    <hyperlink ref="D119" r:id="rId88" xr:uid="{E23DB724-160F-8543-B648-70EB7CA0365F}"/>
-    <hyperlink ref="D120" r:id="rId89" xr:uid="{E29FA1EF-7AB7-E245-832F-7B087D0E7EA3}"/>
-    <hyperlink ref="D121" r:id="rId90" xr:uid="{388C4274-E38A-B449-8F40-7ED095B192D7}"/>
-    <hyperlink ref="D122" r:id="rId91" xr:uid="{A966469C-688F-1E4F-8C89-F7E400609830}"/>
-    <hyperlink ref="D123" r:id="rId92" xr:uid="{51AA50DE-356B-3B4E-A1D7-15FC03EB6DB6}"/>
-    <hyperlink ref="D124" r:id="rId93" xr:uid="{2BB8B043-F3A9-1542-88EC-A24B529AC694}"/>
-    <hyperlink ref="D125" r:id="rId94" xr:uid="{3AB52AD0-26F6-2A4D-8680-5FE5164BC43C}"/>
-    <hyperlink ref="D126" r:id="rId95" xr:uid="{ABFD2F04-F17E-164A-9AB8-3642AE12D100}"/>
-    <hyperlink ref="D127" r:id="rId96" xr:uid="{B7708F6B-F6E6-BF41-8AF3-54C00F11C52B}"/>
-    <hyperlink ref="D130" r:id="rId97" xr:uid="{BF7922F0-DD27-EE45-AF85-5C9161DA389C}"/>
-    <hyperlink ref="D131" r:id="rId98" xr:uid="{BC00976C-C73B-6F4E-B032-65F2D572F141}"/>
-    <hyperlink ref="D132" r:id="rId99" xr:uid="{77C86A54-F6B8-BA40-A768-CCB7D4C99562}"/>
-    <hyperlink ref="D133" r:id="rId100" xr:uid="{CAB158A3-D761-8448-A767-9525660B6326}"/>
-    <hyperlink ref="D134" r:id="rId101" xr:uid="{B81333A7-85AC-474E-BED5-5D3E104F7A1D}"/>
-    <hyperlink ref="D135" r:id="rId102" xr:uid="{34BE3A49-BE9D-4049-97A0-80E02A01A961}"/>
-    <hyperlink ref="D128" r:id="rId103" xr:uid="{781FF30D-914F-7841-92BF-6AD62300904B}"/>
-    <hyperlink ref="D129" r:id="rId104" xr:uid="{3CBAAA26-1E37-B044-B755-258229968E67}"/>
-    <hyperlink ref="D136" r:id="rId105" xr:uid="{DCC7B2BC-EB59-DB49-9BF9-45BF0E030221}"/>
-    <hyperlink ref="D137" r:id="rId106" xr:uid="{22C8D3B5-CBB9-C448-83B5-05CE9F72E696}"/>
-    <hyperlink ref="D138" r:id="rId107" xr:uid="{A3C5359E-186C-1640-839A-F7F1B599F0B5}"/>
-    <hyperlink ref="D139" r:id="rId108" xr:uid="{CD78268C-7DEC-FB44-88AA-75EC6DE77C62}"/>
-    <hyperlink ref="D140" r:id="rId109" xr:uid="{5BC45F49-43E2-5D46-B9F7-C9DE4586524D}"/>
-    <hyperlink ref="D141" r:id="rId110" xr:uid="{3B77FB2E-5F37-D04A-B1B0-08D6A165225B}"/>
-    <hyperlink ref="D142" r:id="rId111" xr:uid="{6EA4E64A-6FFB-FC43-A3F9-B515DC03D9ED}"/>
-    <hyperlink ref="D143" r:id="rId112" xr:uid="{7D0BC227-6BA4-F747-B1DB-B7CCF5D3057E}"/>
-    <hyperlink ref="D144" r:id="rId113" xr:uid="{19FE4A6D-FF5E-BF49-8C4B-F24B3005865C}"/>
-    <hyperlink ref="D145" r:id="rId114" xr:uid="{41D1D3F0-3B5D-964A-BC98-E26309342AC6}"/>
-    <hyperlink ref="D147" r:id="rId115" xr:uid="{C852E2F0-FC27-4F41-89CD-E264B7CB2DF7}"/>
-    <hyperlink ref="D148" r:id="rId116" xr:uid="{DF3B379B-CACF-954D-AEAA-0FF3E835924A}"/>
-    <hyperlink ref="D149" r:id="rId117" xr:uid="{7FADB0C5-8AA0-6F41-A92E-5B09572E4D18}"/>
-    <hyperlink ref="D150" r:id="rId118" xr:uid="{3103A3F7-AC33-1C4E-BCE8-2934FE92BC5F}"/>
-    <hyperlink ref="D151" r:id="rId119" xr:uid="{07DF88EF-4EAA-1440-8D82-60A0FD7CADD1}"/>
-    <hyperlink ref="D152" r:id="rId120" xr:uid="{E19890F5-0215-4644-AEA1-BF7692385DF1}"/>
-    <hyperlink ref="D153" r:id="rId121" xr:uid="{86B64C9A-DAFF-CF44-A151-29AA7D14977F}"/>
-    <hyperlink ref="D154" r:id="rId122" xr:uid="{3FEFD335-04F9-4F41-B6A0-B080D6550649}"/>
-    <hyperlink ref="D155" r:id="rId123" xr:uid="{90B99E7F-0693-D54F-A4F6-34AD69A3D631}"/>
-    <hyperlink ref="D156" r:id="rId124" xr:uid="{B95F960A-6D1F-2D47-8457-F9DE115B5C38}"/>
-    <hyperlink ref="D157" r:id="rId125" xr:uid="{00ECE393-EC26-344F-8B40-377C3EB5D890}"/>
-    <hyperlink ref="D158" r:id="rId126" xr:uid="{C28E61A4-8435-BF4D-8BA4-7A3647FBFF00}"/>
-    <hyperlink ref="D159" r:id="rId127" xr:uid="{3CAEF1A6-A029-A64D-903F-EB0ADFF46D37}"/>
-    <hyperlink ref="D160" r:id="rId128" xr:uid="{9DF090F0-97A2-E946-850D-1ECC6DB92707}"/>
-    <hyperlink ref="D161" r:id="rId129" xr:uid="{C85A63BA-1F71-584A-A604-B6AB345ECE95}"/>
-    <hyperlink ref="D86" r:id="rId130" xr:uid="{2F59B8F2-7AB0-AE47-85CD-C244BB59B3BA}"/>
-    <hyperlink ref="D162" r:id="rId131" xr:uid="{06DC547A-085D-7C45-A4F0-49F7349DAAB0}"/>
-    <hyperlink ref="D163" r:id="rId132" xr:uid="{D65368D6-C0A7-5B4C-83C0-4DFB768DE3C6}"/>
-    <hyperlink ref="D164" r:id="rId133" xr:uid="{B7606443-1D1E-724A-8040-131FD0AC6338}"/>
-    <hyperlink ref="D165" r:id="rId134" xr:uid="{79B43F1F-03A0-F747-AC05-79F3D0B4BCCB}"/>
-    <hyperlink ref="D166" r:id="rId135" location="m_tab-one-panel" xr:uid="{93BFFC1A-D0D5-4A47-B941-A198EF5A5C4C}"/>
-    <hyperlink ref="D167" r:id="rId136" xr:uid="{875EF5F0-7651-8745-87D6-636AD559D72E}"/>
-    <hyperlink ref="D168" r:id="rId137" xr:uid="{6E4DCDAE-D012-BD4D-A394-90B249BB99C5}"/>
-    <hyperlink ref="D169" r:id="rId138" xr:uid="{3DAD8E8C-E2BB-074B-B3F0-D475C7FD6B2D}"/>
-    <hyperlink ref="D170" r:id="rId139" xr:uid="{222D21AE-1088-BD48-BAEE-1EF3912460AF}"/>
-    <hyperlink ref="D171" r:id="rId140" xr:uid="{7AD5FFD0-8F45-1941-9BBF-D91BBC4F0F40}"/>
-    <hyperlink ref="D172" r:id="rId141" xr:uid="{75C68380-CD77-B746-9EA5-48AAFF4A4F72}"/>
-    <hyperlink ref="D173" r:id="rId142" xr:uid="{518258DC-5A20-3D40-91D0-D032DC42B6AD}"/>
-    <hyperlink ref="D174" r:id="rId143" xr:uid="{5B069AF2-81F6-A34E-80A0-7E8EBE3DFA2A}"/>
-    <hyperlink ref="D175" r:id="rId144" xr:uid="{A04E8385-1CE9-364E-91A1-6F09D76ACF42}"/>
-    <hyperlink ref="D176" r:id="rId145" xr:uid="{3113EFF0-EE9A-354C-8BD1-5D9364B99893}"/>
-    <hyperlink ref="D177" r:id="rId146" xr:uid="{A06F9F88-431E-574D-92C0-E68077FC529D}"/>
-    <hyperlink ref="D178" r:id="rId147" xr:uid="{8B4EF43A-AE24-6947-8EFA-E38936068D18}"/>
-    <hyperlink ref="C179" r:id="rId148" display="https://www.bostonmpo.org/node/3243" xr:uid="{655CEEAA-6095-9B47-995E-CD64750746E0}"/>
-    <hyperlink ref="D179" r:id="rId149" xr:uid="{055A514B-7345-F948-9754-CCC9031C0081}"/>
-    <hyperlink ref="D180" r:id="rId150" xr:uid="{90B28A53-CDAB-EC48-9FC0-0E277128FCA7}"/>
-    <hyperlink ref="D181" r:id="rId151" xr:uid="{AC529FF5-CF2C-1D4B-95AB-70ED1909D783}"/>
-    <hyperlink ref="D182" r:id="rId152" xr:uid="{ECE456D6-90BA-E547-8B10-93E537F7BF40}"/>
-    <hyperlink ref="D183" r:id="rId153" xr:uid="{2686E174-B756-124D-82F8-89B4FFA6EE04}"/>
-    <hyperlink ref="D184" r:id="rId154" xr:uid="{F529B5BA-08ED-3642-9481-1E3CCADBB5B4}"/>
-    <hyperlink ref="D185" r:id="rId155" xr:uid="{0D583AB0-0EC1-4143-9730-B654F3258218}"/>
-    <hyperlink ref="D186" r:id="rId156" xr:uid="{D3776250-774B-AB40-A8B2-B7A3B3F11494}"/>
-    <hyperlink ref="D187" r:id="rId157" xr:uid="{23909CD0-3230-734E-8EA2-DD5D2BACF318}"/>
-    <hyperlink ref="D188" r:id="rId158" xr:uid="{AA593C04-D717-4846-89DA-AED5EC901B9D}"/>
-    <hyperlink ref="D189" r:id="rId159" xr:uid="{816B8DD7-C959-7845-A7B3-E11200634DE3}"/>
-    <hyperlink ref="D191" r:id="rId160" xr:uid="{8E6DE810-4336-264A-9286-F5DE4FCB3616}"/>
-    <hyperlink ref="D192" r:id="rId161" xr:uid="{74958D82-AE52-764E-A4F1-2CBA9EA9ACED}"/>
-    <hyperlink ref="D193" r:id="rId162" xr:uid="{4C8C770A-DBF9-8447-AF54-9001929EDD34}"/>
-    <hyperlink ref="D195" r:id="rId163" xr:uid="{263568FF-4DC1-A245-B266-0B8D89A595BD}"/>
-    <hyperlink ref="D196" r:id="rId164" xr:uid="{0BB8C344-5E31-7E4A-927C-AF47B71575BB}"/>
-    <hyperlink ref="D197" r:id="rId165" xr:uid="{903A7E98-5E9D-544C-B0B8-8E7D2C9D47EB}"/>
-    <hyperlink ref="D198" r:id="rId166" xr:uid="{F5E4C67A-545A-BD44-B2A4-28AFA52502AF}"/>
-    <hyperlink ref="D201" r:id="rId167" xr:uid="{2690B48D-BA39-6543-BD43-72740F6D06FB}"/>
-    <hyperlink ref="D202" r:id="rId168" xr:uid="{CA43EE9E-6054-8246-8F09-73619591E4D8}"/>
-    <hyperlink ref="D204" r:id="rId169" xr:uid="{3EBDCE69-25F1-DF45-8571-96E339A1E1A0}"/>
-    <hyperlink ref="D206" r:id="rId170" xr:uid="{5BBBF668-7181-034B-A7E7-B37F0489798D}"/>
-    <hyperlink ref="D207" r:id="rId171" xr:uid="{F25E9123-06C3-4D48-8368-7DC4D8ADFDFE}"/>
-    <hyperlink ref="D210" r:id="rId172" xr:uid="{FE44C4D8-FAA2-6C4A-A061-1E08E9AF9BAE}"/>
-    <hyperlink ref="D211" r:id="rId173" xr:uid="{4A0071B2-48C3-F840-B489-A422B212DF05}"/>
-    <hyperlink ref="D212" r:id="rId174" xr:uid="{0BD877BC-868A-5E4A-987A-4883C51D584C}"/>
-    <hyperlink ref="D213" r:id="rId175" xr:uid="{2E6F2974-F899-5A46-8475-0ADAA6834181}"/>
-    <hyperlink ref="D214" r:id="rId176" xr:uid="{17A16738-54AE-5341-A2C1-7CAA2A130FDC}"/>
-    <hyperlink ref="D216" r:id="rId177" xr:uid="{F7F59C8F-6228-3744-8DF6-9F3A5D6E4A08}"/>
-    <hyperlink ref="D217" r:id="rId178" xr:uid="{79DF1E50-4B51-1348-A8D4-285C17AE4342}"/>
-    <hyperlink ref="D218" r:id="rId179" xr:uid="{8156E09C-4D4B-844F-9152-763F5CBB848C}"/>
-    <hyperlink ref="D219" r:id="rId180" xr:uid="{D66FD1BC-2A48-1D44-9C56-A2091EA6EB4F}"/>
-    <hyperlink ref="D220" r:id="rId181" xr:uid="{EED901F1-9FA7-0241-A3A8-1DEC4ADB4F65}"/>
-    <hyperlink ref="D215" r:id="rId182" xr:uid="{ACBAEB0F-A745-BD4B-A79F-28E87E3B7670}"/>
-    <hyperlink ref="D208" r:id="rId183" xr:uid="{6FE5FEA9-69D3-5B44-8339-E00169C80FE7}"/>
-    <hyperlink ref="D221" r:id="rId184" xr:uid="{4E39217A-DB80-A04A-A66F-DC478E8BD9B0}"/>
-    <hyperlink ref="D223" r:id="rId185" xr:uid="{FD84BB06-83F9-8145-B29B-E82DD0A255FA}"/>
-    <hyperlink ref="D224" r:id="rId186" xr:uid="{0F664415-A56C-5944-BD33-2BBC535C69EE}"/>
-    <hyperlink ref="D225" r:id="rId187" xr:uid="{1B9FDFCF-CDAA-B043-90DF-464B3F19D029}"/>
-    <hyperlink ref="D226" r:id="rId188" xr:uid="{87374CD1-533B-1843-AFD1-A46E4CCC2786}"/>
-    <hyperlink ref="D227" r:id="rId189" xr:uid="{735892DA-3CF9-7D43-938E-C539C1354F7E}"/>
-    <hyperlink ref="D228" r:id="rId190" xr:uid="{25B8E5AB-DD5E-B943-A89D-CF3BCFD8C69D}"/>
-    <hyperlink ref="D229" r:id="rId191" xr:uid="{863254B5-D467-6A40-9BF8-0E3F61B42855}"/>
-    <hyperlink ref="D230" r:id="rId192" xr:uid="{88692FC1-C0F6-FC43-99D6-5645F4B9C696}"/>
-    <hyperlink ref="D231" r:id="rId193" xr:uid="{67565600-29EE-EF48-A979-42DB827EFA61}"/>
-    <hyperlink ref="D232" r:id="rId194" xr:uid="{39827F30-B6A3-1543-AD30-4EAFB12E07F9}"/>
-    <hyperlink ref="D200" r:id="rId195" xr:uid="{70051547-7009-DA49-AD8A-CDA173903436}"/>
-    <hyperlink ref="D233" r:id="rId196" xr:uid="{1F55836F-92FB-504B-8890-DD155568B08F}"/>
-    <hyperlink ref="D234" r:id="rId197" xr:uid="{516BA828-1E71-6740-82CE-9ABCB5B2868A}"/>
-    <hyperlink ref="D235" r:id="rId198" xr:uid="{D01BC6DD-63D5-FE45-8701-DE7626C47912}"/>
-    <hyperlink ref="D236" r:id="rId199" xr:uid="{7F25EAA1-3640-2140-8ED9-4C0C8A766B64}"/>
-    <hyperlink ref="D237" r:id="rId200" location="the-ted-williams-tunnel-" xr:uid="{90CDFCE7-A34F-B543-940D-CBD77B3CA490}"/>
-    <hyperlink ref="D239" r:id="rId201" xr:uid="{33076741-07BA-AD48-9CFF-1F8FA7DC794F}"/>
-    <hyperlink ref="D240" r:id="rId202" xr:uid="{ED191C2D-42FA-B247-8E12-4DAE06218C0C}"/>
-    <hyperlink ref="D241" r:id="rId203" xr:uid="{E2C2519F-06D0-F54F-A190-1006654C1217}"/>
-    <hyperlink ref="D243" r:id="rId204" xr:uid="{21200567-2A05-1B4A-9286-23765C1B5439}"/>
-    <hyperlink ref="D244" r:id="rId205" xr:uid="{3B0065D2-6C14-4643-8519-9BB3E1ABBAC7}"/>
-    <hyperlink ref="D246" r:id="rId206" xr:uid="{8DEBC386-B35E-BF4D-830F-B313B531F036}"/>
-    <hyperlink ref="D247" r:id="rId207" xr:uid="{2CD55170-8C56-B640-8914-62FD2B471773}"/>
-    <hyperlink ref="D245" r:id="rId208" xr:uid="{C5C05C21-059D-3E4F-83CE-07DE43CA77F8}"/>
-    <hyperlink ref="D250" r:id="rId209" xr:uid="{5A018FFC-E064-B841-B16C-1B5FDB1C2373}"/>
-    <hyperlink ref="D251" r:id="rId210" xr:uid="{9ECC5CD3-0C49-6241-9ADA-4B8F147F222D}"/>
-    <hyperlink ref="D248" r:id="rId211" xr:uid="{033BB178-31A9-3E47-B7EC-D294053A56E7}"/>
-    <hyperlink ref="D249" r:id="rId212" xr:uid="{5F8349BB-359A-7949-9708-480CAB866631}"/>
-    <hyperlink ref="D252" r:id="rId213" xr:uid="{79509633-6320-7F4C-8E22-C5B4BAEC20D7}"/>
-    <hyperlink ref="D253" r:id="rId214" xr:uid="{A70D9607-0490-DF4E-85B3-794BEB0DB3CD}"/>
-    <hyperlink ref="D254" r:id="rId215" xr:uid="{7F93E30A-E771-E541-A3E8-E8E115BAC442}"/>
-    <hyperlink ref="D255" r:id="rId216" xr:uid="{DF50B5D9-DAAC-7043-8DA2-3DBF2FCB4882}"/>
-    <hyperlink ref="D257" r:id="rId217" xr:uid="{88721544-7A83-0045-B6A7-188448608657}"/>
-    <hyperlink ref="D256" r:id="rId218" xr:uid="{83108E31-6FB4-974C-8A81-89A0D5728752}"/>
-    <hyperlink ref="D238" r:id="rId219" xr:uid="{2930C349-E6B7-544B-BB2A-773A46E73BCB}"/>
-    <hyperlink ref="D222" r:id="rId220" xr:uid="{2BE70040-B75E-144F-8CF2-C6FAF265243F}"/>
-    <hyperlink ref="D258" r:id="rId221" xr:uid="{69A55749-D9D2-1B4B-B3F9-4B160F762593}"/>
-    <hyperlink ref="D259" r:id="rId222" xr:uid="{FB9E4799-0707-754B-9240-DFB8EFCF3420}"/>
-    <hyperlink ref="D260" r:id="rId223" xr:uid="{EFA9A5C9-A935-FD44-A8C3-75A6D42D9D41}"/>
+    <hyperlink ref="D115" r:id="rId81" xr:uid="{BB764D03-6EBC-9C46-ACF7-5FD301EB57E9}"/>
+    <hyperlink ref="D116" r:id="rId82" xr:uid="{E0E6E7A9-4B34-9D48-B226-2529539960C3}"/>
+    <hyperlink ref="D117" r:id="rId83" xr:uid="{EE01CD31-A0CC-FB4E-9234-D39DC44BBEF2}"/>
+    <hyperlink ref="D118" r:id="rId84" xr:uid="{3C47FF5A-BE3C-7C4E-829E-4945618A9C1F}"/>
+    <hyperlink ref="D119" r:id="rId85" xr:uid="{F5493FE6-0313-1940-AEFF-050A934E8083}"/>
+    <hyperlink ref="D120" r:id="rId86" xr:uid="{F415321A-3F49-EB4E-B6A9-EFE163590B41}"/>
+    <hyperlink ref="D121" r:id="rId87" xr:uid="{C84C6E00-5661-0D49-A0D1-CFD70865A82D}"/>
+    <hyperlink ref="D122" r:id="rId88" xr:uid="{E23DB724-160F-8543-B648-70EB7CA0365F}"/>
+    <hyperlink ref="D123" r:id="rId89" xr:uid="{E29FA1EF-7AB7-E245-832F-7B087D0E7EA3}"/>
+    <hyperlink ref="D124" r:id="rId90" xr:uid="{388C4274-E38A-B449-8F40-7ED095B192D7}"/>
+    <hyperlink ref="D125" r:id="rId91" xr:uid="{A966469C-688F-1E4F-8C89-F7E400609830}"/>
+    <hyperlink ref="D126" r:id="rId92" xr:uid="{51AA50DE-356B-3B4E-A1D7-15FC03EB6DB6}"/>
+    <hyperlink ref="D127" r:id="rId93" xr:uid="{2BB8B043-F3A9-1542-88EC-A24B529AC694}"/>
+    <hyperlink ref="D128" r:id="rId94" xr:uid="{3AB52AD0-26F6-2A4D-8680-5FE5164BC43C}"/>
+    <hyperlink ref="D129" r:id="rId95" xr:uid="{ABFD2F04-F17E-164A-9AB8-3642AE12D100}"/>
+    <hyperlink ref="D130" r:id="rId96" xr:uid="{B7708F6B-F6E6-BF41-8AF3-54C00F11C52B}"/>
+    <hyperlink ref="D133" r:id="rId97" xr:uid="{BF7922F0-DD27-EE45-AF85-5C9161DA389C}"/>
+    <hyperlink ref="D134" r:id="rId98" xr:uid="{BC00976C-C73B-6F4E-B032-65F2D572F141}"/>
+    <hyperlink ref="D135" r:id="rId99" xr:uid="{77C86A54-F6B8-BA40-A768-CCB7D4C99562}"/>
+    <hyperlink ref="D136" r:id="rId100" xr:uid="{CAB158A3-D761-8448-A767-9525660B6326}"/>
+    <hyperlink ref="D137" r:id="rId101" xr:uid="{B81333A7-85AC-474E-BED5-5D3E104F7A1D}"/>
+    <hyperlink ref="D138" r:id="rId102" xr:uid="{34BE3A49-BE9D-4049-97A0-80E02A01A961}"/>
+    <hyperlink ref="D131" r:id="rId103" xr:uid="{781FF30D-914F-7841-92BF-6AD62300904B}"/>
+    <hyperlink ref="D132" r:id="rId104" xr:uid="{3CBAAA26-1E37-B044-B755-258229968E67}"/>
+    <hyperlink ref="D139" r:id="rId105" xr:uid="{DCC7B2BC-EB59-DB49-9BF9-45BF0E030221}"/>
+    <hyperlink ref="D140" r:id="rId106" xr:uid="{22C8D3B5-CBB9-C448-83B5-05CE9F72E696}"/>
+    <hyperlink ref="D141" r:id="rId107" xr:uid="{A3C5359E-186C-1640-839A-F7F1B599F0B5}"/>
+    <hyperlink ref="D142" r:id="rId108" xr:uid="{CD78268C-7DEC-FB44-88AA-75EC6DE77C62}"/>
+    <hyperlink ref="D143" r:id="rId109" xr:uid="{5BC45F49-43E2-5D46-B9F7-C9DE4586524D}"/>
+    <hyperlink ref="D144" r:id="rId110" xr:uid="{3B77FB2E-5F37-D04A-B1B0-08D6A165225B}"/>
+    <hyperlink ref="D145" r:id="rId111" xr:uid="{6EA4E64A-6FFB-FC43-A3F9-B515DC03D9ED}"/>
+    <hyperlink ref="D146" r:id="rId112" xr:uid="{7D0BC227-6BA4-F747-B1DB-B7CCF5D3057E}"/>
+    <hyperlink ref="D147" r:id="rId113" xr:uid="{19FE4A6D-FF5E-BF49-8C4B-F24B3005865C}"/>
+    <hyperlink ref="D148" r:id="rId114" xr:uid="{41D1D3F0-3B5D-964A-BC98-E26309342AC6}"/>
+    <hyperlink ref="D150" r:id="rId115" xr:uid="{C852E2F0-FC27-4F41-89CD-E264B7CB2DF7}"/>
+    <hyperlink ref="D151" r:id="rId116" xr:uid="{DF3B379B-CACF-954D-AEAA-0FF3E835924A}"/>
+    <hyperlink ref="D152" r:id="rId117" xr:uid="{7FADB0C5-8AA0-6F41-A92E-5B09572E4D18}"/>
+    <hyperlink ref="D153" r:id="rId118" xr:uid="{3103A3F7-AC33-1C4E-BCE8-2934FE92BC5F}"/>
+    <hyperlink ref="D154" r:id="rId119" xr:uid="{07DF88EF-4EAA-1440-8D82-60A0FD7CADD1}"/>
+    <hyperlink ref="D155" r:id="rId120" xr:uid="{E19890F5-0215-4644-AEA1-BF7692385DF1}"/>
+    <hyperlink ref="D156" r:id="rId121" xr:uid="{86B64C9A-DAFF-CF44-A151-29AA7D14977F}"/>
+    <hyperlink ref="D157" r:id="rId122" xr:uid="{3FEFD335-04F9-4F41-B6A0-B080D6550649}"/>
+    <hyperlink ref="D158" r:id="rId123" xr:uid="{90B99E7F-0693-D54F-A4F6-34AD69A3D631}"/>
+    <hyperlink ref="D159" r:id="rId124" xr:uid="{B95F960A-6D1F-2D47-8457-F9DE115B5C38}"/>
+    <hyperlink ref="D160" r:id="rId125" xr:uid="{00ECE393-EC26-344F-8B40-377C3EB5D890}"/>
+    <hyperlink ref="D161" r:id="rId126" xr:uid="{C28E61A4-8435-BF4D-8BA4-7A3647FBFF00}"/>
+    <hyperlink ref="D162" r:id="rId127" xr:uid="{3CAEF1A6-A029-A64D-903F-EB0ADFF46D37}"/>
+    <hyperlink ref="D163" r:id="rId128" xr:uid="{9DF090F0-97A2-E946-850D-1ECC6DB92707}"/>
+    <hyperlink ref="D164" r:id="rId129" xr:uid="{C85A63BA-1F71-584A-A604-B6AB345ECE95}"/>
+    <hyperlink ref="D87" r:id="rId130" xr:uid="{2F59B8F2-7AB0-AE47-85CD-C244BB59B3BA}"/>
+    <hyperlink ref="D165" r:id="rId131" xr:uid="{06DC547A-085D-7C45-A4F0-49F7349DAAB0}"/>
+    <hyperlink ref="D166" r:id="rId132" xr:uid="{D65368D6-C0A7-5B4C-83C0-4DFB768DE3C6}"/>
+    <hyperlink ref="D167" r:id="rId133" xr:uid="{B7606443-1D1E-724A-8040-131FD0AC6338}"/>
+    <hyperlink ref="D168" r:id="rId134" xr:uid="{79B43F1F-03A0-F747-AC05-79F3D0B4BCCB}"/>
+    <hyperlink ref="D169" r:id="rId135" location="m_tab-one-panel" xr:uid="{93BFFC1A-D0D5-4A47-B941-A198EF5A5C4C}"/>
+    <hyperlink ref="D170" r:id="rId136" xr:uid="{875EF5F0-7651-8745-87D6-636AD559D72E}"/>
+    <hyperlink ref="D171" r:id="rId137" xr:uid="{6E4DCDAE-D012-BD4D-A394-90B249BB99C5}"/>
+    <hyperlink ref="D172" r:id="rId138" xr:uid="{3DAD8E8C-E2BB-074B-B3F0-D475C7FD6B2D}"/>
+    <hyperlink ref="D173" r:id="rId139" xr:uid="{222D21AE-1088-BD48-BAEE-1EF3912460AF}"/>
+    <hyperlink ref="D174" r:id="rId140" xr:uid="{7AD5FFD0-8F45-1941-9BBF-D91BBC4F0F40}"/>
+    <hyperlink ref="D175" r:id="rId141" xr:uid="{75C68380-CD77-B746-9EA5-48AAFF4A4F72}"/>
+    <hyperlink ref="D176" r:id="rId142" xr:uid="{518258DC-5A20-3D40-91D0-D032DC42B6AD}"/>
+    <hyperlink ref="D177" r:id="rId143" xr:uid="{5B069AF2-81F6-A34E-80A0-7E8EBE3DFA2A}"/>
+    <hyperlink ref="D178" r:id="rId144" xr:uid="{A04E8385-1CE9-364E-91A1-6F09D76ACF42}"/>
+    <hyperlink ref="D179" r:id="rId145" xr:uid="{3113EFF0-EE9A-354C-8BD1-5D9364B99893}"/>
+    <hyperlink ref="D180" r:id="rId146" xr:uid="{A06F9F88-431E-574D-92C0-E68077FC529D}"/>
+    <hyperlink ref="D181" r:id="rId147" xr:uid="{8B4EF43A-AE24-6947-8EFA-E38936068D18}"/>
+    <hyperlink ref="C182" r:id="rId148" display="https://www.bostonmpo.org/node/3243" xr:uid="{655CEEAA-6095-9B47-995E-CD64750746E0}"/>
+    <hyperlink ref="D182" r:id="rId149" xr:uid="{055A514B-7345-F948-9754-CCC9031C0081}"/>
+    <hyperlink ref="D183" r:id="rId150" xr:uid="{90B28A53-CDAB-EC48-9FC0-0E277128FCA7}"/>
+    <hyperlink ref="D184" r:id="rId151" xr:uid="{AC529FF5-CF2C-1D4B-95AB-70ED1909D783}"/>
+    <hyperlink ref="D185" r:id="rId152" xr:uid="{ECE456D6-90BA-E547-8B10-93E537F7BF40}"/>
+    <hyperlink ref="D186" r:id="rId153" xr:uid="{2686E174-B756-124D-82F8-89B4FFA6EE04}"/>
+    <hyperlink ref="D187" r:id="rId154" xr:uid="{F529B5BA-08ED-3642-9481-1E3CCADBB5B4}"/>
+    <hyperlink ref="D188" r:id="rId155" xr:uid="{0D583AB0-0EC1-4143-9730-B654F3258218}"/>
+    <hyperlink ref="D189" r:id="rId156" xr:uid="{D3776250-774B-AB40-A8B2-B7A3B3F11494}"/>
+    <hyperlink ref="D190" r:id="rId157" xr:uid="{23909CD0-3230-734E-8EA2-DD5D2BACF318}"/>
+    <hyperlink ref="D191" r:id="rId158" xr:uid="{AA593C04-D717-4846-89DA-AED5EC901B9D}"/>
+    <hyperlink ref="D192" r:id="rId159" xr:uid="{816B8DD7-C959-7845-A7B3-E11200634DE3}"/>
+    <hyperlink ref="D194" r:id="rId160" xr:uid="{8E6DE810-4336-264A-9286-F5DE4FCB3616}"/>
+    <hyperlink ref="D195" r:id="rId161" xr:uid="{74958D82-AE52-764E-A4F1-2CBA9EA9ACED}"/>
+    <hyperlink ref="D196" r:id="rId162" xr:uid="{4C8C770A-DBF9-8447-AF54-9001929EDD34}"/>
+    <hyperlink ref="D198" r:id="rId163" xr:uid="{263568FF-4DC1-A245-B266-0B8D89A595BD}"/>
+    <hyperlink ref="D199" r:id="rId164" xr:uid="{0BB8C344-5E31-7E4A-927C-AF47B71575BB}"/>
+    <hyperlink ref="D200" r:id="rId165" xr:uid="{903A7E98-5E9D-544C-B0B8-8E7D2C9D47EB}"/>
+    <hyperlink ref="D201" r:id="rId166" xr:uid="{F5E4C67A-545A-BD44-B2A4-28AFA52502AF}"/>
+    <hyperlink ref="D204" r:id="rId167" xr:uid="{2690B48D-BA39-6543-BD43-72740F6D06FB}"/>
+    <hyperlink ref="D205" r:id="rId168" xr:uid="{CA43EE9E-6054-8246-8F09-73619591E4D8}"/>
+    <hyperlink ref="D207" r:id="rId169" xr:uid="{3EBDCE69-25F1-DF45-8571-96E339A1E1A0}"/>
+    <hyperlink ref="D209" r:id="rId170" xr:uid="{5BBBF668-7181-034B-A7E7-B37F0489798D}"/>
+    <hyperlink ref="D210" r:id="rId171" xr:uid="{F25E9123-06C3-4D48-8368-7DC4D8ADFDFE}"/>
+    <hyperlink ref="D213" r:id="rId172" xr:uid="{FE44C4D8-FAA2-6C4A-A061-1E08E9AF9BAE}"/>
+    <hyperlink ref="D214" r:id="rId173" xr:uid="{4A0071B2-48C3-F840-B489-A422B212DF05}"/>
+    <hyperlink ref="D215" r:id="rId174" xr:uid="{0BD877BC-868A-5E4A-987A-4883C51D584C}"/>
+    <hyperlink ref="D216" r:id="rId175" xr:uid="{2E6F2974-F899-5A46-8475-0ADAA6834181}"/>
+    <hyperlink ref="D217" r:id="rId176" xr:uid="{17A16738-54AE-5341-A2C1-7CAA2A130FDC}"/>
+    <hyperlink ref="D219" r:id="rId177" xr:uid="{F7F59C8F-6228-3744-8DF6-9F3A5D6E4A08}"/>
+    <hyperlink ref="D220" r:id="rId178" xr:uid="{79DF1E50-4B51-1348-A8D4-285C17AE4342}"/>
+    <hyperlink ref="D221" r:id="rId179" xr:uid="{8156E09C-4D4B-844F-9152-763F5CBB848C}"/>
+    <hyperlink ref="D222" r:id="rId180" xr:uid="{D66FD1BC-2A48-1D44-9C56-A2091EA6EB4F}"/>
+    <hyperlink ref="D223" r:id="rId181" xr:uid="{EED901F1-9FA7-0241-A3A8-1DEC4ADB4F65}"/>
+    <hyperlink ref="D218" r:id="rId182" xr:uid="{ACBAEB0F-A745-BD4B-A79F-28E87E3B7670}"/>
+    <hyperlink ref="D211" r:id="rId183" xr:uid="{6FE5FEA9-69D3-5B44-8339-E00169C80FE7}"/>
+    <hyperlink ref="D224" r:id="rId184" xr:uid="{4E39217A-DB80-A04A-A66F-DC478E8BD9B0}"/>
+    <hyperlink ref="D226" r:id="rId185" xr:uid="{FD84BB06-83F9-8145-B29B-E82DD0A255FA}"/>
+    <hyperlink ref="D227" r:id="rId186" xr:uid="{0F664415-A56C-5944-BD33-2BBC535C69EE}"/>
+    <hyperlink ref="D228" r:id="rId187" xr:uid="{1B9FDFCF-CDAA-B043-90DF-464B3F19D029}"/>
+    <hyperlink ref="D229" r:id="rId188" xr:uid="{87374CD1-533B-1843-AFD1-A46E4CCC2786}"/>
+    <hyperlink ref="D230" r:id="rId189" xr:uid="{735892DA-3CF9-7D43-938E-C539C1354F7E}"/>
+    <hyperlink ref="D231" r:id="rId190" xr:uid="{25B8E5AB-DD5E-B943-A89D-CF3BCFD8C69D}"/>
+    <hyperlink ref="D232" r:id="rId191" xr:uid="{863254B5-D467-6A40-9BF8-0E3F61B42855}"/>
+    <hyperlink ref="D233" r:id="rId192" xr:uid="{88692FC1-C0F6-FC43-99D6-5645F4B9C696}"/>
+    <hyperlink ref="D234" r:id="rId193" xr:uid="{67565600-29EE-EF48-A979-42DB827EFA61}"/>
+    <hyperlink ref="D235" r:id="rId194" xr:uid="{39827F30-B6A3-1543-AD30-4EAFB12E07F9}"/>
+    <hyperlink ref="D203" r:id="rId195" xr:uid="{70051547-7009-DA49-AD8A-CDA173903436}"/>
+    <hyperlink ref="D236" r:id="rId196" xr:uid="{1F55836F-92FB-504B-8890-DD155568B08F}"/>
+    <hyperlink ref="D237" r:id="rId197" xr:uid="{516BA828-1E71-6740-82CE-9ABCB5B2868A}"/>
+    <hyperlink ref="D238" r:id="rId198" xr:uid="{D01BC6DD-63D5-FE45-8701-DE7626C47912}"/>
+    <hyperlink ref="D239" r:id="rId199" xr:uid="{7F25EAA1-3640-2140-8ED9-4C0C8A766B64}"/>
+    <hyperlink ref="D240" r:id="rId200" location="the-ted-williams-tunnel-" xr:uid="{90CDFCE7-A34F-B543-940D-CBD77B3CA490}"/>
+    <hyperlink ref="D242" r:id="rId201" xr:uid="{33076741-07BA-AD48-9CFF-1F8FA7DC794F}"/>
+    <hyperlink ref="D243" r:id="rId202" xr:uid="{ED191C2D-42FA-B247-8E12-4DAE06218C0C}"/>
+    <hyperlink ref="D244" r:id="rId203" xr:uid="{E2C2519F-06D0-F54F-A190-1006654C1217}"/>
+    <hyperlink ref="D246" r:id="rId204" xr:uid="{21200567-2A05-1B4A-9286-23765C1B5439}"/>
+    <hyperlink ref="D247" r:id="rId205" xr:uid="{3B0065D2-6C14-4643-8519-9BB3E1ABBAC7}"/>
+    <hyperlink ref="D249" r:id="rId206" xr:uid="{8DEBC386-B35E-BF4D-830F-B313B531F036}"/>
+    <hyperlink ref="D250" r:id="rId207" xr:uid="{2CD55170-8C56-B640-8914-62FD2B471773}"/>
+    <hyperlink ref="D248" r:id="rId208" xr:uid="{C5C05C21-059D-3E4F-83CE-07DE43CA77F8}"/>
+    <hyperlink ref="D253" r:id="rId209" xr:uid="{5A018FFC-E064-B841-B16C-1B5FDB1C2373}"/>
+    <hyperlink ref="D254" r:id="rId210" xr:uid="{9ECC5CD3-0C49-6241-9ADA-4B8F147F222D}"/>
+    <hyperlink ref="D251" r:id="rId211" xr:uid="{033BB178-31A9-3E47-B7EC-D294053A56E7}"/>
+    <hyperlink ref="D252" r:id="rId212" xr:uid="{5F8349BB-359A-7949-9708-480CAB866631}"/>
+    <hyperlink ref="D255" r:id="rId213" xr:uid="{79509633-6320-7F4C-8E22-C5B4BAEC20D7}"/>
+    <hyperlink ref="D256" r:id="rId214" xr:uid="{A70D9607-0490-DF4E-85B3-794BEB0DB3CD}"/>
+    <hyperlink ref="D257" r:id="rId215" xr:uid="{7F93E30A-E771-E541-A3E8-E8E115BAC442}"/>
+    <hyperlink ref="D258" r:id="rId216" xr:uid="{DF50B5D9-DAAC-7043-8DA2-3DBF2FCB4882}"/>
+    <hyperlink ref="D260" r:id="rId217" xr:uid="{88721544-7A83-0045-B6A7-188448608657}"/>
+    <hyperlink ref="D259" r:id="rId218" xr:uid="{83108E31-6FB4-974C-8A81-89A0D5728752}"/>
+    <hyperlink ref="D241" r:id="rId219" xr:uid="{2930C349-E6B7-544B-BB2A-773A46E73BCB}"/>
+    <hyperlink ref="D225" r:id="rId220" xr:uid="{2BE70040-B75E-144F-8CF2-C6FAF265243F}"/>
+    <hyperlink ref="D261" r:id="rId221" xr:uid="{69A55749-D9D2-1B4B-B3F9-4B160F762593}"/>
+    <hyperlink ref="D262" r:id="rId222" xr:uid="{FB9E4799-0707-754B-9240-DFB8EFCF3420}"/>
+    <hyperlink ref="D263" r:id="rId223" xr:uid="{EFA9A5C9-A935-FD44-A8C3-75A6D42D9D41}"/>
     <hyperlink ref="D74" r:id="rId224" xr:uid="{18AB1C94-4CE1-2945-92C4-F9826FBC6B4E}"/>
-    <hyperlink ref="D261" r:id="rId225" xr:uid="{C4F6B18C-5177-2443-BF86-A034E4709B73}"/>
-    <hyperlink ref="D262" r:id="rId226" xr:uid="{6CB68E90-F81E-C748-8D45-EFEEC50C2AE3}"/>
-    <hyperlink ref="D263" r:id="rId227" xr:uid="{8303BB33-5888-964E-8CF2-43DD162804AD}"/>
-    <hyperlink ref="D264" r:id="rId228" xr:uid="{6C92D97F-0A5E-394B-ABB8-0A48B9DDE3CE}"/>
-    <hyperlink ref="D265" r:id="rId229" xr:uid="{CA84B07B-1C9B-6945-B5E7-3EE8BD697B35}"/>
-    <hyperlink ref="D266" r:id="rId230" xr:uid="{A23CD4FA-5C90-8B4F-B42D-8F0581378838}"/>
-    <hyperlink ref="D267" r:id="rId231" xr:uid="{A75CA764-6259-D247-9F3E-71FE84093EEF}"/>
-    <hyperlink ref="D268" r:id="rId232" xr:uid="{3A294A0B-01BA-BC47-AEB6-53CB0BE2CF1D}"/>
-    <hyperlink ref="D269" r:id="rId233" xr:uid="{4FCB99F2-3FFA-D440-B956-CC2FD50BB76F}"/>
-    <hyperlink ref="D270" r:id="rId234" xr:uid="{936BB4A4-64DC-4640-8D60-262FEB18B51D}"/>
-    <hyperlink ref="D271" r:id="rId235" xr:uid="{09EB0BAC-80EB-3346-AF8B-932BAB3F6F52}"/>
-    <hyperlink ref="D272" r:id="rId236" xr:uid="{6A769F3D-26AD-7246-B490-BEE25DBAD44F}"/>
-    <hyperlink ref="D273" r:id="rId237" xr:uid="{09E5227C-BF06-3C4D-A347-5ACB9A39218F}"/>
-    <hyperlink ref="D274" r:id="rId238" xr:uid="{249C8010-6579-F842-931C-5A1AA5FFD47E}"/>
-    <hyperlink ref="D275" r:id="rId239" xr:uid="{C11D7F08-A472-D74F-ACD4-DC39321AAA3B}"/>
-    <hyperlink ref="D276" r:id="rId240" xr:uid="{EF696095-531A-9B4E-90F5-CA1166C070EB}"/>
-    <hyperlink ref="D277" r:id="rId241" xr:uid="{7319E358-38E8-6D4F-99E9-A558FF1C66D0}"/>
-    <hyperlink ref="D278" r:id="rId242" xr:uid="{C569513C-F920-6148-BB18-A2830C6CABED}"/>
-    <hyperlink ref="D280" r:id="rId243" xr:uid="{5AE9E7D0-FF0D-6442-87DE-FA61A897B3CE}"/>
-    <hyperlink ref="D281" r:id="rId244" xr:uid="{4DDCE0DF-C4D6-2F48-850A-FFE8E44529B8}"/>
-    <hyperlink ref="D283" r:id="rId245" xr:uid="{54E4386C-E9E6-5947-8BDF-3BBD841882D1}"/>
-    <hyperlink ref="D284" r:id="rId246" xr:uid="{81F19F2E-83E8-4F41-A52E-63787010CAAE}"/>
-    <hyperlink ref="D285" r:id="rId247" xr:uid="{E0DAEF11-F444-344B-922F-A5AFA19CBDAC}"/>
-    <hyperlink ref="D286" r:id="rId248" xr:uid="{9FD33CD5-F342-BC42-A6B7-5CD2049D8920}"/>
-    <hyperlink ref="D279" r:id="rId249" xr:uid="{9E36AED5-0E4B-A447-9436-6F32633D1396}"/>
-    <hyperlink ref="D287" r:id="rId250" xr:uid="{0288DF9D-25CD-1C4B-A841-A046246E02C3}"/>
-    <hyperlink ref="D288" r:id="rId251" xr:uid="{C9DFAC71-5ACF-204D-8F9A-D4FBACBEA7AA}"/>
+    <hyperlink ref="D264" r:id="rId225" xr:uid="{C4F6B18C-5177-2443-BF86-A034E4709B73}"/>
+    <hyperlink ref="D265" r:id="rId226" xr:uid="{6CB68E90-F81E-C748-8D45-EFEEC50C2AE3}"/>
+    <hyperlink ref="D266" r:id="rId227" xr:uid="{8303BB33-5888-964E-8CF2-43DD162804AD}"/>
+    <hyperlink ref="D267" r:id="rId228" xr:uid="{6C92D97F-0A5E-394B-ABB8-0A48B9DDE3CE}"/>
+    <hyperlink ref="D268" r:id="rId229" xr:uid="{CA84B07B-1C9B-6945-B5E7-3EE8BD697B35}"/>
+    <hyperlink ref="D269" r:id="rId230" xr:uid="{A23CD4FA-5C90-8B4F-B42D-8F0581378838}"/>
+    <hyperlink ref="D270" r:id="rId231" xr:uid="{A75CA764-6259-D247-9F3E-71FE84093EEF}"/>
+    <hyperlink ref="D271" r:id="rId232" xr:uid="{3A294A0B-01BA-BC47-AEB6-53CB0BE2CF1D}"/>
+    <hyperlink ref="D272" r:id="rId233" xr:uid="{4FCB99F2-3FFA-D440-B956-CC2FD50BB76F}"/>
+    <hyperlink ref="D273" r:id="rId234" xr:uid="{936BB4A4-64DC-4640-8D60-262FEB18B51D}"/>
+    <hyperlink ref="D274" r:id="rId235" xr:uid="{09EB0BAC-80EB-3346-AF8B-932BAB3F6F52}"/>
+    <hyperlink ref="D275" r:id="rId236" xr:uid="{6A769F3D-26AD-7246-B490-BEE25DBAD44F}"/>
+    <hyperlink ref="D276" r:id="rId237" xr:uid="{09E5227C-BF06-3C4D-A347-5ACB9A39218F}"/>
+    <hyperlink ref="D277" r:id="rId238" xr:uid="{249C8010-6579-F842-931C-5A1AA5FFD47E}"/>
+    <hyperlink ref="D278" r:id="rId239" xr:uid="{C11D7F08-A472-D74F-ACD4-DC39321AAA3B}"/>
+    <hyperlink ref="D279" r:id="rId240" xr:uid="{EF696095-531A-9B4E-90F5-CA1166C070EB}"/>
+    <hyperlink ref="D280" r:id="rId241" xr:uid="{7319E358-38E8-6D4F-99E9-A558FF1C66D0}"/>
+    <hyperlink ref="D281" r:id="rId242" xr:uid="{C569513C-F920-6148-BB18-A2830C6CABED}"/>
+    <hyperlink ref="D283" r:id="rId243" xr:uid="{5AE9E7D0-FF0D-6442-87DE-FA61A897B3CE}"/>
+    <hyperlink ref="D284" r:id="rId244" xr:uid="{4DDCE0DF-C4D6-2F48-850A-FFE8E44529B8}"/>
+    <hyperlink ref="D286" r:id="rId245" xr:uid="{54E4386C-E9E6-5947-8BDF-3BBD841882D1}"/>
+    <hyperlink ref="D287" r:id="rId246" xr:uid="{81F19F2E-83E8-4F41-A52E-63787010CAAE}"/>
+    <hyperlink ref="D288" r:id="rId247" xr:uid="{E0DAEF11-F444-344B-922F-A5AFA19CBDAC}"/>
+    <hyperlink ref="D289" r:id="rId248" xr:uid="{9FD33CD5-F342-BC42-A6B7-5CD2049D8920}"/>
+    <hyperlink ref="D282" r:id="rId249" xr:uid="{9E36AED5-0E4B-A447-9436-6F32633D1396}"/>
+    <hyperlink ref="D290" r:id="rId250" xr:uid="{0288DF9D-25CD-1C4B-A841-A046246E02C3}"/>
+    <hyperlink ref="D291" r:id="rId251" xr:uid="{C9DFAC71-5ACF-204D-8F9A-D4FBACBEA7AA}"/>
+    <hyperlink ref="D100" r:id="rId252" xr:uid="{B4CEFF9C-4149-C147-9750-CA2940A29B5D}"/>
+    <hyperlink ref="D101" r:id="rId253" location="sthash.CLyG4oHQ.dpbs" xr:uid="{785D69EA-E77B-AF48-85EB-249509A6BB77}"/>
+    <hyperlink ref="D79" r:id="rId254" xr:uid="{60A19DED-9CDC-124A-9E44-AA37FD1C44F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New spreadsheet from Ken, dated 7/8/2021.
</commit_message>
<xml_diff>
--- a/xlsx/timeline_links.xlsx
+++ b/xlsx/timeline_links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6D8E45-39ED-4A3A-A9D1-8558AC25E53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75A4679-11F5-4A57-94F8-0EDC11638C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="438">
   <si>
     <t>https://www.bostonmpo.org/node/3251</t>
   </si>
@@ -1278,9 +1278,6 @@
     <t>Congestion Management Process</t>
   </si>
   <si>
-    <t>Coordinated Public Transit–Human Services Transportation Plan</t>
-  </si>
-  <si>
     <t>https://www.bostonmpo.org/cpt-hst</t>
   </si>
   <si>
@@ -1333,6 +1330,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Central Artery</t>
+  </si>
+  <si>
+    <t>A Branch</t>
+  </si>
+  <si>
+    <t>http://www.bostonstreetcars.com/what-happened-to-the-a-line.html</t>
+  </si>
+  <si>
+    <t>Coordinated Public Transit-Human Services Transportation Plan</t>
   </si>
 </sst>
 </file>
@@ -1750,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
-  <dimension ref="A1:E320"/>
+  <dimension ref="A1:E321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2418,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>20</v>
@@ -2786,7 +2792,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>1888</v>
+        <v>1845</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>20</v>
@@ -2826,10 +2832,10 @@
         <v>20</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>435</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>139</v>
+        <v>436</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>65</v>
@@ -2843,10 +2849,10 @@
         <v>20</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>65</v>
@@ -2854,16 +2860,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>1894</v>
+        <v>1889</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>65</v>
@@ -2877,10 +2883,10 @@
         <v>20</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>65</v>
@@ -2894,10 +2900,10 @@
         <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>62</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>63</v>
+        <v>147</v>
+      </c>
+      <c r="D67" t="s">
+        <v>61</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>65</v>
@@ -2905,16 +2911,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>1898</v>
+        <v>1894</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>65</v>
@@ -2922,16 +2928,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1897</v>
+        <v>1898</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>65</v>
@@ -2945,10 +2951,10 @@
         <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>65</v>
@@ -2962,10 +2968,10 @@
         <v>20</v>
       </c>
       <c r="C71" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>65</v>
@@ -2979,10 +2985,10 @@
         <v>20</v>
       </c>
       <c r="C72" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>65</v>
@@ -2996,10 +3002,10 @@
         <v>20</v>
       </c>
       <c r="C73" t="s">
-        <v>376</v>
+        <v>115</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>65</v>
@@ -3013,10 +3019,10 @@
         <v>20</v>
       </c>
       <c r="C74" t="s">
-        <v>92</v>
+        <v>376</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>65</v>
@@ -3024,16 +3030,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>65</v>
@@ -3047,10 +3053,10 @@
         <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>65</v>
@@ -3064,10 +3070,10 @@
         <v>20</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>65</v>
@@ -3081,10 +3087,10 @@
         <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>376</v>
+        <v>89</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>65</v>
@@ -3098,10 +3104,10 @@
         <v>20</v>
       </c>
       <c r="C79" t="s">
-        <v>92</v>
+        <v>376</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>65</v>
@@ -3109,16 +3115,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C80" t="s">
-        <v>318</v>
+        <v>92</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>319</v>
+        <v>57</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>65</v>
@@ -3132,10 +3138,10 @@
         <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>94</v>
+        <v>318</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>93</v>
+        <v>319</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>65</v>
@@ -3143,16 +3149,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C82" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>65</v>
@@ -3166,10 +3172,10 @@
         <v>20</v>
       </c>
       <c r="C83" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>65</v>
@@ -3180,13 +3186,13 @@
         <v>1901</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C84" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>65</v>
@@ -3197,13 +3203,13 @@
         <v>1901</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>382</v>
+        <v>96</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>381</v>
+        <v>97</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>65</v>
@@ -3217,10 +3223,10 @@
         <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>118</v>
+        <v>382</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>119</v>
+        <v>381</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>65</v>
@@ -3234,10 +3240,10 @@
         <v>20</v>
       </c>
       <c r="C87" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>65</v>
@@ -3245,16 +3251,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C88" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>65</v>
@@ -3262,16 +3268,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C89" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>65</v>
@@ -3279,16 +3285,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>1909</v>
+        <v>1861</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C90" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>65</v>
@@ -3302,10 +3308,10 @@
         <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>112</v>
-      </c>
-      <c r="D91" t="s">
-        <v>95</v>
+        <v>100</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>65</v>
@@ -3313,16 +3319,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>1912</v>
+        <v>1909</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
+      </c>
+      <c r="D92" t="s">
+        <v>95</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>65</v>
@@ -3336,10 +3342,10 @@
         <v>20</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>65</v>
@@ -3353,10 +3359,10 @@
         <v>20</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>65</v>
@@ -3370,10 +3376,10 @@
         <v>20</v>
       </c>
       <c r="C95" t="s">
-        <v>109</v>
-      </c>
-      <c r="D95" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>65</v>
@@ -3381,16 +3387,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C96" t="s">
-        <v>98</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>99</v>
+        <v>109</v>
+      </c>
+      <c r="D96" t="s">
+        <v>108</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>65</v>
@@ -3398,16 +3404,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>65</v>
@@ -3415,16 +3421,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C98" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>65</v>
@@ -3432,16 +3438,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C99" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>65</v>
@@ -3449,7 +3455,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>20</v>
@@ -3466,16 +3472,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C101" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>65</v>
@@ -3489,10 +3495,10 @@
         <v>20</v>
       </c>
       <c r="C102" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>65</v>
@@ -3506,10 +3512,10 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>112</v>
-      </c>
-      <c r="D103" t="s">
-        <v>95</v>
+        <v>120</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>65</v>
@@ -3523,10 +3529,10 @@
         <v>20</v>
       </c>
       <c r="C104" t="s">
-        <v>378</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>377</v>
+        <v>112</v>
+      </c>
+      <c r="D104" t="s">
+        <v>95</v>
       </c>
       <c r="E104" s="10" t="s">
         <v>65</v>
@@ -3540,10 +3546,10 @@
         <v>20</v>
       </c>
       <c r="C105" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E105" s="10" t="s">
         <v>65</v>
@@ -3557,10 +3563,10 @@
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>110</v>
+        <v>379</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>111</v>
+        <v>380</v>
       </c>
       <c r="E106" s="10" t="s">
         <v>65</v>
@@ -3568,16 +3574,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>1923</v>
+        <v>1919</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C107" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E107" s="10" t="s">
         <v>65</v>
@@ -3585,16 +3591,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>1927</v>
+        <v>1923</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C108" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E108" s="10" t="s">
         <v>65</v>
@@ -3602,7 +3608,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>20</v>
@@ -3619,7 +3625,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>20</v>
@@ -3642,10 +3648,10 @@
         <v>20</v>
       </c>
       <c r="C111" t="s">
-        <v>124</v>
-      </c>
-      <c r="D111" t="s">
-        <v>123</v>
+        <v>106</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="E111" s="10" t="s">
         <v>65</v>
@@ -3653,16 +3659,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>1934</v>
+        <v>1929</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C112" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D112" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E112" s="10" t="s">
         <v>65</v>
@@ -3670,19 +3676,19 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>129</v>
       </c>
       <c r="D113" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
       <c r="E113" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3693,10 +3699,10 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>28</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="D114" t="s">
+        <v>10</v>
       </c>
       <c r="E114" s="10" t="s">
         <v>64</v>
@@ -3710,10 +3716,10 @@
         <v>4</v>
       </c>
       <c r="C115" t="s">
-        <v>29</v>
-      </c>
-      <c r="D115" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>64</v>
@@ -3727,10 +3733,10 @@
         <v>4</v>
       </c>
       <c r="C116" t="s">
-        <v>390</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>389</v>
+        <v>29</v>
+      </c>
+      <c r="D116" t="s">
+        <v>12</v>
       </c>
       <c r="E116" s="10" t="s">
         <v>64</v>
@@ -3741,13 +3747,13 @@
         <v>1935</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>8</v>
+        <v>390</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>9</v>
+        <v>389</v>
       </c>
       <c r="E117" s="10" t="s">
         <v>64</v>
@@ -3755,19 +3761,19 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>126</v>
-      </c>
-      <c r="D118" t="s">
-        <v>125</v>
+        <v>8</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3778,10 +3784,10 @@
         <v>20</v>
       </c>
       <c r="C119" t="s">
-        <v>127</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+      <c r="D119" t="s">
+        <v>125</v>
       </c>
       <c r="E119" s="10" t="s">
         <v>65</v>
@@ -3789,16 +3795,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C120" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E120" s="10" t="s">
         <v>65</v>
@@ -3812,10 +3818,10 @@
         <v>20</v>
       </c>
       <c r="C121" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>65</v>
@@ -3829,10 +3835,10 @@
         <v>20</v>
       </c>
       <c r="C122" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="E122" s="10" t="s">
         <v>65</v>
@@ -3846,10 +3852,10 @@
         <v>20</v>
       </c>
       <c r="C123" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="E123" s="10" t="s">
         <v>65</v>
@@ -3857,16 +3863,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C124" t="s">
-        <v>131</v>
-      </c>
-      <c r="D124" t="s">
-        <v>132</v>
+        <v>137</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="E124" s="10" t="s">
         <v>65</v>
@@ -3874,16 +3880,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>1950</v>
+        <v>1943</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C125" t="s">
-        <v>143</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
+      </c>
+      <c r="D125" t="s">
+        <v>132</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>65</v>
@@ -3897,10 +3903,10 @@
         <v>20</v>
       </c>
       <c r="C126" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E126" s="10" t="s">
         <v>65</v>
@@ -3908,16 +3914,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C127" t="s">
-        <v>402</v>
+        <v>145</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>401</v>
+        <v>146</v>
       </c>
       <c r="E127" s="10" t="s">
         <v>65</v>
@@ -3931,13 +3937,13 @@
         <v>20</v>
       </c>
       <c r="C128" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3945,13 +3951,13 @@
         <v>1951</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C129" t="s">
-        <v>148</v>
+        <v>404</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>149</v>
+        <v>403</v>
       </c>
       <c r="E129" s="10" t="s">
         <v>64</v>
@@ -3965,10 +3971,10 @@
         <v>4</v>
       </c>
       <c r="C130" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>64</v>
@@ -3982,10 +3988,10 @@
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E131" s="10" t="s">
         <v>64</v>
@@ -3999,10 +4005,10 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E132" s="10" t="s">
         <v>64</v>
@@ -4016,10 +4022,10 @@
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>64</v>
@@ -4033,10 +4039,10 @@
         <v>4</v>
       </c>
       <c r="C134" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E134" s="10" t="s">
         <v>64</v>
@@ -4050,10 +4056,10 @@
         <v>4</v>
       </c>
       <c r="C135" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E135" s="10" t="s">
         <v>64</v>
@@ -4067,10 +4073,10 @@
         <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E136" s="10" t="s">
         <v>64</v>
@@ -4084,10 +4090,10 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E137" s="10" t="s">
         <v>64</v>
@@ -4095,16 +4101,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>27</v>
-      </c>
-      <c r="D138" t="s">
-        <v>10</v>
+        <v>164</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="E138" s="10" t="s">
         <v>64</v>
@@ -4118,10 +4124,10 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>28</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="D139" t="s">
+        <v>10</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>64</v>
@@ -4135,10 +4141,10 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>29</v>
-      </c>
-      <c r="D140" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E140" s="10" t="s">
         <v>64</v>
@@ -4152,10 +4158,10 @@
         <v>4</v>
       </c>
       <c r="C141" t="s">
-        <v>390</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>389</v>
+        <v>29</v>
+      </c>
+      <c r="D141" t="s">
+        <v>12</v>
       </c>
       <c r="E141" s="10" t="s">
         <v>64</v>
@@ -4163,16 +4169,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>27</v>
-      </c>
-      <c r="D142" t="s">
-        <v>10</v>
+        <v>390</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>389</v>
       </c>
       <c r="E142" s="10" t="s">
         <v>64</v>
@@ -4186,10 +4192,10 @@
         <v>4</v>
       </c>
       <c r="C143" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="D143" t="s">
+        <v>10</v>
       </c>
       <c r="E143" s="10" t="s">
         <v>64</v>
@@ -4203,10 +4209,10 @@
         <v>4</v>
       </c>
       <c r="C144" t="s">
-        <v>29</v>
-      </c>
-      <c r="D144" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E144" s="10" t="s">
         <v>64</v>
@@ -4220,10 +4226,10 @@
         <v>4</v>
       </c>
       <c r="C145" t="s">
-        <v>390</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>389</v>
+        <v>29</v>
+      </c>
+      <c r="D145" t="s">
+        <v>12</v>
       </c>
       <c r="E145" s="10" t="s">
         <v>64</v>
@@ -4231,33 +4237,33 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>1957</v>
+        <v>1953</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C146" t="s">
-        <v>167</v>
+        <v>390</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>166</v>
+        <v>389</v>
       </c>
       <c r="E146" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>1952</v>
+        <v>1957</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C147" t="s">
-        <v>60</v>
+        <v>167</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>59</v>
+        <v>166</v>
       </c>
       <c r="E147" s="10" t="s">
         <v>65</v>
@@ -4268,16 +4274,16 @@
         <v>1952</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C148" t="s">
-        <v>407</v>
+        <v>60</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>406</v>
+        <v>59</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4288,10 +4294,10 @@
         <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E149" s="10" t="s">
         <v>64</v>
@@ -4299,16 +4305,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>1957</v>
+        <v>1952</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C150" t="s">
-        <v>174</v>
+        <v>408</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>175</v>
+        <v>405</v>
       </c>
       <c r="E150" s="10" t="s">
         <v>64</v>
@@ -4316,36 +4322,36 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>1952</v>
+        <v>1957</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="E151" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C152" t="s">
-        <v>27</v>
-      </c>
-      <c r="D152" t="s">
-        <v>10</v>
+        <v>102</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="E152" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4356,10 +4362,10 @@
         <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>28</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="D153" t="s">
+        <v>10</v>
       </c>
       <c r="E153" s="10" t="s">
         <v>64</v>
@@ -4373,10 +4379,10 @@
         <v>4</v>
       </c>
       <c r="C154" t="s">
-        <v>29</v>
-      </c>
-      <c r="D154" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E154" s="10" t="s">
         <v>64</v>
@@ -4390,10 +4396,10 @@
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>390</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>389</v>
+        <v>29</v>
+      </c>
+      <c r="D155" t="s">
+        <v>12</v>
       </c>
       <c r="E155" s="10" t="s">
         <v>64</v>
@@ -4401,19 +4407,19 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>431</v>
+        <v>390</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>430</v>
+        <v>389</v>
       </c>
       <c r="E156" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4424,10 +4430,10 @@
         <v>20</v>
       </c>
       <c r="C157" t="s">
-        <v>102</v>
+        <v>430</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>103</v>
+        <v>429</v>
       </c>
       <c r="E157" s="10" t="s">
         <v>65</v>
@@ -4438,16 +4444,16 @@
         <v>1954</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C158" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>177</v>
+        <v>103</v>
       </c>
       <c r="E158" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4458,10 +4464,10 @@
         <v>4</v>
       </c>
       <c r="C159" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>64</v>
@@ -4475,10 +4481,10 @@
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>64</v>
@@ -4486,16 +4492,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C161" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E161" s="10" t="s">
         <v>64</v>
@@ -4509,10 +4515,10 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>64</v>
@@ -4523,16 +4529,16 @@
         <v>1955</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C163" t="s">
-        <v>431</v>
+        <v>178</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>430</v>
+        <v>179</v>
       </c>
       <c r="E163" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4540,30 +4546,30 @@
         <v>1955</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C164" t="s">
-        <v>180</v>
+        <v>430</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>181</v>
+        <v>429</v>
       </c>
       <c r="E164" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>1953</v>
+        <v>1955</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C165" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E165" s="10" t="s">
         <v>64</v>
@@ -4571,36 +4577,36 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C166" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E166" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C167" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="E167" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4611,10 +4617,10 @@
         <v>4</v>
       </c>
       <c r="C168" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E168" s="10" t="s">
         <v>64</v>
@@ -4628,10 +4634,10 @@
         <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E169" s="10" t="s">
         <v>64</v>
@@ -4645,10 +4651,10 @@
         <v>4</v>
       </c>
       <c r="C170" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E170" s="10" t="s">
         <v>64</v>
@@ -4662,10 +4668,10 @@
         <v>4</v>
       </c>
       <c r="C171" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E171" s="10" t="s">
         <v>64</v>
@@ -4673,16 +4679,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E172" s="10" t="s">
         <v>64</v>
@@ -4696,10 +4702,10 @@
         <v>4</v>
       </c>
       <c r="C173" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>64</v>
@@ -4713,10 +4719,10 @@
         <v>4</v>
       </c>
       <c r="C174" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E174" s="10" t="s">
         <v>64</v>
@@ -4730,10 +4736,10 @@
         <v>4</v>
       </c>
       <c r="C175" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E175" s="10" t="s">
         <v>64</v>
@@ -4747,47 +4753,47 @@
         <v>4</v>
       </c>
       <c r="C176" t="s">
+        <v>196</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E176" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>1958</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C177" t="s">
         <v>198</v>
       </c>
-      <c r="D176" s="3" t="s">
+      <c r="D177" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E176" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="7">
+      <c r="E177" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="7">
         <v>1958</v>
       </c>
-      <c r="B177" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C177" s="2" t="s">
+      <c r="B178" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C178" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D177" s="8" t="s">
+      <c r="D178" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E177" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
-        <v>1959</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C178" t="s">
-        <v>200</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E178" s="10" t="s">
-        <v>64</v>
+      <c r="E178" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4798,10 +4804,10 @@
         <v>4</v>
       </c>
       <c r="C179" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="E179" s="10" t="s">
         <v>64</v>
@@ -4815,10 +4821,10 @@
         <v>4</v>
       </c>
       <c r="C180" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E180" s="10" t="s">
         <v>64</v>
@@ -4832,10 +4838,10 @@
         <v>4</v>
       </c>
       <c r="C181" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="E181" s="10" t="s">
         <v>64</v>
@@ -4849,10 +4855,10 @@
         <v>4</v>
       </c>
       <c r="C182" t="s">
-        <v>366</v>
+        <v>202</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E182" s="10" t="s">
         <v>64</v>
@@ -4866,10 +4872,10 @@
         <v>4</v>
       </c>
       <c r="C183" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E183" s="10" t="s">
         <v>64</v>
@@ -4883,10 +4889,10 @@
         <v>4</v>
       </c>
       <c r="C184" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E184" s="10" t="s">
         <v>64</v>
@@ -4900,10 +4906,10 @@
         <v>4</v>
       </c>
       <c r="C185" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E185" s="10" t="s">
         <v>64</v>
@@ -4917,10 +4923,10 @@
         <v>4</v>
       </c>
       <c r="C186" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E186" s="10" t="s">
         <v>64</v>
@@ -4934,10 +4940,10 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E187" s="10" t="s">
         <v>64</v>
@@ -4951,10 +4957,10 @@
         <v>4</v>
       </c>
       <c r="C188" t="s">
-        <v>210</v>
+        <v>371</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E188" s="10" t="s">
         <v>64</v>
@@ -4968,10 +4974,10 @@
         <v>4</v>
       </c>
       <c r="C189" t="s">
-        <v>372</v>
+        <v>210</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E189" s="10" t="s">
         <v>64</v>
@@ -4985,10 +4991,10 @@
         <v>4</v>
       </c>
       <c r="C190" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E190" s="10" t="s">
         <v>64</v>
@@ -5002,10 +5008,10 @@
         <v>4</v>
       </c>
       <c r="C191" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E191" s="10" t="s">
         <v>64</v>
@@ -5019,10 +5025,10 @@
         <v>4</v>
       </c>
       <c r="C192" t="s">
-        <v>215</v>
+        <v>374</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E192" s="10" t="s">
         <v>64</v>
@@ -5033,16 +5039,16 @@
         <v>1959</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C193" t="s">
-        <v>98</v>
+        <v>215</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E193" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5053,10 +5059,10 @@
         <v>20</v>
       </c>
       <c r="C194" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>41</v>
+        <v>222</v>
       </c>
       <c r="E194" s="10" t="s">
         <v>65</v>
@@ -5070,10 +5076,10 @@
         <v>20</v>
       </c>
       <c r="C195" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E195" s="10" t="s">
         <v>65</v>
@@ -5087,10 +5093,10 @@
         <v>20</v>
       </c>
       <c r="C196" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>223</v>
+        <v>40</v>
       </c>
       <c r="E196" s="10" t="s">
         <v>65</v>
@@ -5098,19 +5104,19 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C197" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E197" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5121,10 +5127,10 @@
         <v>4</v>
       </c>
       <c r="C198" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E198" s="10" t="s">
         <v>64</v>
@@ -5138,10 +5144,10 @@
         <v>4</v>
       </c>
       <c r="C199" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E199" s="10" t="s">
         <v>64</v>
@@ -5152,16 +5158,16 @@
         <v>1961</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C200" s="9" t="s">
-        <v>232</v>
+        <v>4</v>
+      </c>
+      <c r="C200" t="s">
+        <v>229</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E200" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5169,50 +5175,50 @@
         <v>1961</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C201" t="s">
-        <v>233</v>
+        <v>20</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E201" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C202" t="s">
-        <v>433</v>
+        <v>233</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>432</v>
+        <v>234</v>
       </c>
       <c r="E202" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C203" t="s">
-        <v>168</v>
+        <v>432</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>169</v>
+        <v>431</v>
       </c>
       <c r="E203" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5223,10 +5229,10 @@
         <v>4</v>
       </c>
       <c r="C204" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E204" s="10" t="s">
         <v>64</v>
@@ -5240,10 +5246,10 @@
         <v>4</v>
       </c>
       <c r="C205" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
       <c r="E205" s="10" t="s">
         <v>64</v>
@@ -5257,10 +5263,10 @@
         <v>4</v>
       </c>
       <c r="C206" t="s">
-        <v>174</v>
+        <v>236</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>175</v>
+        <v>237</v>
       </c>
       <c r="E206" s="10" t="s">
         <v>64</v>
@@ -5274,10 +5280,10 @@
         <v>4</v>
       </c>
       <c r="C207" t="s">
-        <v>238</v>
+        <v>174</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="E207" s="10" t="s">
         <v>64</v>
@@ -5291,10 +5297,10 @@
         <v>4</v>
       </c>
       <c r="C208" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E208" s="10" t="s">
         <v>64</v>
@@ -5307,11 +5313,11 @@
       <c r="B209" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C209" s="12" t="s">
-        <v>245</v>
+      <c r="C209" t="s">
+        <v>240</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E209" s="10" t="s">
         <v>64</v>
@@ -5322,33 +5328,33 @@
         <v>1964</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C210" t="s">
-        <v>235</v>
+        <v>4</v>
+      </c>
+      <c r="C210" s="12" t="s">
+        <v>245</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>57</v>
+        <v>242</v>
       </c>
       <c r="E210" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C211" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>244</v>
+        <v>57</v>
       </c>
       <c r="E211" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5359,10 +5365,10 @@
         <v>4</v>
       </c>
       <c r="C212" t="s">
-        <v>168</v>
+        <v>243</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>169</v>
+        <v>244</v>
       </c>
       <c r="E212" s="10" t="s">
         <v>64</v>
@@ -5376,10 +5382,10 @@
         <v>4</v>
       </c>
       <c r="C213" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E213" s="10" t="s">
         <v>64</v>
@@ -5393,10 +5399,10 @@
         <v>4</v>
       </c>
       <c r="C214" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E214" s="10" t="s">
         <v>64</v>
@@ -5410,10 +5416,10 @@
         <v>4</v>
       </c>
       <c r="C215" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E215" s="10" t="s">
         <v>64</v>
@@ -5427,10 +5433,10 @@
         <v>4</v>
       </c>
       <c r="C216" t="s">
-        <v>246</v>
+        <v>182</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>247</v>
+        <v>183</v>
       </c>
       <c r="E216" s="10" t="s">
         <v>64</v>
@@ -5444,10 +5450,10 @@
         <v>4</v>
       </c>
       <c r="C217" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="E217" s="10" t="s">
         <v>64</v>
@@ -5455,36 +5461,36 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>1971</v>
+        <v>1965</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C218" t="s">
-        <v>106</v>
+        <v>248</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="E218" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>419</v>
+        <v>20</v>
       </c>
       <c r="C219" t="s">
-        <v>410</v>
+        <v>106</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>409</v>
+        <v>107</v>
       </c>
       <c r="E219" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -5492,13 +5498,13 @@
         <v>1973</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C220" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E220" s="10" t="s">
         <v>64</v>
@@ -5509,13 +5515,13 @@
         <v>1973</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C221" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E221" s="10" t="s">
         <v>64</v>
@@ -5526,13 +5532,13 @@
         <v>1973</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C222" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E222" s="10" t="s">
         <v>64</v>
@@ -5543,13 +5549,13 @@
         <v>1973</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C223" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E223" s="10" t="s">
         <v>64</v>
@@ -5560,13 +5566,13 @@
         <v>1973</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C224" t="s">
-        <v>420</v>
+        <v>437</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E224" s="10" t="s">
         <v>64</v>
@@ -5577,13 +5583,13 @@
         <v>1973</v>
       </c>
       <c r="B225" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C225" t="s">
         <v>419</v>
       </c>
-      <c r="C225" t="s">
-        <v>422</v>
-      </c>
       <c r="D225" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E225" s="10" t="s">
         <v>64</v>
@@ -5594,13 +5600,13 @@
         <v>1973</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C226" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E226" s="10" t="s">
         <v>64</v>
@@ -5611,13 +5617,13 @@
         <v>1973</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C227" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="E227" s="10" t="s">
         <v>64</v>
@@ -5628,13 +5634,13 @@
         <v>1973</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C228" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E228" s="10" t="s">
         <v>64</v>
@@ -5645,13 +5651,13 @@
         <v>1973</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>4</v>
+        <v>418</v>
       </c>
       <c r="C229" t="s">
-        <v>251</v>
+        <v>425</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>252</v>
+        <v>426</v>
       </c>
       <c r="E229" s="10" t="s">
         <v>64</v>
@@ -5665,10 +5671,10 @@
         <v>4</v>
       </c>
       <c r="C230" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E230" s="10" t="s">
         <v>64</v>
@@ -5676,33 +5682,33 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C231" t="s">
-        <v>133</v>
+        <v>253</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="E231" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C232" t="s">
-        <v>255</v>
+        <v>133</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>256</v>
+        <v>134</v>
       </c>
       <c r="E232" s="10" t="s">
         <v>65</v>
@@ -5716,10 +5722,10 @@
         <v>20</v>
       </c>
       <c r="C233" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E233" s="10" t="s">
         <v>65</v>
@@ -5733,10 +5739,10 @@
         <v>20</v>
       </c>
       <c r="C234" t="s">
-        <v>112</v>
-      </c>
-      <c r="D234" t="s">
-        <v>95</v>
+        <v>257</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="E234" s="10" t="s">
         <v>65</v>
@@ -5744,16 +5750,16 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C235" t="s">
-        <v>34</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>35</v>
+        <v>112</v>
+      </c>
+      <c r="D235" t="s">
+        <v>95</v>
       </c>
       <c r="E235" s="10" t="s">
         <v>65</v>
@@ -5761,16 +5767,16 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>1965</v>
+        <v>1976</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C236" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="E236" s="10" t="s">
         <v>65</v>
@@ -5778,16 +5784,16 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>1979</v>
+        <v>1965</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C237" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="E237" s="10" t="s">
         <v>65</v>
@@ -5795,7 +5801,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>20</v>
@@ -5812,16 +5818,16 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>1977</v>
+        <v>1980</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C239" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="E239" s="10" t="s">
         <v>65</v>
@@ -5829,16 +5835,16 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>1984</v>
+        <v>1977</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C240" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="E240" s="10" t="s">
         <v>65</v>
@@ -5846,7 +5852,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>20</v>
@@ -5869,30 +5875,30 @@
         <v>20</v>
       </c>
       <c r="C242" t="s">
-        <v>249</v>
+        <v>106</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>250</v>
+        <v>107</v>
       </c>
       <c r="E242" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C243" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="E243" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -5903,10 +5909,10 @@
         <v>20</v>
       </c>
       <c r="C244" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E244" s="10" t="s">
         <v>65</v>
@@ -5920,10 +5926,10 @@
         <v>20</v>
       </c>
       <c r="C245" t="s">
-        <v>112</v>
-      </c>
-      <c r="D245" t="s">
-        <v>95</v>
+        <v>266</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="E245" s="10" t="s">
         <v>65</v>
@@ -5937,10 +5943,10 @@
         <v>20</v>
       </c>
       <c r="C246" t="s">
-        <v>100</v>
-      </c>
-      <c r="D246" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
+      </c>
+      <c r="D246" t="s">
+        <v>95</v>
       </c>
       <c r="E246" s="10" t="s">
         <v>65</v>
@@ -5954,10 +5960,10 @@
         <v>20</v>
       </c>
       <c r="C247" t="s">
-        <v>261</v>
+        <v>100</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>262</v>
+        <v>101</v>
       </c>
       <c r="E247" s="10" t="s">
         <v>65</v>
@@ -5971,10 +5977,10 @@
         <v>20</v>
       </c>
       <c r="C248" t="s">
-        <v>77</v>
+        <v>261</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>76</v>
+        <v>262</v>
       </c>
       <c r="E248" s="10" t="s">
         <v>65</v>
@@ -5985,16 +5991,16 @@
         <v>1987</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C249" t="s">
-        <v>274</v>
+        <v>77</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>273</v>
+        <v>76</v>
       </c>
       <c r="E249" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6002,30 +6008,30 @@
         <v>1987</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C250" t="s">
-        <v>77</v>
+        <v>274</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>76</v>
+        <v>273</v>
       </c>
       <c r="E250" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C251" t="s">
-        <v>267</v>
+        <v>77</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>268</v>
+        <v>76</v>
       </c>
       <c r="E251" s="10" t="s">
         <v>65</v>
@@ -6039,10 +6045,10 @@
         <v>20</v>
       </c>
       <c r="C252" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E252" s="10" t="s">
         <v>65</v>
@@ -6053,13 +6059,13 @@
         <v>1992</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C253" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E253" s="10" t="s">
         <v>65</v>
@@ -6067,53 +6073,53 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C254" t="s">
+        <v>272</v>
+      </c>
+      <c r="D254" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E254" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
         <v>1993</v>
       </c>
-      <c r="B254" s="1" t="s">
+      <c r="B255" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C255" t="s">
         <v>276</v>
       </c>
-      <c r="D254" s="3" t="s">
+      <c r="D255" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="E254" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A255" s="7">
+      <c r="E255" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="7">
         <v>1993</v>
       </c>
-      <c r="B255" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C255" s="2" t="s">
+      <c r="B256" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C256" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D255" s="3" t="s">
+      <c r="D256" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E255" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A256" s="1">
-        <v>1993</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C256" t="s">
-        <v>278</v>
-      </c>
-      <c r="D256" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="E256" s="10" t="s">
-        <v>64</v>
+      <c r="E256" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6121,13 +6127,13 @@
         <v>1993</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C257" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E257" s="10" t="s">
         <v>64</v>
@@ -6135,33 +6141,33 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>1870</v>
+        <v>1993</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="C258" t="s">
-        <v>82</v>
+        <v>279</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>81</v>
+        <v>280</v>
       </c>
       <c r="E258" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>1994</v>
+        <v>1870</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C259" t="s">
-        <v>435</v>
+        <v>82</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>434</v>
+        <v>81</v>
       </c>
       <c r="E259" s="10" t="s">
         <v>65</v>
@@ -6175,10 +6181,10 @@
         <v>20</v>
       </c>
       <c r="C260" t="s">
-        <v>281</v>
+        <v>434</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>282</v>
+        <v>433</v>
       </c>
       <c r="E260" s="10" t="s">
         <v>65</v>
@@ -6189,16 +6195,16 @@
         <v>1994</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C261" t="s">
-        <v>372</v>
+        <v>281</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>212</v>
+        <v>282</v>
       </c>
       <c r="E261" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6209,10 +6215,10 @@
         <v>4</v>
       </c>
       <c r="C262" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E262" s="10" t="s">
         <v>64</v>
@@ -6226,10 +6232,10 @@
         <v>4</v>
       </c>
       <c r="C263" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E263" s="10" t="s">
         <v>64</v>
@@ -6237,33 +6243,33 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>1955</v>
+        <v>1994</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C264" t="s">
-        <v>431</v>
+        <v>374</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>430</v>
+        <v>214</v>
       </c>
       <c r="E264" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C265" t="s">
-        <v>290</v>
+        <v>430</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>289</v>
+        <v>429</v>
       </c>
       <c r="E265" s="10" t="s">
         <v>65</v>
@@ -6274,16 +6280,16 @@
         <v>1995</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C266" t="s">
-        <v>368</v>
+        <v>290</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>206</v>
+        <v>289</v>
       </c>
       <c r="E266" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6294,10 +6300,10 @@
         <v>4</v>
       </c>
       <c r="C267" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E267" s="10" t="s">
         <v>64</v>
@@ -6311,10 +6317,10 @@
         <v>4</v>
       </c>
       <c r="C268" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E268" s="10" t="s">
         <v>64</v>
@@ -6325,49 +6331,49 @@
         <v>1995</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C269" t="s">
+        <v>372</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E269" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C270" t="s">
         <v>292</v>
       </c>
-      <c r="D269" s="3" t="s">
+      <c r="D270" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E269" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A270" s="7">
+      <c r="E270" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="7">
         <v>1995</v>
       </c>
-      <c r="B270" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C270" s="2" t="s">
+      <c r="B271" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C271" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D270" s="3" t="s">
+      <c r="D271" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E270" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
-        <v>1995</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C271" t="s">
-        <v>284</v>
-      </c>
-      <c r="D271" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E271" s="10" t="s">
+      <c r="E271" s="11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6379,10 +6385,10 @@
         <v>20</v>
       </c>
       <c r="C272" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E272" s="10" t="s">
         <v>65</v>
@@ -6390,16 +6396,16 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C273" t="s">
-        <v>38</v>
+        <v>285</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="E273" s="10" t="s">
         <v>65</v>
@@ -6407,16 +6413,16 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C274" t="s">
-        <v>293</v>
+        <v>38</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>294</v>
+        <v>40</v>
       </c>
       <c r="E274" s="10" t="s">
         <v>65</v>
@@ -6427,13 +6433,13 @@
         <v>1998</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>295</v>
+        <v>20</v>
       </c>
       <c r="C275" t="s">
-        <v>297</v>
-      </c>
-      <c r="D275" t="s">
-        <v>296</v>
+        <v>293</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="E275" s="10" t="s">
         <v>65</v>
@@ -6444,13 +6450,13 @@
         <v>1998</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>20</v>
+        <v>295</v>
       </c>
       <c r="C276" t="s">
-        <v>39</v>
-      </c>
-      <c r="D276" s="3" t="s">
-        <v>41</v>
+        <v>297</v>
+      </c>
+      <c r="D276" t="s">
+        <v>296</v>
       </c>
       <c r="E276" s="10" t="s">
         <v>65</v>
@@ -6464,10 +6470,10 @@
         <v>20</v>
       </c>
       <c r="C277" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E277" s="10" t="s">
         <v>65</v>
@@ -6475,16 +6481,16 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>2002</v>
+        <v>1998</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C278" t="s">
-        <v>312</v>
+        <v>34</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>311</v>
+        <v>35</v>
       </c>
       <c r="E278" s="10" t="s">
         <v>65</v>
@@ -6498,10 +6504,10 @@
         <v>20</v>
       </c>
       <c r="C279" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E279" s="10" t="s">
         <v>65</v>
@@ -6512,13 +6518,13 @@
         <v>2002</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>302</v>
+        <v>20</v>
       </c>
       <c r="C280" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="E280" s="10" t="s">
         <v>65</v>
@@ -6529,13 +6535,13 @@
         <v>2002</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>20</v>
+        <v>302</v>
       </c>
       <c r="C281" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E281" s="10" t="s">
         <v>65</v>
@@ -6543,16 +6549,16 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C282" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="E282" s="10" t="s">
         <v>65</v>
@@ -6566,10 +6572,10 @@
         <v>20</v>
       </c>
       <c r="C283" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E283" s="10" t="s">
         <v>65</v>
@@ -6583,10 +6589,10 @@
         <v>20</v>
       </c>
       <c r="C284" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="E284" s="10" t="s">
         <v>65</v>
@@ -6600,10 +6606,10 @@
         <v>20</v>
       </c>
       <c r="C285" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E285" s="10" t="s">
         <v>65</v>
@@ -6614,16 +6620,16 @@
         <v>2003</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C286" t="s">
-        <v>200</v>
+        <v>306</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>201</v>
+        <v>308</v>
       </c>
       <c r="E286" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -6634,10 +6640,10 @@
         <v>4</v>
       </c>
       <c r="C287" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="E287" s="10" t="s">
         <v>64</v>
@@ -6651,10 +6657,10 @@
         <v>4</v>
       </c>
       <c r="C288" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E288" s="10" t="s">
         <v>64</v>
@@ -6662,19 +6668,19 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C289" t="s">
-        <v>305</v>
+        <v>178</v>
       </c>
       <c r="D289" s="3" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="E289" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -6685,10 +6691,10 @@
         <v>20</v>
       </c>
       <c r="C290" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E290" s="10" t="s">
         <v>65</v>
@@ -6696,16 +6702,16 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C291" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="D291" s="3" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="E291" s="10" t="s">
         <v>65</v>
@@ -6719,10 +6725,10 @@
         <v>20</v>
       </c>
       <c r="C292" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D292" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="E292" s="10" t="s">
         <v>65</v>
@@ -6736,10 +6742,10 @@
         <v>20</v>
       </c>
       <c r="C293" t="s">
-        <v>62</v>
+        <v>316</v>
       </c>
       <c r="D293" s="3" t="s">
-        <v>63</v>
+        <v>315</v>
       </c>
       <c r="E293" s="10" t="s">
         <v>65</v>
@@ -6753,10 +6759,10 @@
         <v>20</v>
       </c>
       <c r="C294" t="s">
-        <v>317</v>
+        <v>62</v>
       </c>
       <c r="D294" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E294" s="10" t="s">
         <v>65</v>
@@ -6764,16 +6770,16 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C295" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>323</v>
+        <v>61</v>
       </c>
       <c r="E295" s="10" t="s">
         <v>65</v>
@@ -6781,16 +6787,16 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C296" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D296" s="3" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E296" s="10" t="s">
         <v>65</v>
@@ -6804,10 +6810,10 @@
         <v>20</v>
       </c>
       <c r="C297" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D297" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E297" s="10" t="s">
         <v>65</v>
@@ -6818,47 +6824,47 @@
         <v>2007</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C298" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D298" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E298" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>295</v>
+        <v>13</v>
       </c>
       <c r="C299" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D299" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E299" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>20</v>
+        <v>295</v>
       </c>
       <c r="C300" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D300" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E300" s="10" t="s">
         <v>65</v>
@@ -6869,16 +6875,16 @@
         <v>2009</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C301" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D301" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E301" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -6886,16 +6892,16 @@
         <v>2009</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C302" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D302" s="3" t="s">
-        <v>111</v>
+        <v>336</v>
       </c>
       <c r="E302" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -6906,10 +6912,10 @@
         <v>20</v>
       </c>
       <c r="C303" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
       <c r="D303" s="3" t="s">
-        <v>299</v>
+        <v>111</v>
       </c>
       <c r="E303" s="10" t="s">
         <v>65</v>
@@ -6917,16 +6923,16 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C304" t="s">
-        <v>338</v>
+        <v>298</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="E304" s="10" t="s">
         <v>65</v>
@@ -6937,13 +6943,13 @@
         <v>2010</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C305" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D305" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E305" s="10" t="s">
         <v>65</v>
@@ -6951,16 +6957,16 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C306" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D306" s="3" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E306" s="10" t="s">
         <v>65</v>
@@ -6974,10 +6980,10 @@
         <v>20</v>
       </c>
       <c r="C307" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D307" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E307" s="10" t="s">
         <v>65</v>
@@ -6985,16 +6991,16 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C308" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D308" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E308" s="10" t="s">
         <v>65</v>
@@ -7002,16 +7008,16 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C309" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D309" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E309" s="10" t="s">
         <v>65</v>
@@ -7019,16 +7025,16 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C310" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D310" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E310" s="10" t="s">
         <v>65</v>
@@ -7042,10 +7048,10 @@
         <v>20</v>
       </c>
       <c r="C311" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D311" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E311" s="10" t="s">
         <v>65</v>
@@ -7059,10 +7065,10 @@
         <v>20</v>
       </c>
       <c r="C312" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="D312" s="3" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="E312" s="10" t="s">
         <v>65</v>
@@ -7070,16 +7076,16 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C313" t="s">
-        <v>352</v>
-      </c>
-      <c r="D313" t="s">
-        <v>351</v>
+        <v>360</v>
+      </c>
+      <c r="D313" s="3" t="s">
+        <v>359</v>
       </c>
       <c r="E313" s="10" t="s">
         <v>65</v>
@@ -7093,10 +7099,10 @@
         <v>20</v>
       </c>
       <c r="C314" t="s">
-        <v>167</v>
-      </c>
-      <c r="D314" s="3" t="s">
-        <v>166</v>
+        <v>352</v>
+      </c>
+      <c r="D314" t="s">
+        <v>351</v>
       </c>
       <c r="E314" s="10" t="s">
         <v>65</v>
@@ -7104,16 +7110,16 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C315" t="s">
-        <v>353</v>
+        <v>167</v>
       </c>
       <c r="D315" s="3" t="s">
-        <v>354</v>
+        <v>166</v>
       </c>
       <c r="E315" s="10" t="s">
         <v>65</v>
@@ -7121,19 +7127,19 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C316" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="D316" s="3" t="s">
-        <v>336</v>
+        <v>354</v>
       </c>
       <c r="E316" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -7141,16 +7147,16 @@
         <v>2018</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C317" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="E317" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -7161,10 +7167,10 @@
         <v>20</v>
       </c>
       <c r="C318" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D318" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E318" s="10" t="s">
         <v>65</v>
@@ -7172,16 +7178,16 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C319" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D319" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E319" s="10" t="s">
         <v>65</v>
@@ -7189,18 +7195,35 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C320" t="s">
+        <v>361</v>
+      </c>
+      <c r="D320" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E320" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
         <v>2021</v>
       </c>
-      <c r="B320" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C320" t="s">
+      <c r="B321" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C321" t="s">
         <v>364</v>
       </c>
-      <c r="D320" s="3" t="s">
+      <c r="D321" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="E320" s="10" t="s">
+      <c r="E321" s="10" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7227,7 +7250,7 @@
     <hyperlink ref="D60" r:id="rId19" xr:uid="{F597C50B-1112-5646-ADB0-C72EDC488C7D}"/>
     <hyperlink ref="D62" r:id="rId20" xr:uid="{3F62B3B8-D447-954A-8E0B-70BECA5447EE}"/>
     <hyperlink ref="D17" r:id="rId21" xr:uid="{EE3BB206-C0D2-EB4F-AA70-7C0FFFCCBA5F}"/>
-    <hyperlink ref="D67" r:id="rId22" xr:uid="{B0482045-53D9-474D-B70B-423E86B4B9CE}"/>
+    <hyperlink ref="D68" r:id="rId22" xr:uid="{B0482045-53D9-474D-B70B-423E86B4B9CE}"/>
     <hyperlink ref="D19" r:id="rId23" xr:uid="{AE3F6E1A-176D-9149-B043-D776733464AB}"/>
     <hyperlink ref="D6" r:id="rId24" xr:uid="{4FAAA4DD-C614-D942-8C81-16828DF82F2B}"/>
     <hyperlink ref="D14" r:id="rId25" xr:uid="{393F2075-4A9E-0B47-92DA-FF28CD1D6999}"/>
@@ -7236,187 +7259,187 @@
     <hyperlink ref="D56" r:id="rId28" xr:uid="{329EF611-EF9C-FC4A-9988-9666121DABCD}"/>
     <hyperlink ref="D57" r:id="rId29" xr:uid="{09ABDBF1-B54C-604F-A17B-446CBE1A2A2C}"/>
     <hyperlink ref="D59" r:id="rId30" xr:uid="{96D60956-D26C-CC4C-B361-C31419E06692}"/>
-    <hyperlink ref="D69" r:id="rId31" xr:uid="{90EBC071-E84D-4549-A9CE-645045A70E75}"/>
-    <hyperlink ref="D70" r:id="rId32" xr:uid="{E731DF72-6E9F-0240-B2A4-95E82B8C938A}"/>
-    <hyperlink ref="D73" r:id="rId33" xr:uid="{5391EFF3-6DAD-4E40-9C66-C7501F2ABF1B}"/>
-    <hyperlink ref="D74" r:id="rId34" xr:uid="{EBCA5E87-62CD-FD46-9F99-E2FD5D3229F6}"/>
-    <hyperlink ref="D76" r:id="rId35" xr:uid="{5DFE6518-BD4D-4549-AB00-0EE49338D457}"/>
-    <hyperlink ref="D77" r:id="rId36" xr:uid="{9B51E31E-B1C5-8D4D-81F2-CE7E5FEFD734}"/>
-    <hyperlink ref="D78" r:id="rId37" xr:uid="{0294F04A-3FAD-0B4A-B3C5-136B9BFEB9ED}"/>
-    <hyperlink ref="D79" r:id="rId38" xr:uid="{E304CDD0-F736-9840-B873-3814D3979A08}"/>
-    <hyperlink ref="D81" r:id="rId39" xr:uid="{7F1EFF99-583A-6B4D-A3EB-824895A98C6F}"/>
-    <hyperlink ref="D84" r:id="rId40" xr:uid="{F3A77ECC-804C-1E44-94A7-51411C449BA3}"/>
-    <hyperlink ref="D82" r:id="rId41" xr:uid="{A3CF8173-1ABB-874D-AFE8-C0816C3C4A29}"/>
-    <hyperlink ref="D88" r:id="rId42" xr:uid="{42481CE0-DCAC-7347-A21F-7C04B44C6492}"/>
-    <hyperlink ref="D90" r:id="rId43" xr:uid="{8B79ADB7-F134-A54C-8A6F-8029C920BB98}"/>
-    <hyperlink ref="D93" r:id="rId44" xr:uid="{0F29D32C-0E67-F248-8C35-9710D68A7F85}"/>
-    <hyperlink ref="D94" r:id="rId45" xr:uid="{BA71FBDC-01A3-4A48-BCA0-1C6E4893F910}"/>
-    <hyperlink ref="D75" r:id="rId46" xr:uid="{9995D19A-7C18-FD4A-B802-9520BA771167}"/>
-    <hyperlink ref="D96" r:id="rId47" xr:uid="{304009F6-D9B7-CA4A-8889-BE080E8A7654}"/>
-    <hyperlink ref="D97" r:id="rId48" xr:uid="{4795B6FC-18EE-9043-8CE7-AF2924E6749D}"/>
-    <hyperlink ref="D99" r:id="rId49" xr:uid="{D578DF58-1254-4444-A5AA-946137A0D551}"/>
-    <hyperlink ref="D100" r:id="rId50" xr:uid="{18921900-3790-4748-9B02-AE7CF2E83568}"/>
-    <hyperlink ref="D98" r:id="rId51" xr:uid="{86F5F152-3AE3-C84D-9FFC-1DEDBE048190}"/>
-    <hyperlink ref="D106" r:id="rId52" xr:uid="{AD61CAC4-24BC-954B-A0DF-1642FA6C333B}"/>
-    <hyperlink ref="D101" r:id="rId53" xr:uid="{D07E7B17-1A5D-4544-BA76-5313EC783C1A}"/>
-    <hyperlink ref="D83" r:id="rId54" xr:uid="{A15B0F1F-A780-1F46-B188-D9ABDB5704B5}"/>
-    <hyperlink ref="D102" r:id="rId55" xr:uid="{979D158A-596F-9A47-AB5E-A72097511FA1}"/>
-    <hyperlink ref="D71" r:id="rId56" xr:uid="{A15BE685-A40C-734C-AD72-47F9BF601FDA}"/>
-    <hyperlink ref="D87" r:id="rId57" xr:uid="{FB025A70-6F06-4E4E-8984-BA9B9A2AF297}"/>
-    <hyperlink ref="D86" r:id="rId58" xr:uid="{1E58D491-53C2-2A42-A667-CC2FC0000945}"/>
-    <hyperlink ref="D107" r:id="rId59" xr:uid="{3ACCDC43-EF65-2A4A-A85E-EAF5CBC58797}"/>
-    <hyperlink ref="D108" r:id="rId60" xr:uid="{25D4D054-F5CD-6342-9DEC-8930BA66BE1A}"/>
-    <hyperlink ref="D109" r:id="rId61" xr:uid="{8CCF119F-F952-D34D-AF8C-DFB4362DB485}"/>
-    <hyperlink ref="D110" r:id="rId62" xr:uid="{54F9A12F-EE15-FF41-AC0A-F0A2DEAF65D5}"/>
-    <hyperlink ref="D119" r:id="rId63" xr:uid="{A324DF56-4206-4746-9CDE-46BC8817E2EB}"/>
-    <hyperlink ref="D120" r:id="rId64" xr:uid="{F809319C-4A84-3B46-A615-A43A53515FA1}"/>
-    <hyperlink ref="D121" r:id="rId65" xr:uid="{331E1E74-43DD-8B44-BF01-87A292B96D3E}"/>
-    <hyperlink ref="D123" r:id="rId66" xr:uid="{0450769E-D191-D142-8255-A056AD20F92E}"/>
-    <hyperlink ref="D63" r:id="rId67" xr:uid="{877003D4-412B-1C4A-B9C5-07DF56DA7218}"/>
-    <hyperlink ref="D64" r:id="rId68" xr:uid="{BF399E5E-1ECA-414D-A2D4-57E85D27B367}"/>
-    <hyperlink ref="D125" r:id="rId69" xr:uid="{BB764D03-6EBC-9C46-ACF7-5FD301EB57E9}"/>
-    <hyperlink ref="D126" r:id="rId70" xr:uid="{E0E6E7A9-4B34-9D48-B226-2529539960C3}"/>
-    <hyperlink ref="D129" r:id="rId71" xr:uid="{EE01CD31-A0CC-FB4E-9234-D39DC44BBEF2}"/>
-    <hyperlink ref="D130" r:id="rId72" xr:uid="{3C47FF5A-BE3C-7C4E-829E-4945618A9C1F}"/>
-    <hyperlink ref="D131" r:id="rId73" xr:uid="{F5493FE6-0313-1940-AEFF-050A934E8083}"/>
-    <hyperlink ref="D132" r:id="rId74" xr:uid="{F415321A-3F49-EB4E-B6A9-EFE163590B41}"/>
-    <hyperlink ref="D133" r:id="rId75" xr:uid="{C84C6E00-5661-0D49-A0D1-CFD70865A82D}"/>
-    <hyperlink ref="D134" r:id="rId76" xr:uid="{E23DB724-160F-8543-B648-70EB7CA0365F}"/>
-    <hyperlink ref="D135" r:id="rId77" xr:uid="{E29FA1EF-7AB7-E245-832F-7B087D0E7EA3}"/>
-    <hyperlink ref="D136" r:id="rId78" xr:uid="{388C4274-E38A-B449-8F40-7ED095B192D7}"/>
-    <hyperlink ref="D137" r:id="rId79" xr:uid="{A966469C-688F-1E4F-8C89-F7E400609830}"/>
-    <hyperlink ref="D150" r:id="rId80" xr:uid="{B7708F6B-F6E6-BF41-8AF3-54C00F11C52B}"/>
-    <hyperlink ref="D158" r:id="rId81" xr:uid="{BF7922F0-DD27-EE45-AF85-5C9161DA389C}"/>
-    <hyperlink ref="D159" r:id="rId82" xr:uid="{BC00976C-C73B-6F4E-B032-65F2D572F141}"/>
-    <hyperlink ref="D164" r:id="rId83" xr:uid="{77C86A54-F6B8-BA40-A768-CCB7D4C99562}"/>
-    <hyperlink ref="D165" r:id="rId84" xr:uid="{CAB158A3-D761-8448-A767-9525660B6326}"/>
-    <hyperlink ref="D166" r:id="rId85" xr:uid="{34BE3A49-BE9D-4049-97A0-80E02A01A961}"/>
-    <hyperlink ref="D151" r:id="rId86" xr:uid="{781FF30D-914F-7841-92BF-6AD62300904B}"/>
-    <hyperlink ref="D157" r:id="rId87" xr:uid="{3CBAAA26-1E37-B044-B755-258229968E67}"/>
-    <hyperlink ref="D167" r:id="rId88" xr:uid="{DCC7B2BC-EB59-DB49-9BF9-45BF0E030221}"/>
-    <hyperlink ref="D168" r:id="rId89" xr:uid="{22C8D3B5-CBB9-C448-83B5-05CE9F72E696}"/>
-    <hyperlink ref="D169" r:id="rId90" xr:uid="{A3C5359E-186C-1640-839A-F7F1B599F0B5}"/>
-    <hyperlink ref="D170" r:id="rId91" xr:uid="{CD78268C-7DEC-FB44-88AA-75EC6DE77C62}"/>
-    <hyperlink ref="D171" r:id="rId92" xr:uid="{5BC45F49-43E2-5D46-B9F7-C9DE4586524D}"/>
-    <hyperlink ref="D172" r:id="rId93" xr:uid="{3B77FB2E-5F37-D04A-B1B0-08D6A165225B}"/>
-    <hyperlink ref="D173" r:id="rId94" xr:uid="{6EA4E64A-6FFB-FC43-A3F9-B515DC03D9ED}"/>
-    <hyperlink ref="D174" r:id="rId95" xr:uid="{7D0BC227-6BA4-F747-B1DB-B7CCF5D3057E}"/>
-    <hyperlink ref="D175" r:id="rId96" xr:uid="{19FE4A6D-FF5E-BF49-8C4B-F24B3005865C}"/>
-    <hyperlink ref="D176" r:id="rId97" xr:uid="{41D1D3F0-3B5D-964A-BC98-E26309342AC6}"/>
-    <hyperlink ref="D178" r:id="rId98" xr:uid="{C852E2F0-FC27-4F41-89CD-E264B7CB2DF7}"/>
-    <hyperlink ref="D179" r:id="rId99" xr:uid="{DF3B379B-CACF-954D-AEAA-0FF3E835924A}"/>
-    <hyperlink ref="D180" r:id="rId100" xr:uid="{7FADB0C5-8AA0-6F41-A92E-5B09572E4D18}"/>
-    <hyperlink ref="D181" r:id="rId101" xr:uid="{3103A3F7-AC33-1C4E-BCE8-2934FE92BC5F}"/>
-    <hyperlink ref="D182" r:id="rId102" xr:uid="{07DF88EF-4EAA-1440-8D82-60A0FD7CADD1}"/>
-    <hyperlink ref="D183" r:id="rId103" xr:uid="{E19890F5-0215-4644-AEA1-BF7692385DF1}"/>
-    <hyperlink ref="D184" r:id="rId104" xr:uid="{86B64C9A-DAFF-CF44-A151-29AA7D14977F}"/>
-    <hyperlink ref="D185" r:id="rId105" xr:uid="{3FEFD335-04F9-4F41-B6A0-B080D6550649}"/>
-    <hyperlink ref="D186" r:id="rId106" xr:uid="{90B99E7F-0693-D54F-A4F6-34AD69A3D631}"/>
-    <hyperlink ref="D187" r:id="rId107" xr:uid="{B95F960A-6D1F-2D47-8457-F9DE115B5C38}"/>
-    <hyperlink ref="D188" r:id="rId108" xr:uid="{00ECE393-EC26-344F-8B40-377C3EB5D890}"/>
-    <hyperlink ref="D189" r:id="rId109" xr:uid="{C28E61A4-8435-BF4D-8BA4-7A3647FBFF00}"/>
-    <hyperlink ref="D190" r:id="rId110" xr:uid="{3CAEF1A6-A029-A64D-903F-EB0ADFF46D37}"/>
-    <hyperlink ref="D191" r:id="rId111" xr:uid="{9DF090F0-97A2-E946-850D-1ECC6DB92707}"/>
-    <hyperlink ref="D192" r:id="rId112" xr:uid="{C85A63BA-1F71-584A-A604-B6AB345ECE95}"/>
-    <hyperlink ref="D92" r:id="rId113" xr:uid="{2F59B8F2-7AB0-AE47-85CD-C244BB59B3BA}"/>
-    <hyperlink ref="D193" r:id="rId114" xr:uid="{06DC547A-085D-7C45-A4F0-49F7349DAAB0}"/>
-    <hyperlink ref="D194" r:id="rId115" xr:uid="{D65368D6-C0A7-5B4C-83C0-4DFB768DE3C6}"/>
-    <hyperlink ref="D195" r:id="rId116" xr:uid="{B7606443-1D1E-724A-8040-131FD0AC6338}"/>
-    <hyperlink ref="D196" r:id="rId117" xr:uid="{79B43F1F-03A0-F747-AC05-79F3D0B4BCCB}"/>
-    <hyperlink ref="D197" r:id="rId118" xr:uid="{875EF5F0-7651-8745-87D6-636AD559D72E}"/>
-    <hyperlink ref="D198" r:id="rId119" xr:uid="{6E4DCDAE-D012-BD4D-A394-90B249BB99C5}"/>
-    <hyperlink ref="D199" r:id="rId120" xr:uid="{3DAD8E8C-E2BB-074B-B3F0-D475C7FD6B2D}"/>
-    <hyperlink ref="D200" r:id="rId121" xr:uid="{222D21AE-1088-BD48-BAEE-1EF3912460AF}"/>
-    <hyperlink ref="D201" r:id="rId122" xr:uid="{7AD5FFD0-8F45-1941-9BBF-D91BBC4F0F40}"/>
-    <hyperlink ref="D203" r:id="rId123" xr:uid="{518258DC-5A20-3D40-91D0-D032DC42B6AD}"/>
-    <hyperlink ref="D204" r:id="rId124" xr:uid="{5B069AF2-81F6-A34E-80A0-7E8EBE3DFA2A}"/>
-    <hyperlink ref="D205" r:id="rId125" xr:uid="{A04E8385-1CE9-364E-91A1-6F09D76ACF42}"/>
-    <hyperlink ref="D206" r:id="rId126" xr:uid="{3113EFF0-EE9A-354C-8BD1-5D9364B99893}"/>
-    <hyperlink ref="D207" r:id="rId127" xr:uid="{A06F9F88-431E-574D-92C0-E68077FC529D}"/>
-    <hyperlink ref="D208" r:id="rId128" xr:uid="{8B4EF43A-AE24-6947-8EFA-E38936068D18}"/>
-    <hyperlink ref="C209" r:id="rId129" display="https://www.bostonmpo.org/node/3243" xr:uid="{655CEEAA-6095-9B47-995E-CD64750746E0}"/>
-    <hyperlink ref="D209" r:id="rId130" xr:uid="{055A514B-7345-F948-9754-CCC9031C0081}"/>
-    <hyperlink ref="D211" r:id="rId131" xr:uid="{90B28A53-CDAB-EC48-9FC0-0E277128FCA7}"/>
-    <hyperlink ref="D212" r:id="rId132" xr:uid="{AC529FF5-CF2C-1D4B-95AB-70ED1909D783}"/>
-    <hyperlink ref="D213" r:id="rId133" xr:uid="{ECE456D6-90BA-E547-8B10-93E537F7BF40}"/>
-    <hyperlink ref="D214" r:id="rId134" xr:uid="{2686E174-B756-124D-82F8-89B4FFA6EE04}"/>
-    <hyperlink ref="D215" r:id="rId135" xr:uid="{F529B5BA-08ED-3642-9481-1E3CCADBB5B4}"/>
-    <hyperlink ref="D216" r:id="rId136" xr:uid="{0D583AB0-0EC1-4143-9730-B654F3258218}"/>
-    <hyperlink ref="D217" r:id="rId137" xr:uid="{D3776250-774B-AB40-A8B2-B7A3B3F11494}"/>
-    <hyperlink ref="D218" r:id="rId138" xr:uid="{816B8DD7-C959-7845-A7B3-E11200634DE3}"/>
-    <hyperlink ref="D229" r:id="rId139" xr:uid="{8E6DE810-4336-264A-9286-F5DE4FCB3616}"/>
-    <hyperlink ref="D230" r:id="rId140" xr:uid="{74958D82-AE52-764E-A4F1-2CBA9EA9ACED}"/>
-    <hyperlink ref="D231" r:id="rId141" xr:uid="{4C8C770A-DBF9-8447-AF54-9001929EDD34}"/>
-    <hyperlink ref="D232" r:id="rId142" xr:uid="{263568FF-4DC1-A245-B266-0B8D89A595BD}"/>
-    <hyperlink ref="D233" r:id="rId143" xr:uid="{0BB8C344-5E31-7E4A-927C-AF47B71575BB}"/>
-    <hyperlink ref="D235" r:id="rId144" xr:uid="{903A7E98-5E9D-544C-B0B8-8E7D2C9D47EB}"/>
+    <hyperlink ref="D70" r:id="rId31" xr:uid="{90EBC071-E84D-4549-A9CE-645045A70E75}"/>
+    <hyperlink ref="D71" r:id="rId32" xr:uid="{E731DF72-6E9F-0240-B2A4-95E82B8C938A}"/>
+    <hyperlink ref="D74" r:id="rId33" xr:uid="{5391EFF3-6DAD-4E40-9C66-C7501F2ABF1B}"/>
+    <hyperlink ref="D75" r:id="rId34" xr:uid="{EBCA5E87-62CD-FD46-9F99-E2FD5D3229F6}"/>
+    <hyperlink ref="D77" r:id="rId35" xr:uid="{5DFE6518-BD4D-4549-AB00-0EE49338D457}"/>
+    <hyperlink ref="D78" r:id="rId36" xr:uid="{9B51E31E-B1C5-8D4D-81F2-CE7E5FEFD734}"/>
+    <hyperlink ref="D79" r:id="rId37" xr:uid="{0294F04A-3FAD-0B4A-B3C5-136B9BFEB9ED}"/>
+    <hyperlink ref="D80" r:id="rId38" xr:uid="{E304CDD0-F736-9840-B873-3814D3979A08}"/>
+    <hyperlink ref="D82" r:id="rId39" xr:uid="{7F1EFF99-583A-6B4D-A3EB-824895A98C6F}"/>
+    <hyperlink ref="D85" r:id="rId40" xr:uid="{F3A77ECC-804C-1E44-94A7-51411C449BA3}"/>
+    <hyperlink ref="D83" r:id="rId41" xr:uid="{A3CF8173-1ABB-874D-AFE8-C0816C3C4A29}"/>
+    <hyperlink ref="D89" r:id="rId42" xr:uid="{42481CE0-DCAC-7347-A21F-7C04B44C6492}"/>
+    <hyperlink ref="D91" r:id="rId43" xr:uid="{8B79ADB7-F134-A54C-8A6F-8029C920BB98}"/>
+    <hyperlink ref="D94" r:id="rId44" xr:uid="{0F29D32C-0E67-F248-8C35-9710D68A7F85}"/>
+    <hyperlink ref="D95" r:id="rId45" xr:uid="{BA71FBDC-01A3-4A48-BCA0-1C6E4893F910}"/>
+    <hyperlink ref="D76" r:id="rId46" xr:uid="{9995D19A-7C18-FD4A-B802-9520BA771167}"/>
+    <hyperlink ref="D97" r:id="rId47" xr:uid="{304009F6-D9B7-CA4A-8889-BE080E8A7654}"/>
+    <hyperlink ref="D98" r:id="rId48" xr:uid="{4795B6FC-18EE-9043-8CE7-AF2924E6749D}"/>
+    <hyperlink ref="D100" r:id="rId49" xr:uid="{D578DF58-1254-4444-A5AA-946137A0D551}"/>
+    <hyperlink ref="D101" r:id="rId50" xr:uid="{18921900-3790-4748-9B02-AE7CF2E83568}"/>
+    <hyperlink ref="D99" r:id="rId51" xr:uid="{86F5F152-3AE3-C84D-9FFC-1DEDBE048190}"/>
+    <hyperlink ref="D107" r:id="rId52" xr:uid="{AD61CAC4-24BC-954B-A0DF-1642FA6C333B}"/>
+    <hyperlink ref="D102" r:id="rId53" xr:uid="{D07E7B17-1A5D-4544-BA76-5313EC783C1A}"/>
+    <hyperlink ref="D84" r:id="rId54" xr:uid="{A15B0F1F-A780-1F46-B188-D9ABDB5704B5}"/>
+    <hyperlink ref="D103" r:id="rId55" xr:uid="{979D158A-596F-9A47-AB5E-A72097511FA1}"/>
+    <hyperlink ref="D72" r:id="rId56" xr:uid="{A15BE685-A40C-734C-AD72-47F9BF601FDA}"/>
+    <hyperlink ref="D88" r:id="rId57" xr:uid="{FB025A70-6F06-4E4E-8984-BA9B9A2AF297}"/>
+    <hyperlink ref="D87" r:id="rId58" xr:uid="{1E58D491-53C2-2A42-A667-CC2FC0000945}"/>
+    <hyperlink ref="D108" r:id="rId59" xr:uid="{3ACCDC43-EF65-2A4A-A85E-EAF5CBC58797}"/>
+    <hyperlink ref="D109" r:id="rId60" xr:uid="{25D4D054-F5CD-6342-9DEC-8930BA66BE1A}"/>
+    <hyperlink ref="D110" r:id="rId61" xr:uid="{8CCF119F-F952-D34D-AF8C-DFB4362DB485}"/>
+    <hyperlink ref="D111" r:id="rId62" xr:uid="{54F9A12F-EE15-FF41-AC0A-F0A2DEAF65D5}"/>
+    <hyperlink ref="D120" r:id="rId63" xr:uid="{A324DF56-4206-4746-9CDE-46BC8817E2EB}"/>
+    <hyperlink ref="D121" r:id="rId64" xr:uid="{F809319C-4A84-3B46-A615-A43A53515FA1}"/>
+    <hyperlink ref="D122" r:id="rId65" xr:uid="{331E1E74-43DD-8B44-BF01-87A292B96D3E}"/>
+    <hyperlink ref="D124" r:id="rId66" xr:uid="{0450769E-D191-D142-8255-A056AD20F92E}"/>
+    <hyperlink ref="D64" r:id="rId67" xr:uid="{877003D4-412B-1C4A-B9C5-07DF56DA7218}"/>
+    <hyperlink ref="D65" r:id="rId68" xr:uid="{BF399E5E-1ECA-414D-A2D4-57E85D27B367}"/>
+    <hyperlink ref="D126" r:id="rId69" xr:uid="{BB764D03-6EBC-9C46-ACF7-5FD301EB57E9}"/>
+    <hyperlink ref="D127" r:id="rId70" xr:uid="{E0E6E7A9-4B34-9D48-B226-2529539960C3}"/>
+    <hyperlink ref="D130" r:id="rId71" xr:uid="{EE01CD31-A0CC-FB4E-9234-D39DC44BBEF2}"/>
+    <hyperlink ref="D131" r:id="rId72" xr:uid="{3C47FF5A-BE3C-7C4E-829E-4945618A9C1F}"/>
+    <hyperlink ref="D132" r:id="rId73" xr:uid="{F5493FE6-0313-1940-AEFF-050A934E8083}"/>
+    <hyperlink ref="D133" r:id="rId74" xr:uid="{F415321A-3F49-EB4E-B6A9-EFE163590B41}"/>
+    <hyperlink ref="D134" r:id="rId75" xr:uid="{C84C6E00-5661-0D49-A0D1-CFD70865A82D}"/>
+    <hyperlink ref="D135" r:id="rId76" xr:uid="{E23DB724-160F-8543-B648-70EB7CA0365F}"/>
+    <hyperlink ref="D136" r:id="rId77" xr:uid="{E29FA1EF-7AB7-E245-832F-7B087D0E7EA3}"/>
+    <hyperlink ref="D137" r:id="rId78" xr:uid="{388C4274-E38A-B449-8F40-7ED095B192D7}"/>
+    <hyperlink ref="D138" r:id="rId79" xr:uid="{A966469C-688F-1E4F-8C89-F7E400609830}"/>
+    <hyperlink ref="D151" r:id="rId80" xr:uid="{B7708F6B-F6E6-BF41-8AF3-54C00F11C52B}"/>
+    <hyperlink ref="D159" r:id="rId81" xr:uid="{BF7922F0-DD27-EE45-AF85-5C9161DA389C}"/>
+    <hyperlink ref="D160" r:id="rId82" xr:uid="{BC00976C-C73B-6F4E-B032-65F2D572F141}"/>
+    <hyperlink ref="D165" r:id="rId83" xr:uid="{77C86A54-F6B8-BA40-A768-CCB7D4C99562}"/>
+    <hyperlink ref="D166" r:id="rId84" xr:uid="{CAB158A3-D761-8448-A767-9525660B6326}"/>
+    <hyperlink ref="D167" r:id="rId85" xr:uid="{34BE3A49-BE9D-4049-97A0-80E02A01A961}"/>
+    <hyperlink ref="D152" r:id="rId86" xr:uid="{781FF30D-914F-7841-92BF-6AD62300904B}"/>
+    <hyperlink ref="D158" r:id="rId87" xr:uid="{3CBAAA26-1E37-B044-B755-258229968E67}"/>
+    <hyperlink ref="D168" r:id="rId88" xr:uid="{DCC7B2BC-EB59-DB49-9BF9-45BF0E030221}"/>
+    <hyperlink ref="D169" r:id="rId89" xr:uid="{22C8D3B5-CBB9-C448-83B5-05CE9F72E696}"/>
+    <hyperlink ref="D170" r:id="rId90" xr:uid="{A3C5359E-186C-1640-839A-F7F1B599F0B5}"/>
+    <hyperlink ref="D171" r:id="rId91" xr:uid="{CD78268C-7DEC-FB44-88AA-75EC6DE77C62}"/>
+    <hyperlink ref="D172" r:id="rId92" xr:uid="{5BC45F49-43E2-5D46-B9F7-C9DE4586524D}"/>
+    <hyperlink ref="D173" r:id="rId93" xr:uid="{3B77FB2E-5F37-D04A-B1B0-08D6A165225B}"/>
+    <hyperlink ref="D174" r:id="rId94" xr:uid="{6EA4E64A-6FFB-FC43-A3F9-B515DC03D9ED}"/>
+    <hyperlink ref="D175" r:id="rId95" xr:uid="{7D0BC227-6BA4-F747-B1DB-B7CCF5D3057E}"/>
+    <hyperlink ref="D176" r:id="rId96" xr:uid="{19FE4A6D-FF5E-BF49-8C4B-F24B3005865C}"/>
+    <hyperlink ref="D177" r:id="rId97" xr:uid="{41D1D3F0-3B5D-964A-BC98-E26309342AC6}"/>
+    <hyperlink ref="D179" r:id="rId98" xr:uid="{C852E2F0-FC27-4F41-89CD-E264B7CB2DF7}"/>
+    <hyperlink ref="D180" r:id="rId99" xr:uid="{DF3B379B-CACF-954D-AEAA-0FF3E835924A}"/>
+    <hyperlink ref="D181" r:id="rId100" xr:uid="{7FADB0C5-8AA0-6F41-A92E-5B09572E4D18}"/>
+    <hyperlink ref="D182" r:id="rId101" xr:uid="{3103A3F7-AC33-1C4E-BCE8-2934FE92BC5F}"/>
+    <hyperlink ref="D183" r:id="rId102" xr:uid="{07DF88EF-4EAA-1440-8D82-60A0FD7CADD1}"/>
+    <hyperlink ref="D184" r:id="rId103" xr:uid="{E19890F5-0215-4644-AEA1-BF7692385DF1}"/>
+    <hyperlink ref="D185" r:id="rId104" xr:uid="{86B64C9A-DAFF-CF44-A151-29AA7D14977F}"/>
+    <hyperlink ref="D186" r:id="rId105" xr:uid="{3FEFD335-04F9-4F41-B6A0-B080D6550649}"/>
+    <hyperlink ref="D187" r:id="rId106" xr:uid="{90B99E7F-0693-D54F-A4F6-34AD69A3D631}"/>
+    <hyperlink ref="D188" r:id="rId107" xr:uid="{B95F960A-6D1F-2D47-8457-F9DE115B5C38}"/>
+    <hyperlink ref="D189" r:id="rId108" xr:uid="{00ECE393-EC26-344F-8B40-377C3EB5D890}"/>
+    <hyperlink ref="D190" r:id="rId109" xr:uid="{C28E61A4-8435-BF4D-8BA4-7A3647FBFF00}"/>
+    <hyperlink ref="D191" r:id="rId110" xr:uid="{3CAEF1A6-A029-A64D-903F-EB0ADFF46D37}"/>
+    <hyperlink ref="D192" r:id="rId111" xr:uid="{9DF090F0-97A2-E946-850D-1ECC6DB92707}"/>
+    <hyperlink ref="D193" r:id="rId112" xr:uid="{C85A63BA-1F71-584A-A604-B6AB345ECE95}"/>
+    <hyperlink ref="D93" r:id="rId113" xr:uid="{2F59B8F2-7AB0-AE47-85CD-C244BB59B3BA}"/>
+    <hyperlink ref="D194" r:id="rId114" xr:uid="{06DC547A-085D-7C45-A4F0-49F7349DAAB0}"/>
+    <hyperlink ref="D195" r:id="rId115" xr:uid="{D65368D6-C0A7-5B4C-83C0-4DFB768DE3C6}"/>
+    <hyperlink ref="D196" r:id="rId116" xr:uid="{B7606443-1D1E-724A-8040-131FD0AC6338}"/>
+    <hyperlink ref="D197" r:id="rId117" xr:uid="{79B43F1F-03A0-F747-AC05-79F3D0B4BCCB}"/>
+    <hyperlink ref="D198" r:id="rId118" xr:uid="{875EF5F0-7651-8745-87D6-636AD559D72E}"/>
+    <hyperlink ref="D199" r:id="rId119" xr:uid="{6E4DCDAE-D012-BD4D-A394-90B249BB99C5}"/>
+    <hyperlink ref="D200" r:id="rId120" xr:uid="{3DAD8E8C-E2BB-074B-B3F0-D475C7FD6B2D}"/>
+    <hyperlink ref="D201" r:id="rId121" xr:uid="{222D21AE-1088-BD48-BAEE-1EF3912460AF}"/>
+    <hyperlink ref="D202" r:id="rId122" xr:uid="{7AD5FFD0-8F45-1941-9BBF-D91BBC4F0F40}"/>
+    <hyperlink ref="D204" r:id="rId123" xr:uid="{518258DC-5A20-3D40-91D0-D032DC42B6AD}"/>
+    <hyperlink ref="D205" r:id="rId124" xr:uid="{5B069AF2-81F6-A34E-80A0-7E8EBE3DFA2A}"/>
+    <hyperlink ref="D206" r:id="rId125" xr:uid="{A04E8385-1CE9-364E-91A1-6F09D76ACF42}"/>
+    <hyperlink ref="D207" r:id="rId126" xr:uid="{3113EFF0-EE9A-354C-8BD1-5D9364B99893}"/>
+    <hyperlink ref="D208" r:id="rId127" xr:uid="{A06F9F88-431E-574D-92C0-E68077FC529D}"/>
+    <hyperlink ref="D209" r:id="rId128" xr:uid="{8B4EF43A-AE24-6947-8EFA-E38936068D18}"/>
+    <hyperlink ref="C210" r:id="rId129" display="https://www.bostonmpo.org/node/3243" xr:uid="{655CEEAA-6095-9B47-995E-CD64750746E0}"/>
+    <hyperlink ref="D210" r:id="rId130" xr:uid="{055A514B-7345-F948-9754-CCC9031C0081}"/>
+    <hyperlink ref="D212" r:id="rId131" xr:uid="{90B28A53-CDAB-EC48-9FC0-0E277128FCA7}"/>
+    <hyperlink ref="D213" r:id="rId132" xr:uid="{AC529FF5-CF2C-1D4B-95AB-70ED1909D783}"/>
+    <hyperlink ref="D214" r:id="rId133" xr:uid="{ECE456D6-90BA-E547-8B10-93E537F7BF40}"/>
+    <hyperlink ref="D215" r:id="rId134" xr:uid="{2686E174-B756-124D-82F8-89B4FFA6EE04}"/>
+    <hyperlink ref="D216" r:id="rId135" xr:uid="{F529B5BA-08ED-3642-9481-1E3CCADBB5B4}"/>
+    <hyperlink ref="D217" r:id="rId136" xr:uid="{0D583AB0-0EC1-4143-9730-B654F3258218}"/>
+    <hyperlink ref="D218" r:id="rId137" xr:uid="{D3776250-774B-AB40-A8B2-B7A3B3F11494}"/>
+    <hyperlink ref="D219" r:id="rId138" xr:uid="{816B8DD7-C959-7845-A7B3-E11200634DE3}"/>
+    <hyperlink ref="D230" r:id="rId139" xr:uid="{8E6DE810-4336-264A-9286-F5DE4FCB3616}"/>
+    <hyperlink ref="D231" r:id="rId140" xr:uid="{74958D82-AE52-764E-A4F1-2CBA9EA9ACED}"/>
+    <hyperlink ref="D232" r:id="rId141" xr:uid="{4C8C770A-DBF9-8447-AF54-9001929EDD34}"/>
+    <hyperlink ref="D233" r:id="rId142" xr:uid="{263568FF-4DC1-A245-B266-0B8D89A595BD}"/>
+    <hyperlink ref="D234" r:id="rId143" xr:uid="{0BB8C344-5E31-7E4A-927C-AF47B71575BB}"/>
+    <hyperlink ref="D236" r:id="rId144" xr:uid="{903A7E98-5E9D-544C-B0B8-8E7D2C9D47EB}"/>
     <hyperlink ref="D53" r:id="rId145" xr:uid="{2690B48D-BA39-6543-BD43-72740F6D06FB}"/>
-    <hyperlink ref="D236" r:id="rId146" xr:uid="{CA43EE9E-6054-8246-8F09-73619591E4D8}"/>
-    <hyperlink ref="D240" r:id="rId147" xr:uid="{5BBBF668-7181-034B-A7E7-B37F0489798D}"/>
-    <hyperlink ref="D241" r:id="rId148" xr:uid="{F25E9123-06C3-4D48-8368-7DC4D8ADFDFE}"/>
-    <hyperlink ref="D246" r:id="rId149" xr:uid="{FE44C4D8-FAA2-6C4A-A061-1E08E9AF9BAE}"/>
-    <hyperlink ref="D247" r:id="rId150" xr:uid="{4A0071B2-48C3-F840-B489-A422B212DF05}"/>
-    <hyperlink ref="D248" r:id="rId151" xr:uid="{0BD877BC-868A-5E4A-987A-4883C51D584C}"/>
-    <hyperlink ref="D250" r:id="rId152" xr:uid="{F7F59C8F-6228-3744-8DF6-9F3A5D6E4A08}"/>
-    <hyperlink ref="D251" r:id="rId153" xr:uid="{8156E09C-4D4B-844F-9152-763F5CBB848C}"/>
-    <hyperlink ref="D252" r:id="rId154" xr:uid="{D66FD1BC-2A48-1D44-9C56-A2091EA6EB4F}"/>
-    <hyperlink ref="D253" r:id="rId155" xr:uid="{EED901F1-9FA7-0241-A3A8-1DEC4ADB4F65}"/>
-    <hyperlink ref="D249" r:id="rId156" xr:uid="{ACBAEB0F-A745-BD4B-A79F-28E87E3B7670}"/>
-    <hyperlink ref="D242" r:id="rId157" xr:uid="{6FE5FEA9-69D3-5B44-8339-E00169C80FE7}"/>
-    <hyperlink ref="D254" r:id="rId158" xr:uid="{4E39217A-DB80-A04A-A66F-DC478E8BD9B0}"/>
-    <hyperlink ref="D256" r:id="rId159" xr:uid="{FD84BB06-83F9-8145-B29B-E82DD0A255FA}"/>
-    <hyperlink ref="D257" r:id="rId160" xr:uid="{0F664415-A56C-5944-BD33-2BBC535C69EE}"/>
-    <hyperlink ref="D258" r:id="rId161" xr:uid="{1B9FDFCF-CDAA-B043-90DF-464B3F19D029}"/>
-    <hyperlink ref="D260" r:id="rId162" xr:uid="{87374CD1-533B-1843-AFD1-A46E4CCC2786}"/>
-    <hyperlink ref="D261" r:id="rId163" xr:uid="{735892DA-3CF9-7D43-938E-C539C1354F7E}"/>
-    <hyperlink ref="D262" r:id="rId164" xr:uid="{25B8E5AB-DD5E-B943-A89D-CF3BCFD8C69D}"/>
-    <hyperlink ref="D263" r:id="rId165" xr:uid="{863254B5-D467-6A40-9BF8-0E3F61B42855}"/>
+    <hyperlink ref="D237" r:id="rId146" xr:uid="{CA43EE9E-6054-8246-8F09-73619591E4D8}"/>
+    <hyperlink ref="D241" r:id="rId147" xr:uid="{5BBBF668-7181-034B-A7E7-B37F0489798D}"/>
+    <hyperlink ref="D242" r:id="rId148" xr:uid="{F25E9123-06C3-4D48-8368-7DC4D8ADFDFE}"/>
+    <hyperlink ref="D247" r:id="rId149" xr:uid="{FE44C4D8-FAA2-6C4A-A061-1E08E9AF9BAE}"/>
+    <hyperlink ref="D248" r:id="rId150" xr:uid="{4A0071B2-48C3-F840-B489-A422B212DF05}"/>
+    <hyperlink ref="D249" r:id="rId151" xr:uid="{0BD877BC-868A-5E4A-987A-4883C51D584C}"/>
+    <hyperlink ref="D251" r:id="rId152" xr:uid="{F7F59C8F-6228-3744-8DF6-9F3A5D6E4A08}"/>
+    <hyperlink ref="D252" r:id="rId153" xr:uid="{8156E09C-4D4B-844F-9152-763F5CBB848C}"/>
+    <hyperlink ref="D253" r:id="rId154" xr:uid="{D66FD1BC-2A48-1D44-9C56-A2091EA6EB4F}"/>
+    <hyperlink ref="D254" r:id="rId155" xr:uid="{EED901F1-9FA7-0241-A3A8-1DEC4ADB4F65}"/>
+    <hyperlink ref="D250" r:id="rId156" xr:uid="{ACBAEB0F-A745-BD4B-A79F-28E87E3B7670}"/>
+    <hyperlink ref="D243" r:id="rId157" xr:uid="{6FE5FEA9-69D3-5B44-8339-E00169C80FE7}"/>
+    <hyperlink ref="D255" r:id="rId158" xr:uid="{4E39217A-DB80-A04A-A66F-DC478E8BD9B0}"/>
+    <hyperlink ref="D257" r:id="rId159" xr:uid="{FD84BB06-83F9-8145-B29B-E82DD0A255FA}"/>
+    <hyperlink ref="D258" r:id="rId160" xr:uid="{0F664415-A56C-5944-BD33-2BBC535C69EE}"/>
+    <hyperlink ref="D259" r:id="rId161" xr:uid="{1B9FDFCF-CDAA-B043-90DF-464B3F19D029}"/>
+    <hyperlink ref="D261" r:id="rId162" xr:uid="{87374CD1-533B-1843-AFD1-A46E4CCC2786}"/>
+    <hyperlink ref="D262" r:id="rId163" xr:uid="{735892DA-3CF9-7D43-938E-C539C1354F7E}"/>
+    <hyperlink ref="D263" r:id="rId164" xr:uid="{25B8E5AB-DD5E-B943-A89D-CF3BCFD8C69D}"/>
+    <hyperlink ref="D264" r:id="rId165" xr:uid="{863254B5-D467-6A40-9BF8-0E3F61B42855}"/>
     <hyperlink ref="D52" r:id="rId166" xr:uid="{70051547-7009-DA49-AD8A-CDA173903436}"/>
-    <hyperlink ref="D265" r:id="rId167" xr:uid="{1F55836F-92FB-504B-8890-DD155568B08F}"/>
-    <hyperlink ref="D266" r:id="rId168" xr:uid="{516BA828-1E71-6740-82CE-9ABCB5B2868A}"/>
-    <hyperlink ref="D267" r:id="rId169" xr:uid="{D01BC6DD-63D5-FE45-8701-DE7626C47912}"/>
-    <hyperlink ref="D268" r:id="rId170" xr:uid="{7F25EAA1-3640-2140-8ED9-4C0C8A766B64}"/>
-    <hyperlink ref="D269" r:id="rId171" location="the-ted-williams-tunnel-" xr:uid="{90CDFCE7-A34F-B543-940D-CBD77B3CA490}"/>
-    <hyperlink ref="D273" r:id="rId172" xr:uid="{33076741-07BA-AD48-9CFF-1F8FA7DC794F}"/>
-    <hyperlink ref="D274" r:id="rId173" xr:uid="{E2C2519F-06D0-F54F-A190-1006654C1217}"/>
-    <hyperlink ref="D277" r:id="rId174" xr:uid="{21200567-2A05-1B4A-9286-23765C1B5439}"/>
-    <hyperlink ref="D281" r:id="rId175" xr:uid="{2CD55170-8C56-B640-8914-62FD2B471773}"/>
-    <hyperlink ref="D280" r:id="rId176" xr:uid="{C5C05C21-059D-3E4F-83CE-07DE43CA77F8}"/>
-    <hyperlink ref="D284" r:id="rId177" xr:uid="{5A018FFC-E064-B841-B16C-1B5FDB1C2373}"/>
-    <hyperlink ref="D285" r:id="rId178" xr:uid="{9ECC5CD3-0C49-6241-9ADA-4B8F147F222D}"/>
-    <hyperlink ref="D286" r:id="rId179" xr:uid="{A70D9607-0490-DF4E-85B3-794BEB0DB3CD}"/>
-    <hyperlink ref="D287" r:id="rId180" xr:uid="{7F93E30A-E771-E541-A3E8-E8E115BAC442}"/>
-    <hyperlink ref="D288" r:id="rId181" xr:uid="{DF50B5D9-DAAC-7043-8DA2-3DBF2FCB4882}"/>
-    <hyperlink ref="D270" r:id="rId182" xr:uid="{2930C349-E6B7-544B-BB2A-773A46E73BCB}"/>
-    <hyperlink ref="D255" r:id="rId183" xr:uid="{2BE70040-B75E-144F-8CF2-C6FAF265243F}"/>
-    <hyperlink ref="D292" r:id="rId184" xr:uid="{69A55749-D9D2-1B4B-B3F9-4B160F762593}"/>
-    <hyperlink ref="D293" r:id="rId185" xr:uid="{FB9E4799-0707-754B-9240-DFB8EFCF3420}"/>
-    <hyperlink ref="D294" r:id="rId186" xr:uid="{EFA9A5C9-A935-FD44-A8C3-75A6D42D9D41}"/>
-    <hyperlink ref="D80" r:id="rId187" xr:uid="{18AB1C94-4CE1-2945-92C4-F9826FBC6B4E}"/>
-    <hyperlink ref="D295" r:id="rId188" xr:uid="{6CB68E90-F81E-C748-8D45-EFEEC50C2AE3}"/>
-    <hyperlink ref="D297" r:id="rId189" xr:uid="{8303BB33-5888-964E-8CF2-43DD162804AD}"/>
-    <hyperlink ref="D298" r:id="rId190" xr:uid="{6C92D97F-0A5E-394B-ABB8-0A48B9DDE3CE}"/>
-    <hyperlink ref="D299" r:id="rId191" xr:uid="{A23CD4FA-5C90-8B4F-B42D-8F0581378838}"/>
-    <hyperlink ref="D300" r:id="rId192" xr:uid="{A75CA764-6259-D247-9F3E-71FE84093EEF}"/>
-    <hyperlink ref="D301" r:id="rId193" xr:uid="{4FCB99F2-3FFA-D440-B956-CC2FD50BB76F}"/>
-    <hyperlink ref="D304" r:id="rId194" xr:uid="{936BB4A4-64DC-4640-8D60-262FEB18B51D}"/>
-    <hyperlink ref="D305" r:id="rId195" xr:uid="{09EB0BAC-80EB-3346-AF8B-932BAB3F6F52}"/>
-    <hyperlink ref="D306" r:id="rId196" xr:uid="{249C8010-6579-F842-931C-5A1AA5FFD47E}"/>
-    <hyperlink ref="D307" r:id="rId197" xr:uid="{C11D7F08-A472-D74F-ACD4-DC39321AAA3B}"/>
-    <hyperlink ref="D308" r:id="rId198" xr:uid="{EF696095-531A-9B4E-90F5-CA1166C070EB}"/>
-    <hyperlink ref="D309" r:id="rId199" xr:uid="{7319E358-38E8-6D4F-99E9-A558FF1C66D0}"/>
-    <hyperlink ref="D310" r:id="rId200" xr:uid="{C569513C-F920-6148-BB18-A2830C6CABED}"/>
-    <hyperlink ref="D314" r:id="rId201" xr:uid="{4DDCE0DF-C4D6-2F48-850A-FFE8E44529B8}"/>
-    <hyperlink ref="D315" r:id="rId202" xr:uid="{54E4386C-E9E6-5947-8BDF-3BBD841882D1}"/>
-    <hyperlink ref="D316" r:id="rId203" xr:uid="{81F19F2E-83E8-4F41-A52E-63787010CAAE}"/>
-    <hyperlink ref="D317" r:id="rId204" xr:uid="{E0DAEF11-F444-344B-922F-A5AFA19CBDAC}"/>
-    <hyperlink ref="D318" r:id="rId205" xr:uid="{9FD33CD5-F342-BC42-A6B7-5CD2049D8920}"/>
-    <hyperlink ref="D312" r:id="rId206" xr:uid="{9E36AED5-0E4B-A447-9436-6F32633D1396}"/>
-    <hyperlink ref="D319" r:id="rId207" xr:uid="{0288DF9D-25CD-1C4B-A841-A046246E02C3}"/>
-    <hyperlink ref="D320" r:id="rId208" xr:uid="{C9DFAC71-5ACF-204D-8F9A-D4FBACBEA7AA}"/>
-    <hyperlink ref="D104" r:id="rId209" xr:uid="{B4CEFF9C-4149-C147-9750-CA2940A29B5D}"/>
-    <hyperlink ref="D105" r:id="rId210" location="sthash.CLyG4oHQ.dpbs" xr:uid="{785D69EA-E77B-AF48-85EB-249509A6BB77}"/>
-    <hyperlink ref="D85" r:id="rId211" xr:uid="{60A19DED-9CDC-124A-9E44-AA37FD1C44F1}"/>
+    <hyperlink ref="D266" r:id="rId167" xr:uid="{1F55836F-92FB-504B-8890-DD155568B08F}"/>
+    <hyperlink ref="D267" r:id="rId168" xr:uid="{516BA828-1E71-6740-82CE-9ABCB5B2868A}"/>
+    <hyperlink ref="D268" r:id="rId169" xr:uid="{D01BC6DD-63D5-FE45-8701-DE7626C47912}"/>
+    <hyperlink ref="D269" r:id="rId170" xr:uid="{7F25EAA1-3640-2140-8ED9-4C0C8A766B64}"/>
+    <hyperlink ref="D270" r:id="rId171" location="the-ted-williams-tunnel-" xr:uid="{90CDFCE7-A34F-B543-940D-CBD77B3CA490}"/>
+    <hyperlink ref="D274" r:id="rId172" xr:uid="{33076741-07BA-AD48-9CFF-1F8FA7DC794F}"/>
+    <hyperlink ref="D275" r:id="rId173" xr:uid="{E2C2519F-06D0-F54F-A190-1006654C1217}"/>
+    <hyperlink ref="D278" r:id="rId174" xr:uid="{21200567-2A05-1B4A-9286-23765C1B5439}"/>
+    <hyperlink ref="D282" r:id="rId175" xr:uid="{2CD55170-8C56-B640-8914-62FD2B471773}"/>
+    <hyperlink ref="D281" r:id="rId176" xr:uid="{C5C05C21-059D-3E4F-83CE-07DE43CA77F8}"/>
+    <hyperlink ref="D285" r:id="rId177" xr:uid="{5A018FFC-E064-B841-B16C-1B5FDB1C2373}"/>
+    <hyperlink ref="D286" r:id="rId178" xr:uid="{9ECC5CD3-0C49-6241-9ADA-4B8F147F222D}"/>
+    <hyperlink ref="D287" r:id="rId179" xr:uid="{A70D9607-0490-DF4E-85B3-794BEB0DB3CD}"/>
+    <hyperlink ref="D288" r:id="rId180" xr:uid="{7F93E30A-E771-E541-A3E8-E8E115BAC442}"/>
+    <hyperlink ref="D289" r:id="rId181" xr:uid="{DF50B5D9-DAAC-7043-8DA2-3DBF2FCB4882}"/>
+    <hyperlink ref="D271" r:id="rId182" xr:uid="{2930C349-E6B7-544B-BB2A-773A46E73BCB}"/>
+    <hyperlink ref="D256" r:id="rId183" xr:uid="{2BE70040-B75E-144F-8CF2-C6FAF265243F}"/>
+    <hyperlink ref="D293" r:id="rId184" xr:uid="{69A55749-D9D2-1B4B-B3F9-4B160F762593}"/>
+    <hyperlink ref="D294" r:id="rId185" xr:uid="{FB9E4799-0707-754B-9240-DFB8EFCF3420}"/>
+    <hyperlink ref="D295" r:id="rId186" xr:uid="{EFA9A5C9-A935-FD44-A8C3-75A6D42D9D41}"/>
+    <hyperlink ref="D81" r:id="rId187" xr:uid="{18AB1C94-4CE1-2945-92C4-F9826FBC6B4E}"/>
+    <hyperlink ref="D296" r:id="rId188" xr:uid="{6CB68E90-F81E-C748-8D45-EFEEC50C2AE3}"/>
+    <hyperlink ref="D298" r:id="rId189" xr:uid="{8303BB33-5888-964E-8CF2-43DD162804AD}"/>
+    <hyperlink ref="D299" r:id="rId190" xr:uid="{6C92D97F-0A5E-394B-ABB8-0A48B9DDE3CE}"/>
+    <hyperlink ref="D300" r:id="rId191" xr:uid="{A23CD4FA-5C90-8B4F-B42D-8F0581378838}"/>
+    <hyperlink ref="D301" r:id="rId192" xr:uid="{A75CA764-6259-D247-9F3E-71FE84093EEF}"/>
+    <hyperlink ref="D302" r:id="rId193" xr:uid="{4FCB99F2-3FFA-D440-B956-CC2FD50BB76F}"/>
+    <hyperlink ref="D305" r:id="rId194" xr:uid="{936BB4A4-64DC-4640-8D60-262FEB18B51D}"/>
+    <hyperlink ref="D306" r:id="rId195" xr:uid="{09EB0BAC-80EB-3346-AF8B-932BAB3F6F52}"/>
+    <hyperlink ref="D307" r:id="rId196" xr:uid="{249C8010-6579-F842-931C-5A1AA5FFD47E}"/>
+    <hyperlink ref="D308" r:id="rId197" xr:uid="{C11D7F08-A472-D74F-ACD4-DC39321AAA3B}"/>
+    <hyperlink ref="D309" r:id="rId198" xr:uid="{EF696095-531A-9B4E-90F5-CA1166C070EB}"/>
+    <hyperlink ref="D310" r:id="rId199" xr:uid="{7319E358-38E8-6D4F-99E9-A558FF1C66D0}"/>
+    <hyperlink ref="D311" r:id="rId200" xr:uid="{C569513C-F920-6148-BB18-A2830C6CABED}"/>
+    <hyperlink ref="D315" r:id="rId201" xr:uid="{4DDCE0DF-C4D6-2F48-850A-FFE8E44529B8}"/>
+    <hyperlink ref="D316" r:id="rId202" xr:uid="{54E4386C-E9E6-5947-8BDF-3BBD841882D1}"/>
+    <hyperlink ref="D317" r:id="rId203" xr:uid="{81F19F2E-83E8-4F41-A52E-63787010CAAE}"/>
+    <hyperlink ref="D318" r:id="rId204" xr:uid="{E0DAEF11-F444-344B-922F-A5AFA19CBDAC}"/>
+    <hyperlink ref="D319" r:id="rId205" xr:uid="{9FD33CD5-F342-BC42-A6B7-5CD2049D8920}"/>
+    <hyperlink ref="D313" r:id="rId206" xr:uid="{9E36AED5-0E4B-A447-9436-6F32633D1396}"/>
+    <hyperlink ref="D320" r:id="rId207" xr:uid="{0288DF9D-25CD-1C4B-A841-A046246E02C3}"/>
+    <hyperlink ref="D321" r:id="rId208" xr:uid="{C9DFAC71-5ACF-204D-8F9A-D4FBACBEA7AA}"/>
+    <hyperlink ref="D105" r:id="rId209" xr:uid="{B4CEFF9C-4149-C147-9750-CA2940A29B5D}"/>
+    <hyperlink ref="D106" r:id="rId210" location="sthash.CLyG4oHQ.dpbs" xr:uid="{785D69EA-E77B-AF48-85EB-249509A6BB77}"/>
+    <hyperlink ref="D86" r:id="rId211" xr:uid="{60A19DED-9CDC-124A-9E44-AA37FD1C44F1}"/>
     <hyperlink ref="D23" r:id="rId212" xr:uid="{D1664D41-D33B-4949-839C-271243D7F21B}"/>
     <hyperlink ref="D22" r:id="rId213" xr:uid="{48D024A1-76B5-2148-9BA8-76FC5B789C3C}"/>
     <hyperlink ref="D34" r:id="rId214" xr:uid="{69D07C5C-50D8-A34C-B327-372E9737895F}"/>
@@ -7424,21 +7447,21 @@
     <hyperlink ref="D45" r:id="rId216" xr:uid="{6CBB316C-932E-334D-8420-FEA7F2C4D560}"/>
     <hyperlink ref="D48" r:id="rId217" xr:uid="{D5CEEF90-9389-EE4B-8CE9-0C6FA742EA5A}"/>
     <hyperlink ref="D47" r:id="rId218" xr:uid="{E3CDAE9B-8044-F94D-A9D7-1080A2B10492}"/>
-    <hyperlink ref="D210" r:id="rId219" xr:uid="{50F35F4B-BA0B-624A-B5A4-DC53EF5BCCFD}"/>
-    <hyperlink ref="D238" r:id="rId220" xr:uid="{851BBD79-B0B8-6741-ADC7-18BC6CD77F55}"/>
-    <hyperlink ref="D243" r:id="rId221" xr:uid="{8C80B853-2FB6-BA43-8D77-CA9D0A54C7A8}"/>
-    <hyperlink ref="D244" r:id="rId222" xr:uid="{DCAD803E-9B32-AB4D-B77E-56BD769CEADE}"/>
-    <hyperlink ref="D271" r:id="rId223" xr:uid="{E017BD74-051C-A845-9C99-138027F30F1D}"/>
-    <hyperlink ref="D272" r:id="rId224" xr:uid="{4D72A4C4-AD0C-114A-9C48-41FE25C825EB}"/>
-    <hyperlink ref="D276" r:id="rId225" xr:uid="{2E661DC9-EC98-5C47-99FF-DD5BCC222802}"/>
-    <hyperlink ref="D278" r:id="rId226" xr:uid="{7AEE5148-879B-1244-A65C-DF6A183C8993}"/>
-    <hyperlink ref="D279" r:id="rId227" xr:uid="{5D34A7E5-346F-0E41-89CC-2A9B5F277CED}"/>
-    <hyperlink ref="D282" r:id="rId228" xr:uid="{1F7B4ABD-A97B-634D-94AD-CAE2BBAAA501}"/>
-    <hyperlink ref="D283" r:id="rId229" xr:uid="{8DC5E1D5-E8E2-C244-BB87-6B1B882EA7BF}"/>
-    <hyperlink ref="D291" r:id="rId230" xr:uid="{5D7FBCD9-4BE6-8E41-B16C-4AED44F62DAC}"/>
-    <hyperlink ref="D296" r:id="rId231" xr:uid="{2164D655-9D47-8749-A59F-EC0121D2E68B}"/>
-    <hyperlink ref="D302" r:id="rId232" xr:uid="{D0B3FE4C-F121-8C4F-B063-05A222FFB480}"/>
-    <hyperlink ref="D311" r:id="rId233" xr:uid="{47A1D77B-EB49-D14D-9088-F2DE88D7B296}"/>
+    <hyperlink ref="D211" r:id="rId219" xr:uid="{50F35F4B-BA0B-624A-B5A4-DC53EF5BCCFD}"/>
+    <hyperlink ref="D239" r:id="rId220" xr:uid="{851BBD79-B0B8-6741-ADC7-18BC6CD77F55}"/>
+    <hyperlink ref="D244" r:id="rId221" xr:uid="{8C80B853-2FB6-BA43-8D77-CA9D0A54C7A8}"/>
+    <hyperlink ref="D245" r:id="rId222" xr:uid="{DCAD803E-9B32-AB4D-B77E-56BD769CEADE}"/>
+    <hyperlink ref="D272" r:id="rId223" xr:uid="{E017BD74-051C-A845-9C99-138027F30F1D}"/>
+    <hyperlink ref="D273" r:id="rId224" xr:uid="{4D72A4C4-AD0C-114A-9C48-41FE25C825EB}"/>
+    <hyperlink ref="D277" r:id="rId225" xr:uid="{2E661DC9-EC98-5C47-99FF-DD5BCC222802}"/>
+    <hyperlink ref="D279" r:id="rId226" xr:uid="{7AEE5148-879B-1244-A65C-DF6A183C8993}"/>
+    <hyperlink ref="D280" r:id="rId227" xr:uid="{5D34A7E5-346F-0E41-89CC-2A9B5F277CED}"/>
+    <hyperlink ref="D283" r:id="rId228" xr:uid="{1F7B4ABD-A97B-634D-94AD-CAE2BBAAA501}"/>
+    <hyperlink ref="D284" r:id="rId229" xr:uid="{8DC5E1D5-E8E2-C244-BB87-6B1B882EA7BF}"/>
+    <hyperlink ref="D292" r:id="rId230" xr:uid="{5D7FBCD9-4BE6-8E41-B16C-4AED44F62DAC}"/>
+    <hyperlink ref="D297" r:id="rId231" xr:uid="{2164D655-9D47-8749-A59F-EC0121D2E68B}"/>
+    <hyperlink ref="D303" r:id="rId232" xr:uid="{D0B3FE4C-F121-8C4F-B063-05A222FFB480}"/>
+    <hyperlink ref="D312" r:id="rId233" xr:uid="{47A1D77B-EB49-D14D-9088-F2DE88D7B296}"/>
     <hyperlink ref="D2" r:id="rId234" xr:uid="{34F9D20D-FC31-C344-84F9-1028073719B0}"/>
     <hyperlink ref="D3" r:id="rId235" xr:uid="{5AF14D64-BCD2-B14E-B95E-EF64A59D04A2}"/>
     <hyperlink ref="D9" r:id="rId236" xr:uid="{4E4F2327-D5E2-5445-AD29-35676B61B99D}"/>
@@ -7453,45 +7476,46 @@
     <hyperlink ref="D51" r:id="rId245" xr:uid="{E6644601-F4A2-D842-BAF7-944745C6E1FE}"/>
     <hyperlink ref="D58" r:id="rId246" xr:uid="{518D65ED-893E-8B40-93EC-F10F3DECE27C}"/>
     <hyperlink ref="D61" r:id="rId247" xr:uid="{ECFF16B4-C31C-8445-A4D5-B621F848C623}"/>
-    <hyperlink ref="D117" r:id="rId248" xr:uid="{78E49338-E11A-BE46-9436-98D0C4CBE612}"/>
-    <hyperlink ref="D116" r:id="rId249" xr:uid="{CB0B5113-280A-6745-AB5D-3C542D5F0687}"/>
-    <hyperlink ref="D114" r:id="rId250" xr:uid="{0AF1551E-4845-EE4C-AEF2-1C1B5BE33A23}"/>
-    <hyperlink ref="D127" r:id="rId251" xr:uid="{1CEFADA7-B8F9-D944-B3BE-B97F9806AE93}"/>
-    <hyperlink ref="D128" r:id="rId252" xr:uid="{FEB2D05B-9469-3048-B474-790A27338D84}"/>
-    <hyperlink ref="D149" r:id="rId253" xr:uid="{BBDCCEFF-2304-914E-B8AF-301B6E69A0F6}"/>
-    <hyperlink ref="D148" r:id="rId254" xr:uid="{6D6C1A20-E743-C24C-B1EF-66AB85A681F8}"/>
-    <hyperlink ref="D155" r:id="rId255" xr:uid="{49952D50-B854-274E-B075-25872A09FFF2}"/>
-    <hyperlink ref="D153" r:id="rId256" xr:uid="{95987E18-4521-584B-89BB-CD6CC479A43F}"/>
-    <hyperlink ref="D220" r:id="rId257" xr:uid="{3466ECD5-0908-844C-8F01-361E3D467004}"/>
-    <hyperlink ref="D221" r:id="rId258" xr:uid="{890DC3AF-E6F6-CB44-8C49-1ADF75727656}"/>
-    <hyperlink ref="D222" r:id="rId259" xr:uid="{D2F44FA3-F4FD-FC46-A7BC-A13E2C98DAA7}"/>
-    <hyperlink ref="D224" r:id="rId260" xr:uid="{5E66DDE0-516E-A844-844B-E429227B744A}"/>
-    <hyperlink ref="D225" r:id="rId261" xr:uid="{3E616B3D-EF94-F740-99C3-14D3F74641B5}"/>
-    <hyperlink ref="D226" r:id="rId262" xr:uid="{A49956B5-22E5-584E-81F2-74351DDA9CA4}"/>
-    <hyperlink ref="D227" r:id="rId263" xr:uid="{964BC9E3-33DE-8A45-A898-F579F6C96B50}"/>
-    <hyperlink ref="D228" r:id="rId264" xr:uid="{9A5B45A3-E69A-A24D-A65E-F096B559F4D0}"/>
-    <hyperlink ref="D156" r:id="rId265" xr:uid="{B15D867D-3308-9246-A4EA-4808AC4BE276}"/>
-    <hyperlink ref="D163" r:id="rId266" xr:uid="{BDDAF2F9-5060-C645-ADF6-E8B4AE8D9F21}"/>
-    <hyperlink ref="D147" r:id="rId267" xr:uid="{E7E8F9AA-6410-2446-9EDB-35B487642AB4}"/>
-    <hyperlink ref="D146" r:id="rId268" xr:uid="{50AFC520-0BC0-9940-9530-57493CFFEE9E}"/>
-    <hyperlink ref="D65" r:id="rId269" xr:uid="{24265432-4427-CC45-BD00-6954D542D98E}"/>
-    <hyperlink ref="D160" r:id="rId270" xr:uid="{13C83452-5D80-4D4D-9809-7D4EB289B3E0}"/>
-    <hyperlink ref="D161" r:id="rId271" xr:uid="{C11E50A9-9298-2447-9615-93AF182DED39}"/>
-    <hyperlink ref="D162" r:id="rId272" xr:uid="{804DD6E2-158E-6948-B8FE-24248E381935}"/>
-    <hyperlink ref="D141" r:id="rId273" xr:uid="{93246BB1-F4EB-8248-A367-1EEB230F54CD}"/>
-    <hyperlink ref="D139" r:id="rId274" xr:uid="{F4D3B5EE-9DA2-5E44-9B97-1716680A2A98}"/>
-    <hyperlink ref="D145" r:id="rId275" xr:uid="{874DD896-8AE3-4544-B402-517E0CE5538A}"/>
-    <hyperlink ref="D143" r:id="rId276" xr:uid="{131DA2DA-C659-184F-A2E2-DED984EFF9F2}"/>
-    <hyperlink ref="D202" r:id="rId277" xr:uid="{0BBA263E-DF5D-C04A-B0AE-54E68EA17727}"/>
-    <hyperlink ref="D237" r:id="rId278" xr:uid="{8CBEE6BC-1A1B-3C44-81EB-B467460A4D3D}"/>
-    <hyperlink ref="D289" r:id="rId279" xr:uid="{03CF96D1-AB9C-5544-8333-B3B3DEE35CED}"/>
-    <hyperlink ref="D290" r:id="rId280" xr:uid="{7D0B6149-73B8-2649-A2D4-B40EBE59C5D0}"/>
-    <hyperlink ref="D303" r:id="rId281" xr:uid="{CEA15DA5-CC23-A847-ABD8-07B73CA1E52F}"/>
-    <hyperlink ref="D259" r:id="rId282" xr:uid="{517DC8DE-0AF7-3045-A1E8-1A6460F60813}"/>
-    <hyperlink ref="D264" r:id="rId283" xr:uid="{29DC1A21-0CD1-7B4E-893F-19D32E977C1B}"/>
-    <hyperlink ref="D89" r:id="rId284" xr:uid="{72A2BFE4-23C5-E442-A8F0-0378379CCCEB}"/>
+    <hyperlink ref="D118" r:id="rId248" xr:uid="{78E49338-E11A-BE46-9436-98D0C4CBE612}"/>
+    <hyperlink ref="D117" r:id="rId249" xr:uid="{CB0B5113-280A-6745-AB5D-3C542D5F0687}"/>
+    <hyperlink ref="D115" r:id="rId250" xr:uid="{0AF1551E-4845-EE4C-AEF2-1C1B5BE33A23}"/>
+    <hyperlink ref="D128" r:id="rId251" xr:uid="{1CEFADA7-B8F9-D944-B3BE-B97F9806AE93}"/>
+    <hyperlink ref="D129" r:id="rId252" xr:uid="{FEB2D05B-9469-3048-B474-790A27338D84}"/>
+    <hyperlink ref="D150" r:id="rId253" xr:uid="{BBDCCEFF-2304-914E-B8AF-301B6E69A0F6}"/>
+    <hyperlink ref="D149" r:id="rId254" xr:uid="{6D6C1A20-E743-C24C-B1EF-66AB85A681F8}"/>
+    <hyperlink ref="D156" r:id="rId255" xr:uid="{49952D50-B854-274E-B075-25872A09FFF2}"/>
+    <hyperlink ref="D154" r:id="rId256" xr:uid="{95987E18-4521-584B-89BB-CD6CC479A43F}"/>
+    <hyperlink ref="D221" r:id="rId257" xr:uid="{3466ECD5-0908-844C-8F01-361E3D467004}"/>
+    <hyperlink ref="D222" r:id="rId258" xr:uid="{890DC3AF-E6F6-CB44-8C49-1ADF75727656}"/>
+    <hyperlink ref="D223" r:id="rId259" xr:uid="{D2F44FA3-F4FD-FC46-A7BC-A13E2C98DAA7}"/>
+    <hyperlink ref="D225" r:id="rId260" xr:uid="{5E66DDE0-516E-A844-844B-E429227B744A}"/>
+    <hyperlink ref="D226" r:id="rId261" xr:uid="{3E616B3D-EF94-F740-99C3-14D3F74641B5}"/>
+    <hyperlink ref="D227" r:id="rId262" xr:uid="{A49956B5-22E5-584E-81F2-74351DDA9CA4}"/>
+    <hyperlink ref="D228" r:id="rId263" xr:uid="{964BC9E3-33DE-8A45-A898-F579F6C96B50}"/>
+    <hyperlink ref="D229" r:id="rId264" xr:uid="{9A5B45A3-E69A-A24D-A65E-F096B559F4D0}"/>
+    <hyperlink ref="D157" r:id="rId265" xr:uid="{B15D867D-3308-9246-A4EA-4808AC4BE276}"/>
+    <hyperlink ref="D164" r:id="rId266" xr:uid="{BDDAF2F9-5060-C645-ADF6-E8B4AE8D9F21}"/>
+    <hyperlink ref="D148" r:id="rId267" xr:uid="{E7E8F9AA-6410-2446-9EDB-35B487642AB4}"/>
+    <hyperlink ref="D147" r:id="rId268" xr:uid="{50AFC520-0BC0-9940-9530-57493CFFEE9E}"/>
+    <hyperlink ref="D66" r:id="rId269" xr:uid="{24265432-4427-CC45-BD00-6954D542D98E}"/>
+    <hyperlink ref="D161" r:id="rId270" xr:uid="{13C83452-5D80-4D4D-9809-7D4EB289B3E0}"/>
+    <hyperlink ref="D162" r:id="rId271" xr:uid="{C11E50A9-9298-2447-9615-93AF182DED39}"/>
+    <hyperlink ref="D163" r:id="rId272" xr:uid="{804DD6E2-158E-6948-B8FE-24248E381935}"/>
+    <hyperlink ref="D142" r:id="rId273" xr:uid="{93246BB1-F4EB-8248-A367-1EEB230F54CD}"/>
+    <hyperlink ref="D140" r:id="rId274" xr:uid="{F4D3B5EE-9DA2-5E44-9B97-1716680A2A98}"/>
+    <hyperlink ref="D146" r:id="rId275" xr:uid="{874DD896-8AE3-4544-B402-517E0CE5538A}"/>
+    <hyperlink ref="D144" r:id="rId276" xr:uid="{131DA2DA-C659-184F-A2E2-DED984EFF9F2}"/>
+    <hyperlink ref="D203" r:id="rId277" xr:uid="{0BBA263E-DF5D-C04A-B0AE-54E68EA17727}"/>
+    <hyperlink ref="D238" r:id="rId278" xr:uid="{8CBEE6BC-1A1B-3C44-81EB-B467460A4D3D}"/>
+    <hyperlink ref="D290" r:id="rId279" xr:uid="{03CF96D1-AB9C-5544-8333-B3B3DEE35CED}"/>
+    <hyperlink ref="D291" r:id="rId280" xr:uid="{7D0B6149-73B8-2649-A2D4-B40EBE59C5D0}"/>
+    <hyperlink ref="D304" r:id="rId281" xr:uid="{CEA15DA5-CC23-A847-ABD8-07B73CA1E52F}"/>
+    <hyperlink ref="D260" r:id="rId282" xr:uid="{517DC8DE-0AF7-3045-A1E8-1A6460F60813}"/>
+    <hyperlink ref="D265" r:id="rId283" xr:uid="{29DC1A21-0CD1-7B4E-893F-19D32E977C1B}"/>
+    <hyperlink ref="D90" r:id="rId284" xr:uid="{72A2BFE4-23C5-E442-A8F0-0378379CCCEB}"/>
+    <hyperlink ref="D63" r:id="rId285" xr:uid="{4EF910E4-3EF4-C94E-AF22-6F0BCA9FADAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId285"/>
+  <pageSetup orientation="portrait" r:id="rId286"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Used HTML entity &hyphen; in 1973 'Coordinated Public Transit-Human Services' line.
</commit_message>
<xml_diff>
--- a/xlsx/timeline_links.xlsx
+++ b/xlsx/timeline_links.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\www\apps\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75A4679-11F5-4A57-94F8-0EDC11638C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1338,13 +1337,13 @@
     <t>http://www.bostonstreetcars.com/what-happened-to-the-a-line.html</t>
   </si>
   <si>
-    <t>Coordinated Public Transit-Human Services Transportation Plan</t>
+    <t>Coordinated Public Transit&amp;hyphen;Human Services Transportation Plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1755,11 +1754,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+    <sheetView tabSelected="1" topLeftCell="A207" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7229,291 +7228,291 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{DC368A89-F50A-2B4A-9193-ECD353823943}"/>
-    <hyperlink ref="D12" r:id="rId2" xr:uid="{A158D117-680A-3946-B33F-DFC7615EAB47}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{34FA00CB-819B-F843-AD96-08AB15DF6279}"/>
-    <hyperlink ref="D21" r:id="rId4" xr:uid="{ECFB6FD7-DCC2-0E44-9796-8241FDCCFD84}"/>
-    <hyperlink ref="D20" r:id="rId5" xr:uid="{98EF227F-9082-AA44-AF84-D1CCBBADC8D3}"/>
-    <hyperlink ref="D26" r:id="rId6" xr:uid="{9F1E5346-5C17-BC4D-AF99-1A167F2649B0}"/>
-    <hyperlink ref="D18" r:id="rId7" xr:uid="{BDB15F6B-18EC-3D49-8B72-5137504EF871}"/>
-    <hyperlink ref="D28" r:id="rId8" xr:uid="{6DB67EDD-7E6F-7C4C-ABE1-490A692D4EC1}"/>
-    <hyperlink ref="D29" r:id="rId9" xr:uid="{035B09D4-522D-B944-A866-40A97904064A}"/>
-    <hyperlink ref="D30" r:id="rId10" xr:uid="{03623A48-C19F-8E41-8391-0959682C7481}"/>
-    <hyperlink ref="D32" r:id="rId11" xr:uid="{0D27B085-1280-6942-AC4E-7441347F39C9}"/>
-    <hyperlink ref="D36" r:id="rId12" xr:uid="{DAD721BA-F1E3-8A44-80A7-6024D1018106}"/>
-    <hyperlink ref="D37" r:id="rId13" xr:uid="{D188C94E-96C7-C642-B9AB-369D11836279}"/>
-    <hyperlink ref="D41" r:id="rId14" xr:uid="{58E7FE4B-F168-244B-9CCF-D09EC5EAFD7F}"/>
-    <hyperlink ref="D35" r:id="rId15" xr:uid="{513FE09A-2DAA-5A48-837C-1E64EB4C9DCD}"/>
-    <hyperlink ref="D54" r:id="rId16" xr:uid="{ABC9D923-DD67-FD42-84B8-4D9EA508C329}"/>
-    <hyperlink ref="D55" r:id="rId17" xr:uid="{D01A08EB-5993-564D-BEBB-DB263701B05F}"/>
-    <hyperlink ref="D44" r:id="rId18" xr:uid="{7AD60CA3-1531-0F43-9206-D9BB3D1F9D93}"/>
-    <hyperlink ref="D60" r:id="rId19" xr:uid="{F597C50B-1112-5646-ADB0-C72EDC488C7D}"/>
-    <hyperlink ref="D62" r:id="rId20" xr:uid="{3F62B3B8-D447-954A-8E0B-70BECA5447EE}"/>
-    <hyperlink ref="D17" r:id="rId21" xr:uid="{EE3BB206-C0D2-EB4F-AA70-7C0FFFCCBA5F}"/>
-    <hyperlink ref="D68" r:id="rId22" xr:uid="{B0482045-53D9-474D-B70B-423E86B4B9CE}"/>
-    <hyperlink ref="D19" r:id="rId23" xr:uid="{AE3F6E1A-176D-9149-B043-D776733464AB}"/>
-    <hyperlink ref="D6" r:id="rId24" xr:uid="{4FAAA4DD-C614-D942-8C81-16828DF82F2B}"/>
-    <hyperlink ref="D14" r:id="rId25" xr:uid="{393F2075-4A9E-0B47-92DA-FF28CD1D6999}"/>
-    <hyperlink ref="D16" r:id="rId26" xr:uid="{BCFB6456-8280-6147-8A46-F2D299EFD3BA}"/>
-    <hyperlink ref="D46" r:id="rId27" xr:uid="{A5D390C1-08EE-5649-962C-A440D29BA445}"/>
-    <hyperlink ref="D56" r:id="rId28" xr:uid="{329EF611-EF9C-FC4A-9988-9666121DABCD}"/>
-    <hyperlink ref="D57" r:id="rId29" xr:uid="{09ABDBF1-B54C-604F-A17B-446CBE1A2A2C}"/>
-    <hyperlink ref="D59" r:id="rId30" xr:uid="{96D60956-D26C-CC4C-B361-C31419E06692}"/>
-    <hyperlink ref="D70" r:id="rId31" xr:uid="{90EBC071-E84D-4549-A9CE-645045A70E75}"/>
-    <hyperlink ref="D71" r:id="rId32" xr:uid="{E731DF72-6E9F-0240-B2A4-95E82B8C938A}"/>
-    <hyperlink ref="D74" r:id="rId33" xr:uid="{5391EFF3-6DAD-4E40-9C66-C7501F2ABF1B}"/>
-    <hyperlink ref="D75" r:id="rId34" xr:uid="{EBCA5E87-62CD-FD46-9F99-E2FD5D3229F6}"/>
-    <hyperlink ref="D77" r:id="rId35" xr:uid="{5DFE6518-BD4D-4549-AB00-0EE49338D457}"/>
-    <hyperlink ref="D78" r:id="rId36" xr:uid="{9B51E31E-B1C5-8D4D-81F2-CE7E5FEFD734}"/>
-    <hyperlink ref="D79" r:id="rId37" xr:uid="{0294F04A-3FAD-0B4A-B3C5-136B9BFEB9ED}"/>
-    <hyperlink ref="D80" r:id="rId38" xr:uid="{E304CDD0-F736-9840-B873-3814D3979A08}"/>
-    <hyperlink ref="D82" r:id="rId39" xr:uid="{7F1EFF99-583A-6B4D-A3EB-824895A98C6F}"/>
-    <hyperlink ref="D85" r:id="rId40" xr:uid="{F3A77ECC-804C-1E44-94A7-51411C449BA3}"/>
-    <hyperlink ref="D83" r:id="rId41" xr:uid="{A3CF8173-1ABB-874D-AFE8-C0816C3C4A29}"/>
-    <hyperlink ref="D89" r:id="rId42" xr:uid="{42481CE0-DCAC-7347-A21F-7C04B44C6492}"/>
-    <hyperlink ref="D91" r:id="rId43" xr:uid="{8B79ADB7-F134-A54C-8A6F-8029C920BB98}"/>
-    <hyperlink ref="D94" r:id="rId44" xr:uid="{0F29D32C-0E67-F248-8C35-9710D68A7F85}"/>
-    <hyperlink ref="D95" r:id="rId45" xr:uid="{BA71FBDC-01A3-4A48-BCA0-1C6E4893F910}"/>
-    <hyperlink ref="D76" r:id="rId46" xr:uid="{9995D19A-7C18-FD4A-B802-9520BA771167}"/>
-    <hyperlink ref="D97" r:id="rId47" xr:uid="{304009F6-D9B7-CA4A-8889-BE080E8A7654}"/>
-    <hyperlink ref="D98" r:id="rId48" xr:uid="{4795B6FC-18EE-9043-8CE7-AF2924E6749D}"/>
-    <hyperlink ref="D100" r:id="rId49" xr:uid="{D578DF58-1254-4444-A5AA-946137A0D551}"/>
-    <hyperlink ref="D101" r:id="rId50" xr:uid="{18921900-3790-4748-9B02-AE7CF2E83568}"/>
-    <hyperlink ref="D99" r:id="rId51" xr:uid="{86F5F152-3AE3-C84D-9FFC-1DEDBE048190}"/>
-    <hyperlink ref="D107" r:id="rId52" xr:uid="{AD61CAC4-24BC-954B-A0DF-1642FA6C333B}"/>
-    <hyperlink ref="D102" r:id="rId53" xr:uid="{D07E7B17-1A5D-4544-BA76-5313EC783C1A}"/>
-    <hyperlink ref="D84" r:id="rId54" xr:uid="{A15B0F1F-A780-1F46-B188-D9ABDB5704B5}"/>
-    <hyperlink ref="D103" r:id="rId55" xr:uid="{979D158A-596F-9A47-AB5E-A72097511FA1}"/>
-    <hyperlink ref="D72" r:id="rId56" xr:uid="{A15BE685-A40C-734C-AD72-47F9BF601FDA}"/>
-    <hyperlink ref="D88" r:id="rId57" xr:uid="{FB025A70-6F06-4E4E-8984-BA9B9A2AF297}"/>
-    <hyperlink ref="D87" r:id="rId58" xr:uid="{1E58D491-53C2-2A42-A667-CC2FC0000945}"/>
-    <hyperlink ref="D108" r:id="rId59" xr:uid="{3ACCDC43-EF65-2A4A-A85E-EAF5CBC58797}"/>
-    <hyperlink ref="D109" r:id="rId60" xr:uid="{25D4D054-F5CD-6342-9DEC-8930BA66BE1A}"/>
-    <hyperlink ref="D110" r:id="rId61" xr:uid="{8CCF119F-F952-D34D-AF8C-DFB4362DB485}"/>
-    <hyperlink ref="D111" r:id="rId62" xr:uid="{54F9A12F-EE15-FF41-AC0A-F0A2DEAF65D5}"/>
-    <hyperlink ref="D120" r:id="rId63" xr:uid="{A324DF56-4206-4746-9CDE-46BC8817E2EB}"/>
-    <hyperlink ref="D121" r:id="rId64" xr:uid="{F809319C-4A84-3B46-A615-A43A53515FA1}"/>
-    <hyperlink ref="D122" r:id="rId65" xr:uid="{331E1E74-43DD-8B44-BF01-87A292B96D3E}"/>
-    <hyperlink ref="D124" r:id="rId66" xr:uid="{0450769E-D191-D142-8255-A056AD20F92E}"/>
-    <hyperlink ref="D64" r:id="rId67" xr:uid="{877003D4-412B-1C4A-B9C5-07DF56DA7218}"/>
-    <hyperlink ref="D65" r:id="rId68" xr:uid="{BF399E5E-1ECA-414D-A2D4-57E85D27B367}"/>
-    <hyperlink ref="D126" r:id="rId69" xr:uid="{BB764D03-6EBC-9C46-ACF7-5FD301EB57E9}"/>
-    <hyperlink ref="D127" r:id="rId70" xr:uid="{E0E6E7A9-4B34-9D48-B226-2529539960C3}"/>
-    <hyperlink ref="D130" r:id="rId71" xr:uid="{EE01CD31-A0CC-FB4E-9234-D39DC44BBEF2}"/>
-    <hyperlink ref="D131" r:id="rId72" xr:uid="{3C47FF5A-BE3C-7C4E-829E-4945618A9C1F}"/>
-    <hyperlink ref="D132" r:id="rId73" xr:uid="{F5493FE6-0313-1940-AEFF-050A934E8083}"/>
-    <hyperlink ref="D133" r:id="rId74" xr:uid="{F415321A-3F49-EB4E-B6A9-EFE163590B41}"/>
-    <hyperlink ref="D134" r:id="rId75" xr:uid="{C84C6E00-5661-0D49-A0D1-CFD70865A82D}"/>
-    <hyperlink ref="D135" r:id="rId76" xr:uid="{E23DB724-160F-8543-B648-70EB7CA0365F}"/>
-    <hyperlink ref="D136" r:id="rId77" xr:uid="{E29FA1EF-7AB7-E245-832F-7B087D0E7EA3}"/>
-    <hyperlink ref="D137" r:id="rId78" xr:uid="{388C4274-E38A-B449-8F40-7ED095B192D7}"/>
-    <hyperlink ref="D138" r:id="rId79" xr:uid="{A966469C-688F-1E4F-8C89-F7E400609830}"/>
-    <hyperlink ref="D151" r:id="rId80" xr:uid="{B7708F6B-F6E6-BF41-8AF3-54C00F11C52B}"/>
-    <hyperlink ref="D159" r:id="rId81" xr:uid="{BF7922F0-DD27-EE45-AF85-5C9161DA389C}"/>
-    <hyperlink ref="D160" r:id="rId82" xr:uid="{BC00976C-C73B-6F4E-B032-65F2D572F141}"/>
-    <hyperlink ref="D165" r:id="rId83" xr:uid="{77C86A54-F6B8-BA40-A768-CCB7D4C99562}"/>
-    <hyperlink ref="D166" r:id="rId84" xr:uid="{CAB158A3-D761-8448-A767-9525660B6326}"/>
-    <hyperlink ref="D167" r:id="rId85" xr:uid="{34BE3A49-BE9D-4049-97A0-80E02A01A961}"/>
-    <hyperlink ref="D152" r:id="rId86" xr:uid="{781FF30D-914F-7841-92BF-6AD62300904B}"/>
-    <hyperlink ref="D158" r:id="rId87" xr:uid="{3CBAAA26-1E37-B044-B755-258229968E67}"/>
-    <hyperlink ref="D168" r:id="rId88" xr:uid="{DCC7B2BC-EB59-DB49-9BF9-45BF0E030221}"/>
-    <hyperlink ref="D169" r:id="rId89" xr:uid="{22C8D3B5-CBB9-C448-83B5-05CE9F72E696}"/>
-    <hyperlink ref="D170" r:id="rId90" xr:uid="{A3C5359E-186C-1640-839A-F7F1B599F0B5}"/>
-    <hyperlink ref="D171" r:id="rId91" xr:uid="{CD78268C-7DEC-FB44-88AA-75EC6DE77C62}"/>
-    <hyperlink ref="D172" r:id="rId92" xr:uid="{5BC45F49-43E2-5D46-B9F7-C9DE4586524D}"/>
-    <hyperlink ref="D173" r:id="rId93" xr:uid="{3B77FB2E-5F37-D04A-B1B0-08D6A165225B}"/>
-    <hyperlink ref="D174" r:id="rId94" xr:uid="{6EA4E64A-6FFB-FC43-A3F9-B515DC03D9ED}"/>
-    <hyperlink ref="D175" r:id="rId95" xr:uid="{7D0BC227-6BA4-F747-B1DB-B7CCF5D3057E}"/>
-    <hyperlink ref="D176" r:id="rId96" xr:uid="{19FE4A6D-FF5E-BF49-8C4B-F24B3005865C}"/>
-    <hyperlink ref="D177" r:id="rId97" xr:uid="{41D1D3F0-3B5D-964A-BC98-E26309342AC6}"/>
-    <hyperlink ref="D179" r:id="rId98" xr:uid="{C852E2F0-FC27-4F41-89CD-E264B7CB2DF7}"/>
-    <hyperlink ref="D180" r:id="rId99" xr:uid="{DF3B379B-CACF-954D-AEAA-0FF3E835924A}"/>
-    <hyperlink ref="D181" r:id="rId100" xr:uid="{7FADB0C5-8AA0-6F41-A92E-5B09572E4D18}"/>
-    <hyperlink ref="D182" r:id="rId101" xr:uid="{3103A3F7-AC33-1C4E-BCE8-2934FE92BC5F}"/>
-    <hyperlink ref="D183" r:id="rId102" xr:uid="{07DF88EF-4EAA-1440-8D82-60A0FD7CADD1}"/>
-    <hyperlink ref="D184" r:id="rId103" xr:uid="{E19890F5-0215-4644-AEA1-BF7692385DF1}"/>
-    <hyperlink ref="D185" r:id="rId104" xr:uid="{86B64C9A-DAFF-CF44-A151-29AA7D14977F}"/>
-    <hyperlink ref="D186" r:id="rId105" xr:uid="{3FEFD335-04F9-4F41-B6A0-B080D6550649}"/>
-    <hyperlink ref="D187" r:id="rId106" xr:uid="{90B99E7F-0693-D54F-A4F6-34AD69A3D631}"/>
-    <hyperlink ref="D188" r:id="rId107" xr:uid="{B95F960A-6D1F-2D47-8457-F9DE115B5C38}"/>
-    <hyperlink ref="D189" r:id="rId108" xr:uid="{00ECE393-EC26-344F-8B40-377C3EB5D890}"/>
-    <hyperlink ref="D190" r:id="rId109" xr:uid="{C28E61A4-8435-BF4D-8BA4-7A3647FBFF00}"/>
-    <hyperlink ref="D191" r:id="rId110" xr:uid="{3CAEF1A6-A029-A64D-903F-EB0ADFF46D37}"/>
-    <hyperlink ref="D192" r:id="rId111" xr:uid="{9DF090F0-97A2-E946-850D-1ECC6DB92707}"/>
-    <hyperlink ref="D193" r:id="rId112" xr:uid="{C85A63BA-1F71-584A-A604-B6AB345ECE95}"/>
-    <hyperlink ref="D93" r:id="rId113" xr:uid="{2F59B8F2-7AB0-AE47-85CD-C244BB59B3BA}"/>
-    <hyperlink ref="D194" r:id="rId114" xr:uid="{06DC547A-085D-7C45-A4F0-49F7349DAAB0}"/>
-    <hyperlink ref="D195" r:id="rId115" xr:uid="{D65368D6-C0A7-5B4C-83C0-4DFB768DE3C6}"/>
-    <hyperlink ref="D196" r:id="rId116" xr:uid="{B7606443-1D1E-724A-8040-131FD0AC6338}"/>
-    <hyperlink ref="D197" r:id="rId117" xr:uid="{79B43F1F-03A0-F747-AC05-79F3D0B4BCCB}"/>
-    <hyperlink ref="D198" r:id="rId118" xr:uid="{875EF5F0-7651-8745-87D6-636AD559D72E}"/>
-    <hyperlink ref="D199" r:id="rId119" xr:uid="{6E4DCDAE-D012-BD4D-A394-90B249BB99C5}"/>
-    <hyperlink ref="D200" r:id="rId120" xr:uid="{3DAD8E8C-E2BB-074B-B3F0-D475C7FD6B2D}"/>
-    <hyperlink ref="D201" r:id="rId121" xr:uid="{222D21AE-1088-BD48-BAEE-1EF3912460AF}"/>
-    <hyperlink ref="D202" r:id="rId122" xr:uid="{7AD5FFD0-8F45-1941-9BBF-D91BBC4F0F40}"/>
-    <hyperlink ref="D204" r:id="rId123" xr:uid="{518258DC-5A20-3D40-91D0-D032DC42B6AD}"/>
-    <hyperlink ref="D205" r:id="rId124" xr:uid="{5B069AF2-81F6-A34E-80A0-7E8EBE3DFA2A}"/>
-    <hyperlink ref="D206" r:id="rId125" xr:uid="{A04E8385-1CE9-364E-91A1-6F09D76ACF42}"/>
-    <hyperlink ref="D207" r:id="rId126" xr:uid="{3113EFF0-EE9A-354C-8BD1-5D9364B99893}"/>
-    <hyperlink ref="D208" r:id="rId127" xr:uid="{A06F9F88-431E-574D-92C0-E68077FC529D}"/>
-    <hyperlink ref="D209" r:id="rId128" xr:uid="{8B4EF43A-AE24-6947-8EFA-E38936068D18}"/>
-    <hyperlink ref="C210" r:id="rId129" display="https://www.bostonmpo.org/node/3243" xr:uid="{655CEEAA-6095-9B47-995E-CD64750746E0}"/>
-    <hyperlink ref="D210" r:id="rId130" xr:uid="{055A514B-7345-F948-9754-CCC9031C0081}"/>
-    <hyperlink ref="D212" r:id="rId131" xr:uid="{90B28A53-CDAB-EC48-9FC0-0E277128FCA7}"/>
-    <hyperlink ref="D213" r:id="rId132" xr:uid="{AC529FF5-CF2C-1D4B-95AB-70ED1909D783}"/>
-    <hyperlink ref="D214" r:id="rId133" xr:uid="{ECE456D6-90BA-E547-8B10-93E537F7BF40}"/>
-    <hyperlink ref="D215" r:id="rId134" xr:uid="{2686E174-B756-124D-82F8-89B4FFA6EE04}"/>
-    <hyperlink ref="D216" r:id="rId135" xr:uid="{F529B5BA-08ED-3642-9481-1E3CCADBB5B4}"/>
-    <hyperlink ref="D217" r:id="rId136" xr:uid="{0D583AB0-0EC1-4143-9730-B654F3258218}"/>
-    <hyperlink ref="D218" r:id="rId137" xr:uid="{D3776250-774B-AB40-A8B2-B7A3B3F11494}"/>
-    <hyperlink ref="D219" r:id="rId138" xr:uid="{816B8DD7-C959-7845-A7B3-E11200634DE3}"/>
-    <hyperlink ref="D230" r:id="rId139" xr:uid="{8E6DE810-4336-264A-9286-F5DE4FCB3616}"/>
-    <hyperlink ref="D231" r:id="rId140" xr:uid="{74958D82-AE52-764E-A4F1-2CBA9EA9ACED}"/>
-    <hyperlink ref="D232" r:id="rId141" xr:uid="{4C8C770A-DBF9-8447-AF54-9001929EDD34}"/>
-    <hyperlink ref="D233" r:id="rId142" xr:uid="{263568FF-4DC1-A245-B266-0B8D89A595BD}"/>
-    <hyperlink ref="D234" r:id="rId143" xr:uid="{0BB8C344-5E31-7E4A-927C-AF47B71575BB}"/>
-    <hyperlink ref="D236" r:id="rId144" xr:uid="{903A7E98-5E9D-544C-B0B8-8E7D2C9D47EB}"/>
-    <hyperlink ref="D53" r:id="rId145" xr:uid="{2690B48D-BA39-6543-BD43-72740F6D06FB}"/>
-    <hyperlink ref="D237" r:id="rId146" xr:uid="{CA43EE9E-6054-8246-8F09-73619591E4D8}"/>
-    <hyperlink ref="D241" r:id="rId147" xr:uid="{5BBBF668-7181-034B-A7E7-B37F0489798D}"/>
-    <hyperlink ref="D242" r:id="rId148" xr:uid="{F25E9123-06C3-4D48-8368-7DC4D8ADFDFE}"/>
-    <hyperlink ref="D247" r:id="rId149" xr:uid="{FE44C4D8-FAA2-6C4A-A061-1E08E9AF9BAE}"/>
-    <hyperlink ref="D248" r:id="rId150" xr:uid="{4A0071B2-48C3-F840-B489-A422B212DF05}"/>
-    <hyperlink ref="D249" r:id="rId151" xr:uid="{0BD877BC-868A-5E4A-987A-4883C51D584C}"/>
-    <hyperlink ref="D251" r:id="rId152" xr:uid="{F7F59C8F-6228-3744-8DF6-9F3A5D6E4A08}"/>
-    <hyperlink ref="D252" r:id="rId153" xr:uid="{8156E09C-4D4B-844F-9152-763F5CBB848C}"/>
-    <hyperlink ref="D253" r:id="rId154" xr:uid="{D66FD1BC-2A48-1D44-9C56-A2091EA6EB4F}"/>
-    <hyperlink ref="D254" r:id="rId155" xr:uid="{EED901F1-9FA7-0241-A3A8-1DEC4ADB4F65}"/>
-    <hyperlink ref="D250" r:id="rId156" xr:uid="{ACBAEB0F-A745-BD4B-A79F-28E87E3B7670}"/>
-    <hyperlink ref="D243" r:id="rId157" xr:uid="{6FE5FEA9-69D3-5B44-8339-E00169C80FE7}"/>
-    <hyperlink ref="D255" r:id="rId158" xr:uid="{4E39217A-DB80-A04A-A66F-DC478E8BD9B0}"/>
-    <hyperlink ref="D257" r:id="rId159" xr:uid="{FD84BB06-83F9-8145-B29B-E82DD0A255FA}"/>
-    <hyperlink ref="D258" r:id="rId160" xr:uid="{0F664415-A56C-5944-BD33-2BBC535C69EE}"/>
-    <hyperlink ref="D259" r:id="rId161" xr:uid="{1B9FDFCF-CDAA-B043-90DF-464B3F19D029}"/>
-    <hyperlink ref="D261" r:id="rId162" xr:uid="{87374CD1-533B-1843-AFD1-A46E4CCC2786}"/>
-    <hyperlink ref="D262" r:id="rId163" xr:uid="{735892DA-3CF9-7D43-938E-C539C1354F7E}"/>
-    <hyperlink ref="D263" r:id="rId164" xr:uid="{25B8E5AB-DD5E-B943-A89D-CF3BCFD8C69D}"/>
-    <hyperlink ref="D264" r:id="rId165" xr:uid="{863254B5-D467-6A40-9BF8-0E3F61B42855}"/>
-    <hyperlink ref="D52" r:id="rId166" xr:uid="{70051547-7009-DA49-AD8A-CDA173903436}"/>
-    <hyperlink ref="D266" r:id="rId167" xr:uid="{1F55836F-92FB-504B-8890-DD155568B08F}"/>
-    <hyperlink ref="D267" r:id="rId168" xr:uid="{516BA828-1E71-6740-82CE-9ABCB5B2868A}"/>
-    <hyperlink ref="D268" r:id="rId169" xr:uid="{D01BC6DD-63D5-FE45-8701-DE7626C47912}"/>
-    <hyperlink ref="D269" r:id="rId170" xr:uid="{7F25EAA1-3640-2140-8ED9-4C0C8A766B64}"/>
-    <hyperlink ref="D270" r:id="rId171" location="the-ted-williams-tunnel-" xr:uid="{90CDFCE7-A34F-B543-940D-CBD77B3CA490}"/>
-    <hyperlink ref="D274" r:id="rId172" xr:uid="{33076741-07BA-AD48-9CFF-1F8FA7DC794F}"/>
-    <hyperlink ref="D275" r:id="rId173" xr:uid="{E2C2519F-06D0-F54F-A190-1006654C1217}"/>
-    <hyperlink ref="D278" r:id="rId174" xr:uid="{21200567-2A05-1B4A-9286-23765C1B5439}"/>
-    <hyperlink ref="D282" r:id="rId175" xr:uid="{2CD55170-8C56-B640-8914-62FD2B471773}"/>
-    <hyperlink ref="D281" r:id="rId176" xr:uid="{C5C05C21-059D-3E4F-83CE-07DE43CA77F8}"/>
-    <hyperlink ref="D285" r:id="rId177" xr:uid="{5A018FFC-E064-B841-B16C-1B5FDB1C2373}"/>
-    <hyperlink ref="D286" r:id="rId178" xr:uid="{9ECC5CD3-0C49-6241-9ADA-4B8F147F222D}"/>
-    <hyperlink ref="D287" r:id="rId179" xr:uid="{A70D9607-0490-DF4E-85B3-794BEB0DB3CD}"/>
-    <hyperlink ref="D288" r:id="rId180" xr:uid="{7F93E30A-E771-E541-A3E8-E8E115BAC442}"/>
-    <hyperlink ref="D289" r:id="rId181" xr:uid="{DF50B5D9-DAAC-7043-8DA2-3DBF2FCB4882}"/>
-    <hyperlink ref="D271" r:id="rId182" xr:uid="{2930C349-E6B7-544B-BB2A-773A46E73BCB}"/>
-    <hyperlink ref="D256" r:id="rId183" xr:uid="{2BE70040-B75E-144F-8CF2-C6FAF265243F}"/>
-    <hyperlink ref="D293" r:id="rId184" xr:uid="{69A55749-D9D2-1B4B-B3F9-4B160F762593}"/>
-    <hyperlink ref="D294" r:id="rId185" xr:uid="{FB9E4799-0707-754B-9240-DFB8EFCF3420}"/>
-    <hyperlink ref="D295" r:id="rId186" xr:uid="{EFA9A5C9-A935-FD44-A8C3-75A6D42D9D41}"/>
-    <hyperlink ref="D81" r:id="rId187" xr:uid="{18AB1C94-4CE1-2945-92C4-F9826FBC6B4E}"/>
-    <hyperlink ref="D296" r:id="rId188" xr:uid="{6CB68E90-F81E-C748-8D45-EFEEC50C2AE3}"/>
-    <hyperlink ref="D298" r:id="rId189" xr:uid="{8303BB33-5888-964E-8CF2-43DD162804AD}"/>
-    <hyperlink ref="D299" r:id="rId190" xr:uid="{6C92D97F-0A5E-394B-ABB8-0A48B9DDE3CE}"/>
-    <hyperlink ref="D300" r:id="rId191" xr:uid="{A23CD4FA-5C90-8B4F-B42D-8F0581378838}"/>
-    <hyperlink ref="D301" r:id="rId192" xr:uid="{A75CA764-6259-D247-9F3E-71FE84093EEF}"/>
-    <hyperlink ref="D302" r:id="rId193" xr:uid="{4FCB99F2-3FFA-D440-B956-CC2FD50BB76F}"/>
-    <hyperlink ref="D305" r:id="rId194" xr:uid="{936BB4A4-64DC-4640-8D60-262FEB18B51D}"/>
-    <hyperlink ref="D306" r:id="rId195" xr:uid="{09EB0BAC-80EB-3346-AF8B-932BAB3F6F52}"/>
-    <hyperlink ref="D307" r:id="rId196" xr:uid="{249C8010-6579-F842-931C-5A1AA5FFD47E}"/>
-    <hyperlink ref="D308" r:id="rId197" xr:uid="{C11D7F08-A472-D74F-ACD4-DC39321AAA3B}"/>
-    <hyperlink ref="D309" r:id="rId198" xr:uid="{EF696095-531A-9B4E-90F5-CA1166C070EB}"/>
-    <hyperlink ref="D310" r:id="rId199" xr:uid="{7319E358-38E8-6D4F-99E9-A558FF1C66D0}"/>
-    <hyperlink ref="D311" r:id="rId200" xr:uid="{C569513C-F920-6148-BB18-A2830C6CABED}"/>
-    <hyperlink ref="D315" r:id="rId201" xr:uid="{4DDCE0DF-C4D6-2F48-850A-FFE8E44529B8}"/>
-    <hyperlink ref="D316" r:id="rId202" xr:uid="{54E4386C-E9E6-5947-8BDF-3BBD841882D1}"/>
-    <hyperlink ref="D317" r:id="rId203" xr:uid="{81F19F2E-83E8-4F41-A52E-63787010CAAE}"/>
-    <hyperlink ref="D318" r:id="rId204" xr:uid="{E0DAEF11-F444-344B-922F-A5AFA19CBDAC}"/>
-    <hyperlink ref="D319" r:id="rId205" xr:uid="{9FD33CD5-F342-BC42-A6B7-5CD2049D8920}"/>
-    <hyperlink ref="D313" r:id="rId206" xr:uid="{9E36AED5-0E4B-A447-9436-6F32633D1396}"/>
-    <hyperlink ref="D320" r:id="rId207" xr:uid="{0288DF9D-25CD-1C4B-A841-A046246E02C3}"/>
-    <hyperlink ref="D321" r:id="rId208" xr:uid="{C9DFAC71-5ACF-204D-8F9A-D4FBACBEA7AA}"/>
-    <hyperlink ref="D105" r:id="rId209" xr:uid="{B4CEFF9C-4149-C147-9750-CA2940A29B5D}"/>
-    <hyperlink ref="D106" r:id="rId210" location="sthash.CLyG4oHQ.dpbs" xr:uid="{785D69EA-E77B-AF48-85EB-249509A6BB77}"/>
-    <hyperlink ref="D86" r:id="rId211" xr:uid="{60A19DED-9CDC-124A-9E44-AA37FD1C44F1}"/>
-    <hyperlink ref="D23" r:id="rId212" xr:uid="{D1664D41-D33B-4949-839C-271243D7F21B}"/>
-    <hyperlink ref="D22" r:id="rId213" xr:uid="{48D024A1-76B5-2148-9BA8-76FC5B789C3C}"/>
-    <hyperlink ref="D34" r:id="rId214" xr:uid="{69D07C5C-50D8-A34C-B327-372E9737895F}"/>
-    <hyperlink ref="D39" r:id="rId215" xr:uid="{62C55848-0362-6241-8D45-015F66952E86}"/>
-    <hyperlink ref="D45" r:id="rId216" xr:uid="{6CBB316C-932E-334D-8420-FEA7F2C4D560}"/>
-    <hyperlink ref="D48" r:id="rId217" xr:uid="{D5CEEF90-9389-EE4B-8CE9-0C6FA742EA5A}"/>
-    <hyperlink ref="D47" r:id="rId218" xr:uid="{E3CDAE9B-8044-F94D-A9D7-1080A2B10492}"/>
-    <hyperlink ref="D211" r:id="rId219" xr:uid="{50F35F4B-BA0B-624A-B5A4-DC53EF5BCCFD}"/>
-    <hyperlink ref="D239" r:id="rId220" xr:uid="{851BBD79-B0B8-6741-ADC7-18BC6CD77F55}"/>
-    <hyperlink ref="D244" r:id="rId221" xr:uid="{8C80B853-2FB6-BA43-8D77-CA9D0A54C7A8}"/>
-    <hyperlink ref="D245" r:id="rId222" xr:uid="{DCAD803E-9B32-AB4D-B77E-56BD769CEADE}"/>
-    <hyperlink ref="D272" r:id="rId223" xr:uid="{E017BD74-051C-A845-9C99-138027F30F1D}"/>
-    <hyperlink ref="D273" r:id="rId224" xr:uid="{4D72A4C4-AD0C-114A-9C48-41FE25C825EB}"/>
-    <hyperlink ref="D277" r:id="rId225" xr:uid="{2E661DC9-EC98-5C47-99FF-DD5BCC222802}"/>
-    <hyperlink ref="D279" r:id="rId226" xr:uid="{7AEE5148-879B-1244-A65C-DF6A183C8993}"/>
-    <hyperlink ref="D280" r:id="rId227" xr:uid="{5D34A7E5-346F-0E41-89CC-2A9B5F277CED}"/>
-    <hyperlink ref="D283" r:id="rId228" xr:uid="{1F7B4ABD-A97B-634D-94AD-CAE2BBAAA501}"/>
-    <hyperlink ref="D284" r:id="rId229" xr:uid="{8DC5E1D5-E8E2-C244-BB87-6B1B882EA7BF}"/>
-    <hyperlink ref="D292" r:id="rId230" xr:uid="{5D7FBCD9-4BE6-8E41-B16C-4AED44F62DAC}"/>
-    <hyperlink ref="D297" r:id="rId231" xr:uid="{2164D655-9D47-8749-A59F-EC0121D2E68B}"/>
-    <hyperlink ref="D303" r:id="rId232" xr:uid="{D0B3FE4C-F121-8C4F-B063-05A222FFB480}"/>
-    <hyperlink ref="D312" r:id="rId233" xr:uid="{47A1D77B-EB49-D14D-9088-F2DE88D7B296}"/>
-    <hyperlink ref="D2" r:id="rId234" xr:uid="{34F9D20D-FC31-C344-84F9-1028073719B0}"/>
-    <hyperlink ref="D3" r:id="rId235" xr:uid="{5AF14D64-BCD2-B14E-B95E-EF64A59D04A2}"/>
-    <hyperlink ref="D9" r:id="rId236" xr:uid="{4E4F2327-D5E2-5445-AD29-35676B61B99D}"/>
-    <hyperlink ref="D8" r:id="rId237" xr:uid="{2B90123B-FE28-734C-9172-6A71ECE5B679}"/>
-    <hyperlink ref="D15" r:id="rId238" xr:uid="{789E9A92-CAA4-7F46-9FC2-9ACE89C5BD91}"/>
-    <hyperlink ref="D25" r:id="rId239" xr:uid="{74E1DBFE-8489-BC40-92D6-35C189C135FC}"/>
-    <hyperlink ref="D24" r:id="rId240" xr:uid="{BEFF145D-E190-5441-83F2-4835045FA3A0}"/>
-    <hyperlink ref="D27" r:id="rId241" xr:uid="{2111868E-0414-564B-9DB4-438F1C2A2B56}"/>
-    <hyperlink ref="D31" r:id="rId242" xr:uid="{A4159E37-BAB2-5A48-AA01-BCEA3CBDE7D1}"/>
-    <hyperlink ref="D38" r:id="rId243" xr:uid="{3DFA7B06-1F09-0E41-B8BD-178C25710D74}"/>
-    <hyperlink ref="D50" r:id="rId244" xr:uid="{B4B0A28C-B65F-134B-9B94-9EF6AF4AD81C}"/>
-    <hyperlink ref="D51" r:id="rId245" xr:uid="{E6644601-F4A2-D842-BAF7-944745C6E1FE}"/>
-    <hyperlink ref="D58" r:id="rId246" xr:uid="{518D65ED-893E-8B40-93EC-F10F3DECE27C}"/>
-    <hyperlink ref="D61" r:id="rId247" xr:uid="{ECFF16B4-C31C-8445-A4D5-B621F848C623}"/>
-    <hyperlink ref="D118" r:id="rId248" xr:uid="{78E49338-E11A-BE46-9436-98D0C4CBE612}"/>
-    <hyperlink ref="D117" r:id="rId249" xr:uid="{CB0B5113-280A-6745-AB5D-3C542D5F0687}"/>
-    <hyperlink ref="D115" r:id="rId250" xr:uid="{0AF1551E-4845-EE4C-AEF2-1C1B5BE33A23}"/>
-    <hyperlink ref="D128" r:id="rId251" xr:uid="{1CEFADA7-B8F9-D944-B3BE-B97F9806AE93}"/>
-    <hyperlink ref="D129" r:id="rId252" xr:uid="{FEB2D05B-9469-3048-B474-790A27338D84}"/>
-    <hyperlink ref="D150" r:id="rId253" xr:uid="{BBDCCEFF-2304-914E-B8AF-301B6E69A0F6}"/>
-    <hyperlink ref="D149" r:id="rId254" xr:uid="{6D6C1A20-E743-C24C-B1EF-66AB85A681F8}"/>
-    <hyperlink ref="D156" r:id="rId255" xr:uid="{49952D50-B854-274E-B075-25872A09FFF2}"/>
-    <hyperlink ref="D154" r:id="rId256" xr:uid="{95987E18-4521-584B-89BB-CD6CC479A43F}"/>
-    <hyperlink ref="D221" r:id="rId257" xr:uid="{3466ECD5-0908-844C-8F01-361E3D467004}"/>
-    <hyperlink ref="D222" r:id="rId258" xr:uid="{890DC3AF-E6F6-CB44-8C49-1ADF75727656}"/>
-    <hyperlink ref="D223" r:id="rId259" xr:uid="{D2F44FA3-F4FD-FC46-A7BC-A13E2C98DAA7}"/>
-    <hyperlink ref="D225" r:id="rId260" xr:uid="{5E66DDE0-516E-A844-844B-E429227B744A}"/>
-    <hyperlink ref="D226" r:id="rId261" xr:uid="{3E616B3D-EF94-F740-99C3-14D3F74641B5}"/>
-    <hyperlink ref="D227" r:id="rId262" xr:uid="{A49956B5-22E5-584E-81F2-74351DDA9CA4}"/>
-    <hyperlink ref="D228" r:id="rId263" xr:uid="{964BC9E3-33DE-8A45-A898-F579F6C96B50}"/>
-    <hyperlink ref="D229" r:id="rId264" xr:uid="{9A5B45A3-E69A-A24D-A65E-F096B559F4D0}"/>
-    <hyperlink ref="D157" r:id="rId265" xr:uid="{B15D867D-3308-9246-A4EA-4808AC4BE276}"/>
-    <hyperlink ref="D164" r:id="rId266" xr:uid="{BDDAF2F9-5060-C645-ADF6-E8B4AE8D9F21}"/>
-    <hyperlink ref="D148" r:id="rId267" xr:uid="{E7E8F9AA-6410-2446-9EDB-35B487642AB4}"/>
-    <hyperlink ref="D147" r:id="rId268" xr:uid="{50AFC520-0BC0-9940-9530-57493CFFEE9E}"/>
-    <hyperlink ref="D66" r:id="rId269" xr:uid="{24265432-4427-CC45-BD00-6954D542D98E}"/>
-    <hyperlink ref="D161" r:id="rId270" xr:uid="{13C83452-5D80-4D4D-9809-7D4EB289B3E0}"/>
-    <hyperlink ref="D162" r:id="rId271" xr:uid="{C11E50A9-9298-2447-9615-93AF182DED39}"/>
-    <hyperlink ref="D163" r:id="rId272" xr:uid="{804DD6E2-158E-6948-B8FE-24248E381935}"/>
-    <hyperlink ref="D142" r:id="rId273" xr:uid="{93246BB1-F4EB-8248-A367-1EEB230F54CD}"/>
-    <hyperlink ref="D140" r:id="rId274" xr:uid="{F4D3B5EE-9DA2-5E44-9B97-1716680A2A98}"/>
-    <hyperlink ref="D146" r:id="rId275" xr:uid="{874DD896-8AE3-4544-B402-517E0CE5538A}"/>
-    <hyperlink ref="D144" r:id="rId276" xr:uid="{131DA2DA-C659-184F-A2E2-DED984EFF9F2}"/>
-    <hyperlink ref="D203" r:id="rId277" xr:uid="{0BBA263E-DF5D-C04A-B0AE-54E68EA17727}"/>
-    <hyperlink ref="D238" r:id="rId278" xr:uid="{8CBEE6BC-1A1B-3C44-81EB-B467460A4D3D}"/>
-    <hyperlink ref="D290" r:id="rId279" xr:uid="{03CF96D1-AB9C-5544-8333-B3B3DEE35CED}"/>
-    <hyperlink ref="D291" r:id="rId280" xr:uid="{7D0B6149-73B8-2649-A2D4-B40EBE59C5D0}"/>
-    <hyperlink ref="D304" r:id="rId281" xr:uid="{CEA15DA5-CC23-A847-ABD8-07B73CA1E52F}"/>
-    <hyperlink ref="D260" r:id="rId282" xr:uid="{517DC8DE-0AF7-3045-A1E8-1A6460F60813}"/>
-    <hyperlink ref="D265" r:id="rId283" xr:uid="{29DC1A21-0CD1-7B4E-893F-19D32E977C1B}"/>
-    <hyperlink ref="D90" r:id="rId284" xr:uid="{72A2BFE4-23C5-E442-A8F0-0378379CCCEB}"/>
-    <hyperlink ref="D63" r:id="rId285" xr:uid="{4EF910E4-3EF4-C94E-AF22-6F0BCA9FADAF}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId2"/>
+    <hyperlink ref="D10" r:id="rId3"/>
+    <hyperlink ref="D21" r:id="rId4"/>
+    <hyperlink ref="D20" r:id="rId5"/>
+    <hyperlink ref="D26" r:id="rId6"/>
+    <hyperlink ref="D18" r:id="rId7"/>
+    <hyperlink ref="D28" r:id="rId8"/>
+    <hyperlink ref="D29" r:id="rId9"/>
+    <hyperlink ref="D30" r:id="rId10"/>
+    <hyperlink ref="D32" r:id="rId11"/>
+    <hyperlink ref="D36" r:id="rId12"/>
+    <hyperlink ref="D37" r:id="rId13"/>
+    <hyperlink ref="D41" r:id="rId14"/>
+    <hyperlink ref="D35" r:id="rId15"/>
+    <hyperlink ref="D54" r:id="rId16"/>
+    <hyperlink ref="D55" r:id="rId17"/>
+    <hyperlink ref="D44" r:id="rId18"/>
+    <hyperlink ref="D60" r:id="rId19"/>
+    <hyperlink ref="D62" r:id="rId20"/>
+    <hyperlink ref="D17" r:id="rId21"/>
+    <hyperlink ref="D68" r:id="rId22"/>
+    <hyperlink ref="D19" r:id="rId23"/>
+    <hyperlink ref="D6" r:id="rId24"/>
+    <hyperlink ref="D14" r:id="rId25"/>
+    <hyperlink ref="D16" r:id="rId26"/>
+    <hyperlink ref="D46" r:id="rId27"/>
+    <hyperlink ref="D56" r:id="rId28"/>
+    <hyperlink ref="D57" r:id="rId29"/>
+    <hyperlink ref="D59" r:id="rId30"/>
+    <hyperlink ref="D70" r:id="rId31"/>
+    <hyperlink ref="D71" r:id="rId32"/>
+    <hyperlink ref="D74" r:id="rId33"/>
+    <hyperlink ref="D75" r:id="rId34"/>
+    <hyperlink ref="D77" r:id="rId35"/>
+    <hyperlink ref="D78" r:id="rId36"/>
+    <hyperlink ref="D79" r:id="rId37"/>
+    <hyperlink ref="D80" r:id="rId38"/>
+    <hyperlink ref="D82" r:id="rId39"/>
+    <hyperlink ref="D85" r:id="rId40"/>
+    <hyperlink ref="D83" r:id="rId41"/>
+    <hyperlink ref="D89" r:id="rId42"/>
+    <hyperlink ref="D91" r:id="rId43"/>
+    <hyperlink ref="D94" r:id="rId44"/>
+    <hyperlink ref="D95" r:id="rId45"/>
+    <hyperlink ref="D76" r:id="rId46"/>
+    <hyperlink ref="D97" r:id="rId47"/>
+    <hyperlink ref="D98" r:id="rId48"/>
+    <hyperlink ref="D100" r:id="rId49"/>
+    <hyperlink ref="D101" r:id="rId50"/>
+    <hyperlink ref="D99" r:id="rId51"/>
+    <hyperlink ref="D107" r:id="rId52"/>
+    <hyperlink ref="D102" r:id="rId53"/>
+    <hyperlink ref="D84" r:id="rId54"/>
+    <hyperlink ref="D103" r:id="rId55"/>
+    <hyperlink ref="D72" r:id="rId56"/>
+    <hyperlink ref="D88" r:id="rId57"/>
+    <hyperlink ref="D87" r:id="rId58"/>
+    <hyperlink ref="D108" r:id="rId59"/>
+    <hyperlink ref="D109" r:id="rId60"/>
+    <hyperlink ref="D110" r:id="rId61"/>
+    <hyperlink ref="D111" r:id="rId62"/>
+    <hyperlink ref="D120" r:id="rId63"/>
+    <hyperlink ref="D121" r:id="rId64"/>
+    <hyperlink ref="D122" r:id="rId65"/>
+    <hyperlink ref="D124" r:id="rId66"/>
+    <hyperlink ref="D64" r:id="rId67"/>
+    <hyperlink ref="D65" r:id="rId68"/>
+    <hyperlink ref="D126" r:id="rId69"/>
+    <hyperlink ref="D127" r:id="rId70"/>
+    <hyperlink ref="D130" r:id="rId71"/>
+    <hyperlink ref="D131" r:id="rId72"/>
+    <hyperlink ref="D132" r:id="rId73"/>
+    <hyperlink ref="D133" r:id="rId74"/>
+    <hyperlink ref="D134" r:id="rId75"/>
+    <hyperlink ref="D135" r:id="rId76"/>
+    <hyperlink ref="D136" r:id="rId77"/>
+    <hyperlink ref="D137" r:id="rId78"/>
+    <hyperlink ref="D138" r:id="rId79"/>
+    <hyperlink ref="D151" r:id="rId80"/>
+    <hyperlink ref="D159" r:id="rId81"/>
+    <hyperlink ref="D160" r:id="rId82"/>
+    <hyperlink ref="D165" r:id="rId83"/>
+    <hyperlink ref="D166" r:id="rId84"/>
+    <hyperlink ref="D167" r:id="rId85"/>
+    <hyperlink ref="D152" r:id="rId86"/>
+    <hyperlink ref="D158" r:id="rId87"/>
+    <hyperlink ref="D168" r:id="rId88"/>
+    <hyperlink ref="D169" r:id="rId89"/>
+    <hyperlink ref="D170" r:id="rId90"/>
+    <hyperlink ref="D171" r:id="rId91"/>
+    <hyperlink ref="D172" r:id="rId92"/>
+    <hyperlink ref="D173" r:id="rId93"/>
+    <hyperlink ref="D174" r:id="rId94"/>
+    <hyperlink ref="D175" r:id="rId95"/>
+    <hyperlink ref="D176" r:id="rId96"/>
+    <hyperlink ref="D177" r:id="rId97"/>
+    <hyperlink ref="D179" r:id="rId98"/>
+    <hyperlink ref="D180" r:id="rId99"/>
+    <hyperlink ref="D181" r:id="rId100"/>
+    <hyperlink ref="D182" r:id="rId101"/>
+    <hyperlink ref="D183" r:id="rId102"/>
+    <hyperlink ref="D184" r:id="rId103"/>
+    <hyperlink ref="D185" r:id="rId104"/>
+    <hyperlink ref="D186" r:id="rId105"/>
+    <hyperlink ref="D187" r:id="rId106"/>
+    <hyperlink ref="D188" r:id="rId107"/>
+    <hyperlink ref="D189" r:id="rId108"/>
+    <hyperlink ref="D190" r:id="rId109"/>
+    <hyperlink ref="D191" r:id="rId110"/>
+    <hyperlink ref="D192" r:id="rId111"/>
+    <hyperlink ref="D193" r:id="rId112"/>
+    <hyperlink ref="D93" r:id="rId113"/>
+    <hyperlink ref="D194" r:id="rId114"/>
+    <hyperlink ref="D195" r:id="rId115"/>
+    <hyperlink ref="D196" r:id="rId116"/>
+    <hyperlink ref="D197" r:id="rId117"/>
+    <hyperlink ref="D198" r:id="rId118"/>
+    <hyperlink ref="D199" r:id="rId119"/>
+    <hyperlink ref="D200" r:id="rId120"/>
+    <hyperlink ref="D201" r:id="rId121"/>
+    <hyperlink ref="D202" r:id="rId122"/>
+    <hyperlink ref="D204" r:id="rId123"/>
+    <hyperlink ref="D205" r:id="rId124"/>
+    <hyperlink ref="D206" r:id="rId125"/>
+    <hyperlink ref="D207" r:id="rId126"/>
+    <hyperlink ref="D208" r:id="rId127"/>
+    <hyperlink ref="D209" r:id="rId128"/>
+    <hyperlink ref="C210" r:id="rId129" display="https://www.bostonmpo.org/node/3243"/>
+    <hyperlink ref="D210" r:id="rId130"/>
+    <hyperlink ref="D212" r:id="rId131"/>
+    <hyperlink ref="D213" r:id="rId132"/>
+    <hyperlink ref="D214" r:id="rId133"/>
+    <hyperlink ref="D215" r:id="rId134"/>
+    <hyperlink ref="D216" r:id="rId135"/>
+    <hyperlink ref="D217" r:id="rId136"/>
+    <hyperlink ref="D218" r:id="rId137"/>
+    <hyperlink ref="D219" r:id="rId138"/>
+    <hyperlink ref="D230" r:id="rId139"/>
+    <hyperlink ref="D231" r:id="rId140"/>
+    <hyperlink ref="D232" r:id="rId141"/>
+    <hyperlink ref="D233" r:id="rId142"/>
+    <hyperlink ref="D234" r:id="rId143"/>
+    <hyperlink ref="D236" r:id="rId144"/>
+    <hyperlink ref="D53" r:id="rId145"/>
+    <hyperlink ref="D237" r:id="rId146"/>
+    <hyperlink ref="D241" r:id="rId147"/>
+    <hyperlink ref="D242" r:id="rId148"/>
+    <hyperlink ref="D247" r:id="rId149"/>
+    <hyperlink ref="D248" r:id="rId150"/>
+    <hyperlink ref="D249" r:id="rId151"/>
+    <hyperlink ref="D251" r:id="rId152"/>
+    <hyperlink ref="D252" r:id="rId153"/>
+    <hyperlink ref="D253" r:id="rId154"/>
+    <hyperlink ref="D254" r:id="rId155"/>
+    <hyperlink ref="D250" r:id="rId156"/>
+    <hyperlink ref="D243" r:id="rId157"/>
+    <hyperlink ref="D255" r:id="rId158"/>
+    <hyperlink ref="D257" r:id="rId159"/>
+    <hyperlink ref="D258" r:id="rId160"/>
+    <hyperlink ref="D259" r:id="rId161"/>
+    <hyperlink ref="D261" r:id="rId162"/>
+    <hyperlink ref="D262" r:id="rId163"/>
+    <hyperlink ref="D263" r:id="rId164"/>
+    <hyperlink ref="D264" r:id="rId165"/>
+    <hyperlink ref="D52" r:id="rId166"/>
+    <hyperlink ref="D266" r:id="rId167"/>
+    <hyperlink ref="D267" r:id="rId168"/>
+    <hyperlink ref="D268" r:id="rId169"/>
+    <hyperlink ref="D269" r:id="rId170"/>
+    <hyperlink ref="D270" r:id="rId171" location="the-ted-williams-tunnel-"/>
+    <hyperlink ref="D274" r:id="rId172"/>
+    <hyperlink ref="D275" r:id="rId173"/>
+    <hyperlink ref="D278" r:id="rId174"/>
+    <hyperlink ref="D282" r:id="rId175"/>
+    <hyperlink ref="D281" r:id="rId176"/>
+    <hyperlink ref="D285" r:id="rId177"/>
+    <hyperlink ref="D286" r:id="rId178"/>
+    <hyperlink ref="D287" r:id="rId179"/>
+    <hyperlink ref="D288" r:id="rId180"/>
+    <hyperlink ref="D289" r:id="rId181"/>
+    <hyperlink ref="D271" r:id="rId182"/>
+    <hyperlink ref="D256" r:id="rId183"/>
+    <hyperlink ref="D293" r:id="rId184"/>
+    <hyperlink ref="D294" r:id="rId185"/>
+    <hyperlink ref="D295" r:id="rId186"/>
+    <hyperlink ref="D81" r:id="rId187"/>
+    <hyperlink ref="D296" r:id="rId188"/>
+    <hyperlink ref="D298" r:id="rId189"/>
+    <hyperlink ref="D299" r:id="rId190"/>
+    <hyperlink ref="D300" r:id="rId191"/>
+    <hyperlink ref="D301" r:id="rId192"/>
+    <hyperlink ref="D302" r:id="rId193"/>
+    <hyperlink ref="D305" r:id="rId194"/>
+    <hyperlink ref="D306" r:id="rId195"/>
+    <hyperlink ref="D307" r:id="rId196"/>
+    <hyperlink ref="D308" r:id="rId197"/>
+    <hyperlink ref="D309" r:id="rId198"/>
+    <hyperlink ref="D310" r:id="rId199"/>
+    <hyperlink ref="D311" r:id="rId200"/>
+    <hyperlink ref="D315" r:id="rId201"/>
+    <hyperlink ref="D316" r:id="rId202"/>
+    <hyperlink ref="D317" r:id="rId203"/>
+    <hyperlink ref="D318" r:id="rId204"/>
+    <hyperlink ref="D319" r:id="rId205"/>
+    <hyperlink ref="D313" r:id="rId206"/>
+    <hyperlink ref="D320" r:id="rId207"/>
+    <hyperlink ref="D321" r:id="rId208"/>
+    <hyperlink ref="D105" r:id="rId209"/>
+    <hyperlink ref="D106" r:id="rId210" location="sthash.CLyG4oHQ.dpbs"/>
+    <hyperlink ref="D86" r:id="rId211"/>
+    <hyperlink ref="D23" r:id="rId212"/>
+    <hyperlink ref="D22" r:id="rId213"/>
+    <hyperlink ref="D34" r:id="rId214"/>
+    <hyperlink ref="D39" r:id="rId215"/>
+    <hyperlink ref="D45" r:id="rId216"/>
+    <hyperlink ref="D48" r:id="rId217"/>
+    <hyperlink ref="D47" r:id="rId218"/>
+    <hyperlink ref="D211" r:id="rId219"/>
+    <hyperlink ref="D239" r:id="rId220"/>
+    <hyperlink ref="D244" r:id="rId221"/>
+    <hyperlink ref="D245" r:id="rId222"/>
+    <hyperlink ref="D272" r:id="rId223"/>
+    <hyperlink ref="D273" r:id="rId224"/>
+    <hyperlink ref="D277" r:id="rId225"/>
+    <hyperlink ref="D279" r:id="rId226"/>
+    <hyperlink ref="D280" r:id="rId227"/>
+    <hyperlink ref="D283" r:id="rId228"/>
+    <hyperlink ref="D284" r:id="rId229"/>
+    <hyperlink ref="D292" r:id="rId230"/>
+    <hyperlink ref="D297" r:id="rId231"/>
+    <hyperlink ref="D303" r:id="rId232"/>
+    <hyperlink ref="D312" r:id="rId233"/>
+    <hyperlink ref="D2" r:id="rId234"/>
+    <hyperlink ref="D3" r:id="rId235"/>
+    <hyperlink ref="D9" r:id="rId236"/>
+    <hyperlink ref="D8" r:id="rId237"/>
+    <hyperlink ref="D15" r:id="rId238"/>
+    <hyperlink ref="D25" r:id="rId239"/>
+    <hyperlink ref="D24" r:id="rId240"/>
+    <hyperlink ref="D27" r:id="rId241"/>
+    <hyperlink ref="D31" r:id="rId242"/>
+    <hyperlink ref="D38" r:id="rId243"/>
+    <hyperlink ref="D50" r:id="rId244"/>
+    <hyperlink ref="D51" r:id="rId245"/>
+    <hyperlink ref="D58" r:id="rId246"/>
+    <hyperlink ref="D61" r:id="rId247"/>
+    <hyperlink ref="D118" r:id="rId248"/>
+    <hyperlink ref="D117" r:id="rId249"/>
+    <hyperlink ref="D115" r:id="rId250"/>
+    <hyperlink ref="D128" r:id="rId251"/>
+    <hyperlink ref="D129" r:id="rId252"/>
+    <hyperlink ref="D150" r:id="rId253"/>
+    <hyperlink ref="D149" r:id="rId254"/>
+    <hyperlink ref="D156" r:id="rId255"/>
+    <hyperlink ref="D154" r:id="rId256"/>
+    <hyperlink ref="D221" r:id="rId257"/>
+    <hyperlink ref="D222" r:id="rId258"/>
+    <hyperlink ref="D223" r:id="rId259"/>
+    <hyperlink ref="D225" r:id="rId260"/>
+    <hyperlink ref="D226" r:id="rId261"/>
+    <hyperlink ref="D227" r:id="rId262"/>
+    <hyperlink ref="D228" r:id="rId263"/>
+    <hyperlink ref="D229" r:id="rId264"/>
+    <hyperlink ref="D157" r:id="rId265"/>
+    <hyperlink ref="D164" r:id="rId266"/>
+    <hyperlink ref="D148" r:id="rId267"/>
+    <hyperlink ref="D147" r:id="rId268"/>
+    <hyperlink ref="D66" r:id="rId269"/>
+    <hyperlink ref="D161" r:id="rId270"/>
+    <hyperlink ref="D162" r:id="rId271"/>
+    <hyperlink ref="D163" r:id="rId272"/>
+    <hyperlink ref="D142" r:id="rId273"/>
+    <hyperlink ref="D140" r:id="rId274"/>
+    <hyperlink ref="D146" r:id="rId275"/>
+    <hyperlink ref="D144" r:id="rId276"/>
+    <hyperlink ref="D203" r:id="rId277"/>
+    <hyperlink ref="D238" r:id="rId278"/>
+    <hyperlink ref="D290" r:id="rId279"/>
+    <hyperlink ref="D291" r:id="rId280"/>
+    <hyperlink ref="D304" r:id="rId281"/>
+    <hyperlink ref="D260" r:id="rId282"/>
+    <hyperlink ref="D265" r:id="rId283"/>
+    <hyperlink ref="D90" r:id="rId284"/>
+    <hyperlink ref="D63" r:id="rId285"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId286"/>

</xml_diff>